<commit_message>
updating testcases in webflux demo for responseEntity cases
</commit_message>
<xml_diff>
--- a/src/test/resources/auto-test-resources/webflux-demo-integration-resources.xlsx
+++ b/src/test/resources/auto-test-resources/webflux-demo-integration-resources.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4927" uniqueCount="809">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4927" uniqueCount="813">
   <si>
     <t>Class</t>
   </si>
@@ -2487,6 +2487,9 @@
 ()Lorg/springframework/http/ResponseEntity&lt;Lreactor/core/publisher/Flux&lt;Ljava/lang/Integer;&gt;;&gt;;</t>
   </si>
   <si>
+    <t>{"headers":{},"body":[1,2,3,4],"status":"OK"}</t>
+  </si>
+  <si>
     <t>org.springframework.http.ResponseEntity&lt;reactor.core.publisher.Flux&lt;java.lang.Integer&gt;&gt;</t>
   </si>
   <si>
@@ -2507,6 +2510,9 @@
 (I)Lorg/springframework/http/ResponseEntity&lt;Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/model/StaffDTO;&gt;;&gt;;</t>
   </si>
   <si>
+    <t>{"headers":{},"body":{"id":2,"name":"staff2"},"status":"OK"}</t>
+  </si>
+  <si>
     <t>{"cause":null,"stackTrace":[{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"OperatorSingle.java","lineNumber":115,"nativeMethod":false,"className":"rx.internal.operators.OperatorSingle$ParentSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"SerializedObserver.java","lineNumber":176,"nativeMethod":false,"className":"rx.observers.SerializedObserver"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"SerializedSubscriber.java","lineNumber":64,"nativeMethod":false,"className":"rx.observers.SerializedSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"drain","fileName":"OnSubscribeConcatMap.java","lineNumber":246,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap$ConcatMapSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"OnSubscribeConcatMap.java","lineNumber":169,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap$ConcatMapSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"OnSubscribeMap.java","lineNumber":97,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeMap$MapSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"SerializedObserver.java","lineNumber":176,"nativeMethod":false,"className":"rx.observers.SerializedObserver"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"SerializedSubscriber.java","lineNumber":64,"nativeMethod":false,"className":"rx.observers.SerializedSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"drain","fileName":"OnSubscribeConcatMap.java","lineNumber":246,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap$ConcatMapSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"OnSubscribeConcatMap.java","lineNumber":169,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap$ConcatMapSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"slowPath","fileName":"OnSubscribeFromArray.java","lineNumber":106,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeFromArray$FromArrayProducer"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"OnSubscribeFromArray.java","lineNumber":63,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeFromArray$FromArrayProducer"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"setProducer","fileName":"Subscriber.java","lineNumber":211,"nativeMethod":false,"className":"rx.Subscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeFromArray.java","lineNumber":32,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeFromArray"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeFromArray.java","lineNumber":24,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeFromArray"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"unsafeSubscribe","fileName":"Observable.java","lineNumber":10327,"nativeMethod":false,"className":"rx.Observable"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeConcatMap.java","lineNumber":94,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeConcatMap.java","lineNumber":42,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"unsafeSubscribe","fileName":"Observable.java","lineNumber":10327,"nativeMethod":false,"className":"rx.Observable"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeMap.java","lineNumber":48,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeMap"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeMap.java","lineNumber":33,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeMap"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"unsafeSubscribe","fileName":"Observable.java","lineNumber":10327,"nativeMethod":false,"className":"rx.Observable"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeConcatMap.java","lineNumber":94,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeConcatMap.java","lineNumber":42,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeLift.java","lineNumber":48,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeLift"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeLift.java","lineNumber":30,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeLift"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"Observable.java","lineNumber":10423,"nativeMethod":false,"className":"rx.Observable"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"Observable.java","lineNumber":10390,"nativeMethod":false,"className":"rx.Observable"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"blockForSingle","fileName":"BlockingObservable.java","lineNumber":443,"nativeMethod":false,"className":"rx.observables.BlockingObservable"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"single","fileName":"BlockingObservable.java","lineNumber":340,"nativeMethod":false,"className":"rx.observables.BlockingObservable"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"findStaffById","fileName":"RXjavaSqlRepoImpl.java","lineNumber":43,"nativeMethod":false,"className":"org.unlogged.springwebfluxdemo.repository.flow1.RXjavaSqlRepoImpl"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"invoke0","fileName":"NativeMethodAccessorImpl.java","lineNumber":-2,"nativeMethod":true,"className":"jdk.internal.reflect.NativeMethodAccessorImpl"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"invoke","fileName":"NativeMethodAccessorImpl.java","lineNumber":77,"nativeMethod":false,"className":"jdk.internal.reflect.NativeMethodAccessorImpl"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"invoke","fileName":"DelegatingMethodAccessorImpl.java","lineNumber":43,"nativeMethod":false,"className":"jdk.internal.reflect.DelegatingMethodAccessorImpl"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"invoke","fileName":"Method.java","lineNumber":568,"nativeMethod":false,"className":"java.lang.reflect.Method"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"invokeJoinpointUsingReflection","fileName":"AopUtils.java","lineNumber":351,"nativeMethod":false,"className":"org.springframework.aop.support.AopUtils"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"invokeJoinpoint","fileName":"ReflectiveMethodInvocation.java","lineNumber":196,"nativeMethod":false,"className":"org.springframework.aop.framework.ReflectiveMethodInvocation"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"proceed","fileName":"ReflectiveMethodInvocation.java","lineNumber":163,"nativeMethod":false,"className":"org.springframework.aop.framework.ReflectiveMethodInvocation"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"proceed","fileName":"CglibAopProxy.java","lineNumber":765,"nativeMethod":false,"className":"org.springframework.aop.framework.CglibAopProxy$CglibMethodInvocation"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"invoke","fileName":"PersistenceExceptionTranslationInterceptor.java","lineNumber":137,"nativeMethod":false,"className":"org.springframework.dao.support.PersistenceExceptionTranslationInterceptor"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"proceed","fileName":"ReflectiveMethodInvocation.java","lineNumber":184,"nativeMethod":false,"className":"org.springframework.aop.framework.ReflectiveMethodInvocation"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"proceed","fileName":"CglibAopProxy.java","lineNumber":765,"nativeMethod":false,"className":"org.springframework.aop.framework.CglibAopProxy$CglibMethodInvocation"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"intercept","fileName":"CglibAopProxy.java","lineNumber":717,"nativeMethod":false,"className":"org.springframework.aop.framework.CglibAopProxy$DynamicAdvisedInterceptor"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"findStaffById","fileName":"&lt;generated&gt;","lineNumber":-1,"nativeMethod":false,"className":"org.unlogged.springwebfluxdemo.repository.flow1.RXjavaSqlRepoImpl$$SpringCGLIB$$0"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"getStaffById","fileName":"CustomServiceCEImpl.java","lineNumber":36,"nativeMethod":false,"className":"org.unlogged.springwebfluxdemo.service.flow1.CustomServiceCEImpl"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"getStaffById","fileName":"CustomControllerCE.java","lineNumber":31,"nativeMethod":false,"className":"org.unlogged.springwebfluxdemo.controller.flow1.CustomControllerCE"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"invoke0","fileName":"NativeMethodAccessorImpl.java","lineNumber":-2,"nativeMethod":true,"className":"jdk.internal.reflect.NativeMethodAccessorImpl"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"invoke","fileName":"NativeMethodAccessorImpl.java","lineNumber":77,"nativeMethod":false,"className":"jdk.internal.reflect.NativeMethodAccessorImpl"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"invoke","fileName":"DelegatingMethodAccessorImpl.java","lineNumber":43,"nativeMethod":false,"className":"jdk.internal.reflect.DelegatingMethodAccessorImpl"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"invoke","fileName":"Method.java","lineNumber":568,"nativeMethod":false,"className":"java.lang.reflect.Method"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"executeCommandRaw","fileName":"AgentCommandExecutorImpl.java","lineNumber":386,"nativeMethod":false,"className":"io.unlogged.AgentCommandExecutorImpl"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"executeCommand","fileName":"AgentCommandExecutorImpl.java","lineNumber":456,"nativeMethod":false,"className":"io.unlogged.AgentCommandExecutorImpl"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"serve","fileName":"AgentCommandServer.java","lineNumber":69,"nativeMethod":false,"className":"io.unlogged.command.AgentCommandServer"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"execute","fileName":"NanoHTTPD.java","lineNumber":945,"nativeMethod":false,"className":"fi.iki.elonen.NanoHTTPD$HTTPSession"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"run","fileName":"NanoHTTPD.java","lineNumber":192,"nativeMethod":false,"className":"fi.iki.elonen.NanoHTTPD$ClientHandler"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"run","fileName":"Thread.java","lineNumber":840,"nativeMethod":false,"className":"java.lang.Thread"}],"message":"Sequence contains no elements","suppressed":[],"localizedMessage":"Sequence contains no elements"}</t>
   </si>
   <si>
@@ -2535,7 +2541,7 @@
 (I)Lorg/springframework/http/ResponseEntity&lt;Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/model/UniversityProfileDTO;&gt;;&gt;;</t>
   </si>
   <si>
-    <t>[{"id":2,"name":"staff2"},{"id":2,"name":"staff2"}]</t>
+    <t>{"headers":{},"body":[{"id":2,"name":"staff2"},{"id":2,"name":"staff2"}],"status":"OK"}</t>
   </si>
   <si>
     <t>{"cause":null,"stackTrace":[{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"OperatorSingle.java","lineNumber":115,"nativeMethod":false,"className":"rx.internal.operators.OperatorSingle$ParentSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"SerializedObserver.java","lineNumber":176,"nativeMethod":false,"className":"rx.observers.SerializedObserver"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"SerializedSubscriber.java","lineNumber":64,"nativeMethod":false,"className":"rx.observers.SerializedSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"drain","fileName":"OnSubscribeConcatMap.java","lineNumber":246,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap$ConcatMapSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"OnSubscribeConcatMap.java","lineNumber":169,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap$ConcatMapSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"OnSubscribeMap.java","lineNumber":97,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeMap$MapSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"SerializedObserver.java","lineNumber":176,"nativeMethod":false,"className":"rx.observers.SerializedObserver"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"SerializedSubscriber.java","lineNumber":64,"nativeMethod":false,"className":"rx.observers.SerializedSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"drain","fileName":"OnSubscribeConcatMap.java","lineNumber":246,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap$ConcatMapSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"OnSubscribeConcatMap.java","lineNumber":169,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap$ConcatMapSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"slowPath","fileName":"OnSubscribeFromArray.java","lineNumber":106,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeFromArray$FromArrayProducer"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"OnSubscribeFromArray.java","lineNumber":63,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeFromArray$FromArrayProducer"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"setProducer","fileName":"Subscriber.java","lineNumber":211,"nativeMethod":false,"className":"rx.Subscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeFromArray.java","lineNumber":32,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeFromArray"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeFromArray.java","lineNumber":24,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeFromArray"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"unsafeSubscribe","fileName":"Observable.java","lineNumber":10327,"nativeMethod":false,"className":"rx.Observable"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeConcatMap.java","lineNumber":94,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeConcatMap.java","lineNumber":42,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"unsafeSubscribe","fileName":"Observable.java","lineNumber":10327,"nativeMethod":false,"className":"rx.Observable"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeMap.java","lineNumber":48,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeMap"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeMap.java","lineNumber":33,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeMap"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"unsafeSubscribe","fileName":"Observable.java","lineNumber":10327,"nativeMethod":false,"className":"rx.Observable"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeConcatMap.java","lineNumber":94,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeConcatMap.java","lineNumber":42,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeLift.java","lineNumber":48,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeLift"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeLift.java","lineNumber":30,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeLift"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"Observable.java","lineNumber":10423,"nativeMethod":false,"className":"rx.Observable"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"Observable.java","lineNumber":10390,"nativeMethod":false,"className":"rx.Observable"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"blockForSingle","fileName":"BlockingObservable.java","lineNumber":443,"nativeMethod":false,"className":"rx.observables.BlockingObservable"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"single","fileName":"BlockingObservable.java","lineNumber":340,"nativeMethod":false,"className":"rx.observables.BlockingObservable"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"getUniversityProfile","fileName":"RXjavaSqlRepoImpl.java","lineNumber":98,"nativeMethod":false,"className":"org.unlogged.springwebfluxdemo.repository.flow1.RXjavaSqlRepoImpl"},{"classLoaderName":null,"moduleName":null,"moduleVersion":null,"methodName":"invoke","fileName":null,"lineNumber":-1,"nativeMethod":false,"className":"jdk.internal.reflect.GeneratedMethodAccessor66"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"invoke","fileName":"DelegatingMethodAccessorImpl.java","lineNumber":43,"nativeMethod":false,"className":"jdk.internal.reflect.DelegatingMethodAccessorImpl"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"invoke","fileName":"Method.java","lineNumber":568,"nativeMethod":false,"className":"java.lang.reflect.Method"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"invokeJoinpointUsingReflection","fileName":"AopUtils.java","lineNumber":351,"nativeMethod":false,"className":"org.springframework.aop.support.AopUtils"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"invokeJoinpoint","fileName":"ReflectiveMethodInvocation.java","lineNumber":196,"nativeMethod":false,"className":"org.springframework.aop.framework.ReflectiveMethodInvocation"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"proceed","fileName":"ReflectiveMethodInvocation.java","lineNumber":163,"nativeMethod":false,"className":"org.springframework.aop.framework.ReflectiveMethodInvocation"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"proceed","fileName":"CglibAopProxy.java","lineNumber":765,"nativeMethod":false,"className":"org.springframework.aop.framework.CglibAopProxy$CglibMethodInvocation"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"invoke","fileName":"PersistenceExceptionTranslationInterceptor.java","lineNumber":137,"nativeMethod":false,"className":"org.springframework.dao.support.PersistenceExceptionTranslationInterceptor"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"proceed","fileName":"ReflectiveMethodInvocation.java","lineNumber":184,"nativeMethod":false,"className":"org.springframework.aop.framework.ReflectiveMethodInvocation"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"proceed","fileName":"CglibAopProxy.java","lineNumber":765,"nativeMethod":false,"className":"org.springframework.aop.framework.CglibAopProxy$CglibMethodInvocation"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"intercept","fileName":"CglibAopProxy.java","lineNumber":717,"nativeMethod":false,"className":"org.springframework.aop.framework.CglibAopProxy$DynamicAdvisedInterceptor"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"getUniversityProfile","fileName":"&lt;generated&gt;","lineNumber":-1,"nativeMethod":false,"className":"org.unlogged.springwebfluxdemo.repository.flow1.RXjavaSqlRepoImpl$$SpringCGLIB$$0"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"getUniversityProfile","fileName":"CustomServiceCEImpl.java","lineNumber":56,"nativeMethod":false,"className":"org.unlogged.springwebfluxdemo.service.flow1.CustomServiceCEImpl"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"getListofStaffForUniversity","fileName":"CustomControllerCE.java","lineNumber":51,"nativeMethod":false,"className":"org.unlogged.springwebfluxdemo.controller.flow1.CustomControllerCE"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"invoke0","fileName":"NativeMethodAccessorImpl.java","lineNumber":-2,"nativeMethod":true,"className":"jdk.internal.reflect.NativeMethodAccessorImpl"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"invoke","fileName":"NativeMethodAccessorImpl.java","lineNumber":77,"nativeMethod":false,"className":"jdk.internal.reflect.NativeMethodAccessorImpl"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"invoke","fileName":"DelegatingMethodAccessorImpl.java","lineNumber":43,"nativeMethod":false,"className":"jdk.internal.reflect.DelegatingMethodAccessorImpl"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"invoke","fileName":"Method.java","lineNumber":568,"nativeMethod":false,"className":"java.lang.reflect.Method"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"executeCommandRaw","fileName":"AgentCommandExecutorImpl.java","lineNumber":386,"nativeMethod":false,"className":"io.unlogged.AgentCommandExecutorImpl"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"executeCommand","fileName":"AgentCommandExecutorImpl.java","lineNumber":456,"nativeMethod":false,"className":"io.unlogged.AgentCommandExecutorImpl"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"serve","fileName":"AgentCommandServer.java","lineNumber":69,"nativeMethod":false,"className":"io.unlogged.command.AgentCommandServer"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"execute","fileName":"NanoHTTPD.java","lineNumber":945,"nativeMethod":false,"className":"fi.iki.elonen.NanoHTTPD$HTTPSession"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"run","fileName":"NanoHTTPD.java","lineNumber":192,"nativeMethod":false,"className":"fi.iki.elonen.NanoHTTPD$ClientHandler"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"run","fileName":"Thread.java","lineNumber":840,"nativeMethod":false,"className":"java.lang.Thread"}],"message":"Sequence contains no elements","suppressed":[],"localizedMessage":"Sequence contains no elements"}</t>
@@ -2548,6 +2554,9 @@
 (I)Lorg/springframework/http/ResponseEntity&lt;Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/model/UniversityFoodInfo;&gt;;&gt;;</t>
   </si>
   <si>
+    <t>{"headers":{},"body":{"universityId":1,"universityName":"university1","beveragesAvailable":[{"id":"ff585c90-4126-4011-a712-be2f098017f1","name":"Black Alert Redis"},{"id":"eb063c5c-11e9-4116-b6e3-ae00e3d33873","name":"Darth Redis"},{"id":"7337d5d1-b7ec-4436-bde3-2dfacef5a45a","name":"Jet Black Redis"}]},"status":"OK"}</t>
+  </si>
+  <si>
     <t>{"cause":null,"stackTrace":[{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"OperatorSingle.java","lineNumber":115,"nativeMethod":false,"className":"rx.internal.operators.OperatorSingle$ParentSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"SerializedObserver.java","lineNumber":176,"nativeMethod":false,"className":"rx.observers.SerializedObserver"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"SerializedSubscriber.java","lineNumber":64,"nativeMethod":false,"className":"rx.observers.SerializedSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"drain","fileName":"OnSubscribeConcatMap.java","lineNumber":246,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap$ConcatMapSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"OnSubscribeConcatMap.java","lineNumber":169,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap$ConcatMapSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"OnSubscribeMap.java","lineNumber":97,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeMap$MapSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"SerializedObserver.java","lineNumber":176,"nativeMethod":false,"className":"rx.observers.SerializedObserver"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"SerializedSubscriber.java","lineNumber":64,"nativeMethod":false,"className":"rx.observers.SerializedSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"drain","fileName":"OnSubscribeConcatMap.java","lineNumber":246,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap$ConcatMapSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"OnSubscribeConcatMap.java","lineNumber":169,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap$ConcatMapSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"slowPath","fileName":"OnSubscribeFromArray.java","lineNumber":106,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeFromArray$FromArrayProducer"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"OnSubscribeFromArray.java","lineNumber":63,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeFromArray$FromArrayProducer"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"setProducer","fileName":"Subscriber.java","lineNumber":211,"nativeMethod":false,"className":"rx.Subscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeFromArray.java","lineNumber":32,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeFromArray"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeFromArray.java","lineNumber":24,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeFromArray"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"unsafeSubscribe","fileName":"Observable.java","lineNumber":10327,"nativeMethod":false,"className":"rx.Observable"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeConcatMap.java","lineNumber":94,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeConcatMap.java","lineNumber":42,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"unsafeSubscribe","fileName":"Observable.java","lineNumber":10327,"nativeMethod":false,"className":"rx.Observable"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeMap.java","lineNumber":48,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeMap"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeMap.java","lineNumber":33,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeMap"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"unsafeSubscribe","fileName":"Observable.java","lineNumber":10327,"nativeMethod":false,"className":"rx.Observable"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeConcatMap.java","lineNumber":94,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeConcatMap.java","lineNumber":42,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeLift.java","lineNumber":48,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeLift"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeLift.java","lineNumber":30,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeLift"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"Observable.java","lineNumber":10423,"nativeMethod":false,"className":"rx.Observable"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"Observable.java","lineNumber":10390,"nativeMethod":false,"className":"rx.Observable"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"blockForSingle","fileName":"BlockingObservable.java","lineNumber":443,"nativeMethod":false,"className":"rx.observables.BlockingObservable"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"single","fileName":"BlockingObservable.java","lineNumber":340,"nativeMethod":false,"className":"rx.observables.BlockingObservable"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"getUniversityProfile","fileName":"RXjavaSqlRepoImpl.java","lineNumber":98,"nativeMethod":false,"className":"org.unlogged.springwebfluxdemo.repository.flow1.RXjavaSqlRepoImpl"},{"classLoaderName":null,"moduleName":null,"moduleVersion":null,"methodName":"invoke","fileName":null,"lineNumber":-1,"nativeMethod":false,"className":"jdk.internal.reflect.GeneratedMethodAccessor66"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"invoke","fileName":"DelegatingMethodAccessorImpl.java","lineNumber":43,"nativeMethod":false,"className":"jdk.internal.reflect.DelegatingMethodAccessorImpl"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"invoke","fileName":"Method.java","lineNumber":568,"nativeMethod":false,"className":"java.lang.reflect.Method"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"invokeJoinpointUsingReflection","fileName":"AopUtils.java","lineNumber":351,"nativeMethod":false,"className":"org.springframework.aop.support.AopUtils"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"invokeJoinpoint","fileName":"ReflectiveMethodInvocation.java","lineNumber":196,"nativeMethod":false,"className":"org.springframework.aop.framework.ReflectiveMethodInvocation"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"proceed","fileName":"ReflectiveMethodInvocation.java","lineNumber":163,"nativeMethod":false,"className":"org.springframework.aop.framework.ReflectiveMethodInvocation"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"proceed","fileName":"CglibAopProxy.java","lineNumber":765,"nativeMethod":false,"className":"org.springframework.aop.framework.CglibAopProxy$CglibMethodInvocation"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"invoke","fileName":"PersistenceExceptionTranslationInterceptor.java","lineNumber":137,"nativeMethod":false,"className":"org.springframework.dao.support.PersistenceExceptionTranslationInterceptor"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"proceed","fileName":"ReflectiveMethodInvocation.java","lineNumber":184,"nativeMethod":false,"className":"org.springframework.aop.framework.ReflectiveMethodInvocation"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"proceed","fileName":"CglibAopProxy.java","lineNumber":765,"nativeMethod":false,"className":"org.springframework.aop.framework.CglibAopProxy$CglibMethodInvocation"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"intercept","fileName":"CglibAopProxy.java","lineNumber":717,"nativeMethod":false,"className":"org.springframework.aop.framework.CglibAopProxy$DynamicAdvisedInterceptor"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"getUniversityProfile","fileName":"&lt;generated&gt;","lineNumber":-1,"nativeMethod":false,"className":"org.unlogged.springwebfluxdemo.repository.flow1.RXjavaSqlRepoImpl$$SpringCGLIB$$0"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"getUniversityProfile","fileName":"CustomServiceCEImpl.java","lineNumber":56,"nativeMethod":false,"className":"org.unlogged.springwebfluxdemo.service.flow1.CustomServiceCEImpl"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"getFoodProfileForUniversity","fileName":"CustomServiceCEImpl.java","lineNumber":64,"nativeMethod":false,"className":"org.unlogged.springwebfluxdemo.service.flow1.CustomServiceCEImpl"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"getFoodInfoProfileForUniversity","fileName":"CustomControllerCE.java","lineNumber":56,"nativeMethod":false,"className":"org.unlogged.springwebfluxdemo.controller.flow1.CustomControllerCE"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"invoke0","fileName":"NativeMethodAccessorImpl.java","lineNumber":-2,"nativeMethod":true,"className":"jdk.internal.reflect.NativeMethodAccessorImpl"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"invoke","fileName":"NativeMethodAccessorImpl.java","lineNumber":77,"nativeMethod":false,"className":"jdk.internal.reflect.NativeMethodAccessorImpl"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"invoke","fileName":"DelegatingMethodAccessorImpl.java","lineNumber":43,"nativeMethod":false,"className":"jdk.internal.reflect.DelegatingMethodAccessorImpl"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"invoke","fileName":"Method.java","lineNumber":568,"nativeMethod":false,"className":"java.lang.reflect.Method"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"executeCommandRaw","fileName":"AgentCommandExecutorImpl.java","lineNumber":386,"nativeMethod":false,"className":"io.unlogged.AgentCommandExecutorImpl"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"executeCommand","fileName":"AgentCommandExecutorImpl.java","lineNumber":456,"nativeMethod":false,"className":"io.unlogged.AgentCommandExecutorImpl"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"serve","fileName":"AgentCommandServer.java","lineNumber":69,"nativeMethod":false,"className":"io.unlogged.command.AgentCommandServer"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"execute","fileName":"NanoHTTPD.java","lineNumber":945,"nativeMethod":false,"className":"fi.iki.elonen.NanoHTTPD$HTTPSession"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"run","fileName":"NanoHTTPD.java","lineNumber":192,"nativeMethod":false,"className":"fi.iki.elonen.NanoHTTPD$ClientHandler"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"run","fileName":"Thread.java","lineNumber":840,"nativeMethod":false,"className":"java.lang.Thread"}],"message":"Sequence contains no elements","suppressed":[],"localizedMessage":"Sequence contains no elements"}</t>
   </si>
   <si>
@@ -2580,6 +2589,9 @@
   <si>
     <t>getUniversityV2
 (I)Lorg/springframework/http/ResponseEntity&lt;Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/model/UniversityProfileV2;&gt;;&gt;;</t>
+  </si>
+  <si>
+    <t>{"headers":{},"body":{"id":1,"name":"university1","beverages":[{"id":"d90817a3-5b03-4ca1-808a-6d324f475588","name":"Black Alert Redis"},{"id":"d28d23d0-b510-422f-a001-38cee61abea0","name":"Jet Black Redis"},{"id":"35255993-a060-4f08-b6c7-cfc45293a3ed","name":"Darth Redis"}],"listOfStudents":[{"id":"65dc19bca9251b174f3f7a24","name":"amg","age":26},{"id":"65dc46237cad7f231af36f0c","name":"amg","age":26},{"id":"65dc476d6ab2e823a98f1446","name":"amg","age":26}],"listOfSeniorMembers":[{"id":"65dc47c1d81d7e5d0d6946c1","name":"bababooey","age":420},{"id":"65dc6e65a51e4e2079024dcf","name":"personX","age":64},{"id":"65e1de11bb4de67e4d8565a3","name":"personY","age":63}],"staffDTOList":[{"id":1,"name":"staffmember1"},{"id":1,"name":"staffmember1"}]},"status":"OK"}</t>
   </si>
   <si>
     <t>{"cause":null,"stackTrace":[{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"OperatorSingle.java","lineNumber":115,"nativeMethod":false,"className":"rx.internal.operators.OperatorSingle$ParentSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"SerializedObserver.java","lineNumber":176,"nativeMethod":false,"className":"rx.observers.SerializedObserver"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"SerializedSubscriber.java","lineNumber":64,"nativeMethod":false,"className":"rx.observers.SerializedSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"drain","fileName":"OnSubscribeConcatMap.java","lineNumber":246,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap$ConcatMapSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"OnSubscribeConcatMap.java","lineNumber":169,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap$ConcatMapSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"OnSubscribeMap.java","lineNumber":97,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeMap$MapSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"SerializedObserver.java","lineNumber":176,"nativeMethod":false,"className":"rx.observers.SerializedObserver"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"SerializedSubscriber.java","lineNumber":64,"nativeMethod":false,"className":"rx.observers.SerializedSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"drain","fileName":"OnSubscribeConcatMap.java","lineNumber":246,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap$ConcatMapSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onCompleted","fileName":"OnSubscribeConcatMap.java","lineNumber":169,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap$ConcatMapSubscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"slowPath","fileName":"OnSubscribeFromArray.java","lineNumber":106,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeFromArray$FromArrayProducer"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"OnSubscribeFromArray.java","lineNumber":63,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeFromArray$FromArrayProducer"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"setProducer","fileName":"Subscriber.java","lineNumber":211,"nativeMethod":false,"className":"rx.Subscriber"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeFromArray.java","lineNumber":32,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeFromArray"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeFromArray.java","lineNumber":24,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeFromArray"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"unsafeSubscribe","fileName":"Observable.java","lineNumber":10327,"nativeMethod":false,"className":"rx.Observable"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeConcatMap.java","lineNumber":94,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeConcatMap.java","lineNumber":42,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"unsafeSubscribe","fileName":"Observable.java","lineNumber":10327,"nativeMethod":false,"className":"rx.Observable"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeMap.java","lineNumber":48,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeMap"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeMap.java","lineNumber":33,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeMap"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"unsafeSubscribe","fileName":"Observable.java","lineNumber":10327,"nativeMethod":false,"className":"rx.Observable"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeConcatMap.java","lineNumber":94,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeConcatMap.java","lineNumber":42,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeConcatMap"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeLift.java","lineNumber":48,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeLift"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"call","fileName":"OnSubscribeLift.java","lineNumber":30,"nativeMethod":false,"className":"rx.internal.operators.OnSubscribeLift"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"Observable.java","lineNumber":10423,"nativeMethod":false,"className":"rx.Observable"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"Observable.java","lineNumber":10390,"nativeMethod":false,"className":"rx.Observable"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"blockForSingle","fileName":"BlockingObservable.java","lineNumber":443,"nativeMethod":false,"className":"rx.observables.BlockingObservable"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"single","fileName":"BlockingObservable.java","lineNumber":340,"nativeMethod":false,"className":"rx.observables.BlockingObservable"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"getUniversityProfile","fileName":"RXjavaSqlRepoImpl.java","lineNumber":98,"nativeMethod":false,"className":"org.unlogged.springwebfluxdemo.repository.flow1.RXjavaSqlRepoImpl"},{"classLoaderName":null,"moduleName":null,"moduleVersion":null,"methodName":"invoke","fileName":null,"lineNumber":-1,"nativeMethod":false,"className":"jdk.internal.reflect.GeneratedMethodAccessor66"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"invoke","fileName":"DelegatingMethodAccessorImpl.java","lineNumber":43,"nativeMethod":false,"className":"jdk.internal.reflect.DelegatingMethodAccessorImpl"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"invoke","fileName":"Method.java","lineNumber":568,"nativeMethod":false,"className":"java.lang.reflect.Method"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"invokeJoinpointUsingReflection","fileName":"AopUtils.java","lineNumber":351,"nativeMethod":false,"className":"org.springframework.aop.support.AopUtils"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"invokeJoinpoint","fileName":"ReflectiveMethodInvocation.java","lineNumber":196,"nativeMethod":false,"className":"org.springframework.aop.framework.ReflectiveMethodInvocation"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"proceed","fileName":"ReflectiveMethodInvocation.java","lineNumber":163,"nativeMethod":false,"className":"org.springframework.aop.framework.ReflectiveMethodInvocation"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"proceed","fileName":"CglibAopProxy.java","lineNumber":765,"nativeMethod":false,"className":"org.springframework.aop.framework.CglibAopProxy$CglibMethodInvocation"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"invoke","fileName":"PersistenceExceptionTranslationInterceptor.java","lineNumber":137,"nativeMethod":false,"className":"org.springframework.dao.support.PersistenceExceptionTranslationInterceptor"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"proceed","fileName":"ReflectiveMethodInvocation.java","lineNumber":184,"nativeMethod":false,"className":"org.springframework.aop.framework.ReflectiveMethodInvocation"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"proceed","fileName":"CglibAopProxy.java","lineNumber":765,"nativeMethod":false,"className":"org.springframework.aop.framework.CglibAopProxy$CglibMethodInvocation"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"intercept","fileName":"CglibAopProxy.java","lineNumber":717,"nativeMethod":false,"className":"org.springframework.aop.framework.CglibAopProxy$DynamicAdvisedInterceptor"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"getUniversityProfile","fileName":"&lt;generated&gt;","lineNumber":-1,"nativeMethod":false,"className":"org.unlogged.springwebfluxdemo.repository.flow1.RXjavaSqlRepoImpl$$SpringCGLIB$$0"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"getUniversityProfile","fileName":"CustomServiceCEImpl.java","lineNumber":56,"nativeMethod":false,"className":"org.unlogged.springwebfluxdemo.service.flow1.CustomServiceCEImpl"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"getFoodProfileForUniversity","fileName":"CustomServiceCEImpl.java","lineNumber":64,"nativeMethod":false,"className":"org.unlogged.springwebfluxdemo.service.flow1.CustomServiceCEImpl"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"getUniversityV2","fileName":"CustomServiceCEImpl.java","lineNumber":87,"nativeMethod":false,"className":"org.unlogged.springwebfluxdemo.service.flow1.CustomServiceCEImpl"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"getUniversityV2","fileName":"CustomControllerCE.java","lineNumber":75,"nativeMethod":false,"className":"org.unlogged.springwebfluxdemo.controller.flow1.CustomControllerCE"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"invoke0","fileName":"NativeMethodAccessorImpl.java","lineNumber":-2,"nativeMethod":true,"className":"jdk.internal.reflect.NativeMethodAccessorImpl"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"invoke","fileName":"NativeMethodAccessorImpl.java","lineNumber":77,"nativeMethod":false,"className":"jdk.internal.reflect.NativeMethodAccessorImpl"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"invoke","fileName":"DelegatingMethodAccessorImpl.java","lineNumber":43,"nativeMethod":false,"className":"jdk.internal.reflect.DelegatingMethodAccessorImpl"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"invoke","fileName":"Method.java","lineNumber":568,"nativeMethod":false,"className":"java.lang.reflect.Method"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"executeCommandRaw","fileName":"AgentCommandExecutorImpl.java","lineNumber":386,"nativeMethod":false,"className":"io.unlogged.AgentCommandExecutorImpl"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"executeCommand","fileName":"AgentCommandExecutorImpl.java","lineNumber":456,"nativeMethod":false,"className":"io.unlogged.AgentCommandExecutorImpl"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"serve","fileName":"AgentCommandServer.java","lineNumber":69,"nativeMethod":false,"className":"io.unlogged.command.AgentCommandServer"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"execute","fileName":"NanoHTTPD.java","lineNumber":945,"nativeMethod":false,"className":"fi.iki.elonen.NanoHTTPD$HTTPSession"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"run","fileName":"NanoHTTPD.java","lineNumber":192,"nativeMethod":false,"className":"fi.iki.elonen.NanoHTTPD$ClientHandler"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"run","fileName":"Thread.java","lineNumber":840,"nativeMethod":false,"className":"java.lang.Thread"}],"message":"Sequence contains no elements","suppressed":[],"localizedMessage":"Sequence contains no elements"}</t>
@@ -16071,7 +16083,7 @@
         <v>15</v>
       </c>
       <c r="G369" s="2" t="s">
-        <v>16</v>
+        <v>704</v>
       </c>
       <c r="H369" s="1" t="s">
         <v>17</v>
@@ -16083,42 +16095,42 @@
         <v>14</v>
       </c>
       <c r="K369" s="1" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
     </row>
     <row r="370" ht="15.75" customHeight="1">
       <c r="A370" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B370" s="1" t="s">
         <v>703</v>
       </c>
       <c r="C370" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="D370" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E370" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F370" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G370" s="2" t="s">
+        <v>704</v>
+      </c>
+      <c r="H370" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I370" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J370" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K370" s="1" t="s">
         <v>705</v>
-      </c>
-      <c r="D370" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E370" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F370" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G370" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H370" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I370" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J370" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K370" s="1" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="371" ht="15.75" customHeight="1">
@@ -16126,7 +16138,7 @@
         <v>702</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="C371" s="1" t="s">
         <v>702</v>
@@ -16141,7 +16153,7 @@
         <v>65</v>
       </c>
       <c r="G371" s="2" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H371" s="1" t="s">
         <v>17</v>
@@ -16153,18 +16165,18 @@
         <v>14</v>
       </c>
       <c r="K371" s="1" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
     </row>
     <row r="372" ht="15.75" customHeight="1">
       <c r="A372" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B372" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="C372" s="1" t="s">
         <v>706</v>
-      </c>
-      <c r="C372" s="1" t="s">
-        <v>705</v>
       </c>
       <c r="D372" s="1" t="s">
         <v>13</v>
@@ -16176,7 +16188,7 @@
         <v>65</v>
       </c>
       <c r="G372" s="2" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H372" s="1" t="s">
         <v>17</v>
@@ -16188,7 +16200,7 @@
         <v>14</v>
       </c>
       <c r="K372" s="1" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
     </row>
     <row r="373" ht="15.75" customHeight="1">
@@ -16196,7 +16208,7 @@
         <v>702</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="C373" s="1" t="s">
         <v>702</v>
@@ -16211,10 +16223,10 @@
         <v>15</v>
       </c>
       <c r="G373" s="2" t="s">
-        <v>500</v>
+        <v>711</v>
       </c>
       <c r="H373" s="1" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="I373" s="1" t="s">
         <v>22</v>
@@ -16223,18 +16235,18 @@
         <v>14</v>
       </c>
       <c r="K373" s="1" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
     </row>
     <row r="374" ht="15.75" customHeight="1">
       <c r="A374" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="C374" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D374" s="1" t="s">
         <v>54</v>
@@ -16246,10 +16258,10 @@
         <v>15</v>
       </c>
       <c r="G374" s="2" t="s">
-        <v>500</v>
+        <v>711</v>
       </c>
       <c r="H374" s="1" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="I374" s="1" t="s">
         <v>22</v>
@@ -16258,7 +16270,7 @@
         <v>14</v>
       </c>
       <c r="K374" s="1" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
     </row>
     <row r="375" ht="15.75" customHeight="1">
@@ -16266,7 +16278,7 @@
         <v>702</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="C375" s="1" t="s">
         <v>702</v>
@@ -16281,7 +16293,7 @@
         <v>15</v>
       </c>
       <c r="G375" s="2" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="H375" s="1" t="s">
         <v>17</v>
@@ -16293,18 +16305,18 @@
         <v>14</v>
       </c>
       <c r="K375" s="1" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
     </row>
     <row r="376" ht="15.75" customHeight="1">
       <c r="A376" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="C376" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D376" s="1" t="s">
         <v>13</v>
@@ -16316,7 +16328,7 @@
         <v>15</v>
       </c>
       <c r="G376" s="2" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="H376" s="1" t="s">
         <v>17</v>
@@ -16328,7 +16340,7 @@
         <v>14</v>
       </c>
       <c r="K376" s="1" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
     </row>
     <row r="377" ht="15.75" customHeight="1">
@@ -16336,7 +16348,7 @@
         <v>702</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="C377" s="1" t="s">
         <v>702</v>
@@ -16351,7 +16363,7 @@
         <v>15</v>
       </c>
       <c r="G377" s="2" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="H377" s="1" t="s">
         <v>17</v>
@@ -16363,18 +16375,18 @@
         <v>14</v>
       </c>
       <c r="K377" s="1" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
     </row>
     <row r="378" ht="15.75" customHeight="1">
       <c r="A378" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B378" s="1" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="C378" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D378" s="1" t="s">
         <v>13</v>
@@ -16386,7 +16398,7 @@
         <v>15</v>
       </c>
       <c r="G378" s="2" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="H378" s="1" t="s">
         <v>17</v>
@@ -16398,7 +16410,7 @@
         <v>14</v>
       </c>
       <c r="K378" s="1" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
     </row>
     <row r="379" ht="15.75" customHeight="1">
@@ -16406,7 +16418,7 @@
         <v>702</v>
       </c>
       <c r="B379" s="1" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="C379" s="1" t="s">
         <v>702</v>
@@ -16421,7 +16433,7 @@
         <v>15</v>
       </c>
       <c r="G379" s="2" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="H379" s="1" t="s">
         <v>17</v>
@@ -16433,18 +16445,18 @@
         <v>14</v>
       </c>
       <c r="K379" s="1" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
     </row>
     <row r="380" ht="15.75" customHeight="1">
       <c r="A380" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="C380" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D380" s="1" t="s">
         <v>54</v>
@@ -16468,7 +16480,7 @@
         <v>14</v>
       </c>
       <c r="K380" s="1" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
     </row>
     <row r="381" ht="15.75" customHeight="1">
@@ -16476,7 +16488,7 @@
         <v>702</v>
       </c>
       <c r="B381" s="1" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="C381" s="1" t="s">
         <v>702</v>
@@ -16491,10 +16503,10 @@
         <v>15</v>
       </c>
       <c r="G381" s="2" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="H381" s="1" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="I381" s="1" t="s">
         <v>22</v>
@@ -16503,18 +16515,18 @@
         <v>14</v>
       </c>
       <c r="K381" s="1" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
     </row>
     <row r="382" ht="15.75" customHeight="1">
       <c r="A382" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B382" s="1" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="C382" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D382" s="1" t="s">
         <v>54</v>
@@ -16526,10 +16538,10 @@
         <v>15</v>
       </c>
       <c r="G382" s="2" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="H382" s="1" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="I382" s="1" t="s">
         <v>22</v>
@@ -16538,7 +16550,7 @@
         <v>14</v>
       </c>
       <c r="K382" s="1" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
     </row>
     <row r="383" ht="15.75" customHeight="1">
@@ -16546,7 +16558,7 @@
         <v>702</v>
       </c>
       <c r="B383" s="1" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="C383" s="1" t="s">
         <v>702</v>
@@ -16561,10 +16573,10 @@
         <v>15</v>
       </c>
       <c r="G383" s="2" t="s">
-        <v>415</v>
+        <v>724</v>
       </c>
       <c r="H383" s="1" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="I383" s="1" t="s">
         <v>22</v>
@@ -16573,18 +16585,18 @@
         <v>14</v>
       </c>
       <c r="K383" s="1" t="s">
-        <v>723</v>
+        <v>726</v>
       </c>
     </row>
     <row r="384" ht="15.75" customHeight="1">
       <c r="A384" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="C384" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D384" s="1" t="s">
         <v>54</v>
@@ -16596,10 +16608,10 @@
         <v>15</v>
       </c>
       <c r="G384" s="2" t="s">
-        <v>415</v>
+        <v>724</v>
       </c>
       <c r="H384" s="1" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="I384" s="1" t="s">
         <v>22</v>
@@ -16608,7 +16620,7 @@
         <v>14</v>
       </c>
       <c r="K384" s="1" t="s">
-        <v>723</v>
+        <v>726</v>
       </c>
     </row>
     <row r="385" ht="15.75" customHeight="1">
@@ -16616,7 +16628,7 @@
         <v>702</v>
       </c>
       <c r="B385" s="1" t="s">
-        <v>724</v>
+        <v>727</v>
       </c>
       <c r="C385" s="1" t="s">
         <v>702</v>
@@ -16634,7 +16646,7 @@
         <v>415</v>
       </c>
       <c r="H385" s="1" t="s">
-        <v>725</v>
+        <v>728</v>
       </c>
       <c r="I385" s="1" t="s">
         <v>22</v>
@@ -16648,13 +16660,13 @@
     </row>
     <row r="386" ht="15.75" customHeight="1">
       <c r="A386" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>724</v>
+        <v>727</v>
       </c>
       <c r="C386" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D386" s="1" t="s">
         <v>54</v>
@@ -16669,7 +16681,7 @@
         <v>415</v>
       </c>
       <c r="H386" s="1" t="s">
-        <v>725</v>
+        <v>728</v>
       </c>
       <c r="I386" s="1" t="s">
         <v>22</v>
@@ -16686,7 +16698,7 @@
         <v>702</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>726</v>
+        <v>729</v>
       </c>
       <c r="C387" s="1" t="s">
         <v>702</v>
@@ -16704,7 +16716,7 @@
         <v>87</v>
       </c>
       <c r="H387" s="1" t="s">
-        <v>727</v>
+        <v>730</v>
       </c>
       <c r="I387" s="1" t="s">
         <v>22</v>
@@ -16718,13 +16730,13 @@
     </row>
     <row r="388" ht="15.75" customHeight="1">
       <c r="A388" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>726</v>
+        <v>729</v>
       </c>
       <c r="C388" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D388" s="1" t="s">
         <v>54</v>
@@ -16739,7 +16751,7 @@
         <v>87</v>
       </c>
       <c r="H388" s="1" t="s">
-        <v>727</v>
+        <v>730</v>
       </c>
       <c r="I388" s="1" t="s">
         <v>22</v>
@@ -16756,7 +16768,7 @@
         <v>702</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="C389" s="1" t="s">
         <v>702</v>
@@ -16771,10 +16783,10 @@
         <v>37</v>
       </c>
       <c r="G389" s="2" t="s">
-        <v>729</v>
+        <v>732</v>
       </c>
       <c r="H389" s="1" t="s">
-        <v>730</v>
+        <v>733</v>
       </c>
       <c r="I389" s="1" t="s">
         <v>22</v>
@@ -16788,13 +16800,13 @@
     </row>
     <row r="390" ht="15.75" customHeight="1">
       <c r="A390" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B390" s="1" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="C390" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D390" s="1" t="s">
         <v>54</v>
@@ -16806,10 +16818,10 @@
         <v>37</v>
       </c>
       <c r="G390" s="1" t="s">
-        <v>730</v>
+        <v>733</v>
       </c>
       <c r="H390" s="1" t="s">
-        <v>730</v>
+        <v>733</v>
       </c>
       <c r="I390" s="1" t="s">
         <v>22</v>
@@ -16826,7 +16838,7 @@
         <v>702</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="C391" s="1" t="s">
         <v>702</v>
@@ -16841,10 +16853,10 @@
         <v>15</v>
       </c>
       <c r="G391" s="2" t="s">
-        <v>87</v>
+        <v>735</v>
       </c>
       <c r="H391" s="1" t="s">
-        <v>732</v>
+        <v>736</v>
       </c>
       <c r="I391" s="1" t="s">
         <v>22</v>
@@ -16853,18 +16865,18 @@
         <v>14</v>
       </c>
       <c r="K391" s="1" t="s">
-        <v>733</v>
+        <v>737</v>
       </c>
     </row>
     <row r="392" ht="15.75" customHeight="1">
       <c r="A392" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B392" s="1" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="C392" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D392" s="1" t="s">
         <v>54</v>
@@ -16876,10 +16888,10 @@
         <v>15</v>
       </c>
       <c r="G392" s="2" t="s">
-        <v>87</v>
+        <v>735</v>
       </c>
       <c r="H392" s="1" t="s">
-        <v>732</v>
+        <v>736</v>
       </c>
       <c r="I392" s="1" t="s">
         <v>22</v>
@@ -16888,7 +16900,7 @@
         <v>14</v>
       </c>
       <c r="K392" s="1" t="s">
-        <v>733</v>
+        <v>737</v>
       </c>
     </row>
     <row r="393" ht="15.75" customHeight="1">
@@ -16896,7 +16908,7 @@
         <v>702</v>
       </c>
       <c r="B393" s="1" t="s">
-        <v>734</v>
+        <v>738</v>
       </c>
       <c r="C393" s="1" t="s">
         <v>702</v>
@@ -16911,10 +16923,10 @@
         <v>37</v>
       </c>
       <c r="G393" s="1" t="s">
-        <v>735</v>
+        <v>739</v>
       </c>
       <c r="H393" s="1" t="s">
-        <v>735</v>
+        <v>739</v>
       </c>
       <c r="I393" s="1" t="s">
         <v>22</v>
@@ -16928,13 +16940,13 @@
     </row>
     <row r="394" ht="15.75" customHeight="1">
       <c r="A394" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B394" s="1" t="s">
-        <v>734</v>
+        <v>738</v>
       </c>
       <c r="C394" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D394" s="1" t="s">
         <v>54</v>
@@ -16946,10 +16958,10 @@
         <v>37</v>
       </c>
       <c r="G394" s="1" t="s">
-        <v>735</v>
+        <v>739</v>
       </c>
       <c r="H394" s="1" t="s">
-        <v>735</v>
+        <v>739</v>
       </c>
       <c r="I394" s="1" t="s">
         <v>22</v>
@@ -16963,13 +16975,13 @@
     </row>
     <row r="395" ht="15.75" customHeight="1">
       <c r="A395" s="1" t="s">
-        <v>736</v>
+        <v>740</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>737</v>
+        <v>741</v>
       </c>
       <c r="C395" s="1" t="s">
-        <v>736</v>
+        <v>740</v>
       </c>
       <c r="D395" s="1" t="s">
         <v>13</v>
@@ -16981,7 +16993,7 @@
         <v>37</v>
       </c>
       <c r="G395" s="1" t="s">
-        <v>738</v>
+        <v>742</v>
       </c>
       <c r="H395" s="1" t="s">
         <v>17</v>
@@ -16993,33 +17005,33 @@
         <v>14</v>
       </c>
       <c r="K395" s="1" t="s">
-        <v>739</v>
+        <v>743</v>
       </c>
     </row>
     <row r="396" ht="15.75" customHeight="1">
       <c r="A396" s="1" t="s">
-        <v>736</v>
+        <v>740</v>
       </c>
       <c r="B396" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="C396" s="1" t="s">
         <v>740</v>
-      </c>
-      <c r="C396" s="1" t="s">
-        <v>736</v>
       </c>
       <c r="D396" s="1" t="s">
         <v>54</v>
       </c>
       <c r="E396" s="1" t="s">
-        <v>741</v>
+        <v>745</v>
       </c>
       <c r="F396" s="2" t="s">
         <v>37</v>
       </c>
       <c r="G396" s="1" t="s">
-        <v>742</v>
+        <v>746</v>
       </c>
       <c r="H396" s="1" t="s">
-        <v>742</v>
+        <v>746</v>
       </c>
       <c r="I396" s="1" t="s">
         <v>22</v>
@@ -17028,33 +17040,33 @@
         <v>14</v>
       </c>
       <c r="K396" s="1" t="s">
-        <v>739</v>
+        <v>743</v>
       </c>
     </row>
     <row r="397" ht="15.75" customHeight="1">
       <c r="A397" s="1" t="s">
-        <v>736</v>
+        <v>740</v>
       </c>
       <c r="B397" s="1" t="s">
-        <v>743</v>
+        <v>747</v>
       </c>
       <c r="C397" s="1" t="s">
-        <v>736</v>
+        <v>740</v>
       </c>
       <c r="D397" s="1" t="s">
         <v>54</v>
       </c>
       <c r="E397" s="1" t="s">
-        <v>741</v>
+        <v>745</v>
       </c>
       <c r="F397" s="2" t="s">
         <v>37</v>
       </c>
       <c r="G397" s="1" t="s">
-        <v>744</v>
+        <v>748</v>
       </c>
       <c r="H397" s="1" t="s">
-        <v>744</v>
+        <v>748</v>
       </c>
       <c r="I397" s="1" t="s">
         <v>22</v>
@@ -17068,28 +17080,28 @@
     </row>
     <row r="398" ht="15.75" customHeight="1">
       <c r="A398" s="1" t="s">
-        <v>736</v>
+        <v>740</v>
       </c>
       <c r="B398" s="1" t="s">
-        <v>745</v>
+        <v>749</v>
       </c>
       <c r="C398" s="1" t="s">
-        <v>736</v>
+        <v>740</v>
       </c>
       <c r="D398" s="1" t="s">
         <v>54</v>
       </c>
       <c r="E398" s="1" t="s">
-        <v>741</v>
+        <v>745</v>
       </c>
       <c r="F398" s="2" t="s">
         <v>37</v>
       </c>
       <c r="G398" s="1" t="s">
-        <v>746</v>
+        <v>750</v>
       </c>
       <c r="H398" s="1" t="s">
-        <v>746</v>
+        <v>750</v>
       </c>
       <c r="I398" s="1" t="s">
         <v>22</v>
@@ -17098,18 +17110,18 @@
         <v>14</v>
       </c>
       <c r="K398" s="1" t="s">
-        <v>739</v>
+        <v>743</v>
       </c>
     </row>
     <row r="399" ht="15.75" customHeight="1">
       <c r="A399" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="B399" s="1" t="s">
         <v>152</v>
       </c>
       <c r="C399" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="D399" s="1" t="s">
         <v>13</v>
@@ -17138,13 +17150,13 @@
     </row>
     <row r="400" ht="15.75" customHeight="1">
       <c r="A400" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="B400" s="1" t="s">
         <v>153</v>
       </c>
       <c r="C400" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="D400" s="1" t="s">
         <v>13</v>
@@ -17173,13 +17185,13 @@
     </row>
     <row r="401" ht="15.75" customHeight="1">
       <c r="A401" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="B401" s="1" t="s">
-        <v>748</v>
+        <v>752</v>
       </c>
       <c r="C401" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="D401" s="1" t="s">
         <v>13</v>
@@ -17208,13 +17220,13 @@
     </row>
     <row r="402" ht="15.75" customHeight="1">
       <c r="A402" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="B402" s="1" t="s">
-        <v>749</v>
+        <v>753</v>
       </c>
       <c r="C402" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="D402" s="1" t="s">
         <v>13</v>
@@ -17243,13 +17255,13 @@
     </row>
     <row r="403" ht="15.75" customHeight="1">
       <c r="A403" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="B403" s="1" t="s">
-        <v>750</v>
+        <v>754</v>
       </c>
       <c r="C403" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="D403" s="1" t="s">
         <v>13</v>
@@ -17278,13 +17290,13 @@
     </row>
     <row r="404" ht="15.75" customHeight="1">
       <c r="A404" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="B404" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="C404" s="1" t="s">
         <v>751</v>
-      </c>
-      <c r="C404" s="1" t="s">
-        <v>747</v>
       </c>
       <c r="D404" s="1" t="s">
         <v>13</v>
@@ -17313,13 +17325,13 @@
     </row>
     <row r="405" ht="15.75" customHeight="1">
       <c r="A405" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="B405" s="1" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
       <c r="C405" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="D405" s="1" t="s">
         <v>13</v>
@@ -17348,13 +17360,13 @@
     </row>
     <row r="406" ht="15.75" customHeight="1">
       <c r="A406" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="B406" s="1" t="s">
-        <v>753</v>
+        <v>757</v>
       </c>
       <c r="C406" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="D406" s="1" t="s">
         <v>13</v>
@@ -17383,13 +17395,13 @@
     </row>
     <row r="407" ht="15.75" customHeight="1">
       <c r="A407" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="B407" s="1" t="s">
-        <v>754</v>
+        <v>758</v>
       </c>
       <c r="C407" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="D407" s="1" t="s">
         <v>13</v>
@@ -17418,13 +17430,13 @@
     </row>
     <row r="408" ht="15.75" customHeight="1">
       <c r="A408" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="B408" s="1" t="s">
-        <v>755</v>
+        <v>759</v>
       </c>
       <c r="C408" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="D408" s="1" t="s">
         <v>13</v>
@@ -17453,13 +17465,13 @@
     </row>
     <row r="409" ht="15.75" customHeight="1">
       <c r="A409" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="B409" s="1" t="s">
         <v>226</v>
       </c>
       <c r="C409" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="D409" s="1" t="s">
         <v>13</v>
@@ -17488,13 +17500,13 @@
     </row>
     <row r="410" ht="15.75" customHeight="1">
       <c r="A410" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="B410" s="1" t="s">
         <v>229</v>
       </c>
       <c r="C410" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="D410" s="1" t="s">
         <v>13</v>
@@ -17523,13 +17535,13 @@
     </row>
     <row r="411" ht="15.75" customHeight="1">
       <c r="A411" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>756</v>
+        <v>760</v>
       </c>
       <c r="C411" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="D411" s="1" t="s">
         <v>13</v>
@@ -17558,13 +17570,13 @@
     </row>
     <row r="412" ht="15.75" customHeight="1">
       <c r="A412" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>757</v>
+        <v>761</v>
       </c>
       <c r="C412" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="D412" s="1" t="s">
         <v>13</v>
@@ -17593,13 +17605,13 @@
     </row>
     <row r="413" ht="15.75" customHeight="1">
       <c r="A413" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="B413" s="1" t="s">
-        <v>758</v>
+        <v>762</v>
       </c>
       <c r="C413" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="D413" s="1" t="s">
         <v>13</v>
@@ -17611,7 +17623,7 @@
         <v>37</v>
       </c>
       <c r="G413" s="1" t="s">
-        <v>759</v>
+        <v>763</v>
       </c>
       <c r="H413" s="1" t="s">
         <v>17</v>
@@ -17623,24 +17635,24 @@
         <v>14</v>
       </c>
       <c r="K413" s="1" t="s">
-        <v>760</v>
+        <v>764</v>
       </c>
     </row>
     <row r="414" ht="15.75" customHeight="1">
       <c r="A414" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="B414" s="1" t="s">
-        <v>761</v>
+        <v>765</v>
       </c>
       <c r="C414" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="D414" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E414" s="1" t="s">
-        <v>762</v>
+        <v>766</v>
       </c>
       <c r="F414" s="2" t="s">
         <v>37</v>
@@ -17663,13 +17675,13 @@
     </row>
     <row r="415" ht="15.75" customHeight="1">
       <c r="A415" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="B415" s="1" t="s">
-        <v>763</v>
+        <v>767</v>
       </c>
       <c r="C415" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="D415" s="1" t="s">
         <v>13</v>
@@ -17698,13 +17710,13 @@
     </row>
     <row r="416" ht="15.75" customHeight="1">
       <c r="A416" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="B416" s="1" t="s">
-        <v>764</v>
+        <v>768</v>
       </c>
       <c r="C416" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="D416" s="1" t="s">
         <v>13</v>
@@ -17733,13 +17745,13 @@
     </row>
     <row r="417" ht="15.75" customHeight="1">
       <c r="A417" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="B417" s="1" t="s">
         <v>232</v>
       </c>
       <c r="C417" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="D417" s="1" t="s">
         <v>13</v>
@@ -17768,13 +17780,13 @@
     </row>
     <row r="418" ht="15.75" customHeight="1">
       <c r="A418" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="B418" s="1" t="s">
         <v>233</v>
       </c>
       <c r="C418" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="D418" s="1" t="s">
         <v>13</v>
@@ -17803,13 +17815,13 @@
     </row>
     <row r="419" ht="15.75" customHeight="1">
       <c r="A419" s="1" t="s">
-        <v>765</v>
+        <v>769</v>
       </c>
       <c r="B419" s="1" t="s">
-        <v>766</v>
+        <v>770</v>
       </c>
       <c r="C419" s="1" t="s">
-        <v>765</v>
+        <v>769</v>
       </c>
       <c r="D419" s="1" t="s">
         <v>13</v>
@@ -17821,7 +17833,7 @@
         <v>15</v>
       </c>
       <c r="G419" s="1" t="s">
-        <v>767</v>
+        <v>771</v>
       </c>
       <c r="H419" s="1" t="s">
         <v>17</v>
@@ -17838,13 +17850,13 @@
     </row>
     <row r="420" ht="15.75" customHeight="1">
       <c r="A420" s="1" t="s">
-        <v>765</v>
+        <v>769</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>768</v>
+        <v>772</v>
       </c>
       <c r="C420" s="1" t="s">
-        <v>765</v>
+        <v>769</v>
       </c>
       <c r="D420" s="1" t="s">
         <v>13</v>
@@ -17856,7 +17868,7 @@
         <v>15</v>
       </c>
       <c r="G420" s="1" t="s">
-        <v>769</v>
+        <v>773</v>
       </c>
       <c r="H420" s="1" t="s">
         <v>17</v>
@@ -17873,13 +17885,13 @@
     </row>
     <row r="421" ht="15.75" customHeight="1">
       <c r="A421" s="1" t="s">
-        <v>770</v>
+        <v>774</v>
       </c>
       <c r="B421" s="1" t="s">
-        <v>771</v>
+        <v>775</v>
       </c>
       <c r="C421" s="1" t="s">
-        <v>770</v>
+        <v>774</v>
       </c>
       <c r="D421" s="1" t="s">
         <v>13</v>
@@ -17891,7 +17903,7 @@
         <v>37</v>
       </c>
       <c r="G421" s="1" t="s">
-        <v>772</v>
+        <v>776</v>
       </c>
       <c r="H421" s="1" t="s">
         <v>17</v>
@@ -17903,7 +17915,7 @@
         <v>14</v>
       </c>
       <c r="K421" s="1" t="s">
-        <v>773</v>
+        <v>777</v>
       </c>
     </row>
     <row r="422" ht="15.75" customHeight="1">
@@ -17911,7 +17923,7 @@
         <v>702</v>
       </c>
       <c r="B422" s="1" t="s">
-        <v>734</v>
+        <v>738</v>
       </c>
       <c r="C422" s="1" t="s">
         <v>702</v>
@@ -17926,10 +17938,10 @@
         <v>37</v>
       </c>
       <c r="G422" s="1" t="s">
-        <v>735</v>
+        <v>739</v>
       </c>
       <c r="H422" s="1" t="s">
-        <v>735</v>
+        <v>739</v>
       </c>
       <c r="I422" s="1" t="s">
         <v>22</v>
@@ -17943,13 +17955,13 @@
     </row>
     <row r="423" ht="15.75" customHeight="1">
       <c r="A423" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B423" s="1" t="s">
-        <v>734</v>
+        <v>738</v>
       </c>
       <c r="C423" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D423" s="1" t="s">
         <v>54</v>
@@ -17961,10 +17973,10 @@
         <v>37</v>
       </c>
       <c r="G423" s="1" t="s">
-        <v>735</v>
+        <v>739</v>
       </c>
       <c r="H423" s="1" t="s">
-        <v>735</v>
+        <v>739</v>
       </c>
       <c r="I423" s="1" t="s">
         <v>22</v>
@@ -17978,13 +17990,13 @@
     </row>
     <row r="424" ht="15.75" customHeight="1">
       <c r="A424" s="1" t="s">
-        <v>774</v>
+        <v>778</v>
       </c>
       <c r="B424" s="1" t="s">
-        <v>775</v>
+        <v>779</v>
       </c>
       <c r="C424" s="1" t="s">
-        <v>774</v>
+        <v>778</v>
       </c>
       <c r="D424" s="1" t="s">
         <v>13</v>
@@ -17996,7 +18008,7 @@
         <v>37</v>
       </c>
       <c r="G424" s="1" t="s">
-        <v>776</v>
+        <v>780</v>
       </c>
       <c r="H424" s="1" t="s">
         <v>17</v>
@@ -18008,18 +18020,18 @@
         <v>14</v>
       </c>
       <c r="K424" s="1" t="s">
-        <v>774</v>
+        <v>778</v>
       </c>
     </row>
     <row r="425" ht="15.75" customHeight="1">
       <c r="A425" s="1" t="s">
-        <v>774</v>
+        <v>778</v>
       </c>
       <c r="B425" s="1" t="s">
-        <v>777</v>
+        <v>781</v>
       </c>
       <c r="C425" s="1" t="s">
-        <v>774</v>
+        <v>778</v>
       </c>
       <c r="D425" s="1" t="s">
         <v>13</v>
@@ -18031,7 +18043,7 @@
         <v>37</v>
       </c>
       <c r="G425" s="1" t="s">
-        <v>778</v>
+        <v>782</v>
       </c>
       <c r="H425" s="1" t="s">
         <v>17</v>
@@ -18043,18 +18055,18 @@
         <v>14</v>
       </c>
       <c r="K425" s="1" t="s">
-        <v>779</v>
+        <v>783</v>
       </c>
     </row>
     <row r="426" ht="15.75" customHeight="1">
       <c r="A426" s="1" t="s">
-        <v>774</v>
+        <v>778</v>
       </c>
       <c r="B426" s="1" t="s">
-        <v>780</v>
+        <v>784</v>
       </c>
       <c r="C426" s="1" t="s">
-        <v>774</v>
+        <v>778</v>
       </c>
       <c r="D426" s="1" t="s">
         <v>13</v>
@@ -18083,13 +18095,13 @@
     </row>
     <row r="427" ht="15.75" customHeight="1">
       <c r="A427" s="1" t="s">
-        <v>781</v>
+        <v>785</v>
       </c>
       <c r="B427" s="1" t="s">
-        <v>782</v>
+        <v>786</v>
       </c>
       <c r="C427" s="1" t="s">
-        <v>781</v>
+        <v>785</v>
       </c>
       <c r="D427" s="1" t="s">
         <v>13</v>
@@ -18101,7 +18113,7 @@
         <v>37</v>
       </c>
       <c r="G427" s="1" t="s">
-        <v>783</v>
+        <v>787</v>
       </c>
       <c r="H427" s="1" t="s">
         <v>17</v>
@@ -18113,18 +18125,18 @@
         <v>14</v>
       </c>
       <c r="K427" s="1" t="s">
-        <v>784</v>
+        <v>788</v>
       </c>
     </row>
     <row r="428" ht="15.75" customHeight="1">
       <c r="A428" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="B428" s="1" t="s">
-        <v>782</v>
+        <v>786</v>
       </c>
       <c r="C428" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="D428" s="1" t="s">
         <v>13</v>
@@ -18136,7 +18148,7 @@
         <v>37</v>
       </c>
       <c r="G428" s="1" t="s">
-        <v>785</v>
+        <v>789</v>
       </c>
       <c r="H428" s="1" t="s">
         <v>17</v>
@@ -18148,18 +18160,18 @@
         <v>14</v>
       </c>
       <c r="K428" s="1" t="s">
-        <v>784</v>
+        <v>788</v>
       </c>
     </row>
     <row r="429" ht="15.75" customHeight="1">
       <c r="A429" s="1" t="s">
-        <v>781</v>
+        <v>785</v>
       </c>
       <c r="B429" s="1" t="s">
-        <v>786</v>
+        <v>790</v>
       </c>
       <c r="C429" s="1" t="s">
-        <v>781</v>
+        <v>785</v>
       </c>
       <c r="D429" s="1" t="s">
         <v>13</v>
@@ -18188,13 +18200,13 @@
     </row>
     <row r="430" ht="15.75" customHeight="1">
       <c r="A430" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="B430" s="1" t="s">
-        <v>786</v>
+        <v>790</v>
       </c>
       <c r="C430" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="D430" s="1" t="s">
         <v>13</v>
@@ -18223,26 +18235,26 @@
     </row>
     <row r="431" ht="15.75" customHeight="1">
       <c r="A431" s="1" t="s">
-        <v>781</v>
+        <v>785</v>
       </c>
       <c r="B431" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="C431" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="D431" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E431" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F431" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G431" s="1" t="s">
         <v>787</v>
       </c>
-      <c r="C431" s="1" t="s">
-        <v>781</v>
-      </c>
-      <c r="D431" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E431" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F431" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G431" s="1" t="s">
-        <v>783</v>
-      </c>
       <c r="H431" s="1" t="s">
         <v>17</v>
       </c>
@@ -18253,18 +18265,18 @@
         <v>14</v>
       </c>
       <c r="K431" s="1" t="s">
-        <v>784</v>
+        <v>788</v>
       </c>
     </row>
     <row r="432" ht="15.75" customHeight="1">
       <c r="A432" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="B432" s="1" t="s">
-        <v>787</v>
+        <v>791</v>
       </c>
       <c r="C432" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="D432" s="1" t="s">
         <v>13</v>
@@ -18276,7 +18288,7 @@
         <v>37</v>
       </c>
       <c r="G432" s="1" t="s">
-        <v>785</v>
+        <v>789</v>
       </c>
       <c r="H432" s="1" t="s">
         <v>17</v>
@@ -18288,18 +18300,18 @@
         <v>14</v>
       </c>
       <c r="K432" s="1" t="s">
-        <v>784</v>
+        <v>788</v>
       </c>
     </row>
     <row r="433" ht="15.75" customHeight="1">
       <c r="A433" s="1" t="s">
-        <v>781</v>
+        <v>785</v>
       </c>
       <c r="B433" s="1" t="s">
-        <v>788</v>
+        <v>792</v>
       </c>
       <c r="C433" s="1" t="s">
-        <v>781</v>
+        <v>785</v>
       </c>
       <c r="D433" s="1" t="s">
         <v>13</v>
@@ -18328,13 +18340,13 @@
     </row>
     <row r="434" ht="15.75" customHeight="1">
       <c r="A434" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="B434" s="1" t="s">
-        <v>788</v>
+        <v>792</v>
       </c>
       <c r="C434" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="D434" s="1" t="s">
         <v>13</v>
@@ -18363,13 +18375,13 @@
     </row>
     <row r="435" ht="15.75" customHeight="1">
       <c r="A435" s="1" t="s">
-        <v>781</v>
+        <v>785</v>
       </c>
       <c r="B435" s="1" t="s">
         <v>168</v>
       </c>
       <c r="C435" s="1" t="s">
-        <v>781</v>
+        <v>785</v>
       </c>
       <c r="D435" s="1" t="s">
         <v>13</v>
@@ -18381,7 +18393,7 @@
         <v>37</v>
       </c>
       <c r="G435" s="1" t="s">
-        <v>789</v>
+        <v>793</v>
       </c>
       <c r="H435" s="1" t="s">
         <v>17</v>
@@ -18398,13 +18410,13 @@
     </row>
     <row r="436" ht="15.75" customHeight="1">
       <c r="A436" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="B436" s="1" t="s">
         <v>168</v>
       </c>
       <c r="C436" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="D436" s="1" t="s">
         <v>13</v>
@@ -18416,7 +18428,7 @@
         <v>37</v>
       </c>
       <c r="G436" s="1" t="s">
-        <v>790</v>
+        <v>794</v>
       </c>
       <c r="H436" s="1" t="s">
         <v>17</v>
@@ -18433,13 +18445,13 @@
     </row>
     <row r="437" ht="15.75" customHeight="1">
       <c r="A437" s="1" t="s">
-        <v>791</v>
+        <v>795</v>
       </c>
       <c r="B437" s="1" t="s">
         <v>250</v>
       </c>
       <c r="C437" s="1" t="s">
-        <v>791</v>
+        <v>795</v>
       </c>
       <c r="D437" s="1" t="s">
         <v>13</v>
@@ -18468,13 +18480,13 @@
     </row>
     <row r="438" ht="15.75" customHeight="1">
       <c r="A438" s="1" t="s">
-        <v>781</v>
+        <v>785</v>
       </c>
       <c r="B438" s="1" t="s">
         <v>250</v>
       </c>
       <c r="C438" s="1" t="s">
-        <v>781</v>
+        <v>785</v>
       </c>
       <c r="D438" s="1" t="s">
         <v>13</v>
@@ -18503,13 +18515,13 @@
     </row>
     <row r="439" ht="15.75" customHeight="1">
       <c r="A439" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="B439" s="1" t="s">
         <v>250</v>
       </c>
       <c r="C439" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="D439" s="1" t="s">
         <v>13</v>
@@ -18538,13 +18550,13 @@
     </row>
     <row r="440" ht="15.75" customHeight="1">
       <c r="A440" s="1" t="s">
-        <v>791</v>
+        <v>795</v>
       </c>
       <c r="B440" s="1" t="s">
         <v>251</v>
       </c>
       <c r="C440" s="1" t="s">
-        <v>791</v>
+        <v>795</v>
       </c>
       <c r="D440" s="1" t="s">
         <v>13</v>
@@ -18573,13 +18585,13 @@
     </row>
     <row r="441" ht="15.75" customHeight="1">
       <c r="A441" s="1" t="s">
-        <v>781</v>
+        <v>785</v>
       </c>
       <c r="B441" s="1" t="s">
         <v>251</v>
       </c>
       <c r="C441" s="1" t="s">
-        <v>781</v>
+        <v>785</v>
       </c>
       <c r="D441" s="1" t="s">
         <v>13</v>
@@ -18608,13 +18620,13 @@
     </row>
     <row r="442" ht="15.75" customHeight="1">
       <c r="A442" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="B442" s="1" t="s">
         <v>251</v>
       </c>
       <c r="C442" s="1" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="D442" s="1" t="s">
         <v>13</v>
@@ -18643,13 +18655,13 @@
     </row>
     <row r="443" ht="15.75" customHeight="1">
       <c r="A443" s="1" t="s">
-        <v>792</v>
+        <v>796</v>
       </c>
       <c r="B443" s="1" t="s">
-        <v>793</v>
+        <v>797</v>
       </c>
       <c r="C443" s="1" t="s">
-        <v>794</v>
+        <v>798</v>
       </c>
       <c r="D443" s="1" t="s">
         <v>13</v>
@@ -18661,7 +18673,7 @@
         <v>15</v>
       </c>
       <c r="G443" s="1" t="s">
-        <v>795</v>
+        <v>799</v>
       </c>
       <c r="H443" s="1" t="s">
         <v>17</v>
@@ -18673,18 +18685,18 @@
         <v>14</v>
       </c>
       <c r="K443" s="1" t="s">
-        <v>796</v>
+        <v>800</v>
       </c>
     </row>
     <row r="444" ht="15.75" customHeight="1">
       <c r="A444" s="1" t="s">
-        <v>794</v>
+        <v>798</v>
       </c>
       <c r="B444" s="1" t="s">
-        <v>793</v>
+        <v>797</v>
       </c>
       <c r="C444" s="1" t="s">
-        <v>794</v>
+        <v>798</v>
       </c>
       <c r="D444" s="1" t="s">
         <v>13</v>
@@ -18696,7 +18708,7 @@
         <v>15</v>
       </c>
       <c r="G444" s="1" t="s">
-        <v>795</v>
+        <v>799</v>
       </c>
       <c r="H444" s="1" t="s">
         <v>17</v>
@@ -18708,18 +18720,18 @@
         <v>14</v>
       </c>
       <c r="K444" s="1" t="s">
-        <v>796</v>
+        <v>800</v>
       </c>
     </row>
     <row r="445" ht="15.75" customHeight="1">
       <c r="A445" s="1" t="s">
-        <v>797</v>
+        <v>801</v>
       </c>
       <c r="B445" s="1" t="s">
-        <v>798</v>
+        <v>802</v>
       </c>
       <c r="C445" s="1" t="s">
-        <v>797</v>
+        <v>801</v>
       </c>
       <c r="D445" s="1" t="s">
         <v>13</v>
@@ -18731,7 +18743,7 @@
         <v>37</v>
       </c>
       <c r="G445" s="1" t="s">
-        <v>799</v>
+        <v>803</v>
       </c>
       <c r="H445" s="1" t="s">
         <v>17</v>
@@ -18743,18 +18755,18 @@
         <v>14</v>
       </c>
       <c r="K445" s="1" t="s">
-        <v>800</v>
+        <v>804</v>
       </c>
     </row>
     <row r="446" ht="15.75" customHeight="1">
       <c r="A446" s="1" t="s">
-        <v>797</v>
+        <v>801</v>
       </c>
       <c r="B446" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="C446" s="1" t="s">
         <v>801</v>
-      </c>
-      <c r="C446" s="1" t="s">
-        <v>797</v>
       </c>
       <c r="D446" s="1" t="s">
         <v>13</v>
@@ -18766,7 +18778,7 @@
         <v>37</v>
       </c>
       <c r="G446" s="1" t="s">
-        <v>799</v>
+        <v>803</v>
       </c>
       <c r="H446" s="1" t="s">
         <v>17</v>
@@ -18778,31 +18790,31 @@
         <v>14</v>
       </c>
       <c r="K446" s="1" t="s">
-        <v>800</v>
+        <v>804</v>
       </c>
     </row>
     <row r="447" ht="15.75" customHeight="1">
       <c r="A447" s="1" t="s">
-        <v>797</v>
+        <v>801</v>
       </c>
       <c r="B447" s="1" t="s">
-        <v>802</v>
+        <v>806</v>
       </c>
       <c r="C447" s="1" t="s">
-        <v>797</v>
+        <v>801</v>
       </c>
       <c r="D447" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E447" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="F447" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G447" s="1" t="s">
         <v>803</v>
       </c>
-      <c r="F447" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G447" s="1" t="s">
-        <v>799</v>
-      </c>
       <c r="H447" s="1" t="s">
         <v>17</v>
       </c>
@@ -18813,33 +18825,33 @@
         <v>14</v>
       </c>
       <c r="K447" s="1" t="s">
-        <v>800</v>
+        <v>804</v>
       </c>
     </row>
     <row r="448" ht="15.75" customHeight="1">
       <c r="A448" s="1" t="s">
-        <v>804</v>
+        <v>808</v>
       </c>
       <c r="B448" s="1" t="s">
-        <v>805</v>
+        <v>809</v>
       </c>
       <c r="C448" s="1" t="s">
-        <v>804</v>
+        <v>808</v>
       </c>
       <c r="D448" s="1" t="s">
         <v>54</v>
       </c>
       <c r="E448" s="1" t="s">
-        <v>806</v>
+        <v>810</v>
       </c>
       <c r="F448" s="2" t="s">
         <v>37</v>
       </c>
       <c r="G448" s="1" t="s">
-        <v>807</v>
+        <v>811</v>
       </c>
       <c r="H448" s="1" t="s">
-        <v>807</v>
+        <v>811</v>
       </c>
       <c r="I448" s="1" t="s">
         <v>22</v>
@@ -18848,7 +18860,7 @@
         <v>14</v>
       </c>
       <c r="K448" s="1" t="s">
-        <v>808</v>
+        <v>812</v>
       </c>
     </row>
     <row r="449" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
updated 2 enrichment cases
</commit_message>
<xml_diff>
--- a/src/test/resources/auto-test-resources/webflux-demo-integration-resources.xlsx
+++ b/src/test/resources/auto-test-resources/webflux-demo-integration-resources.xlsx
@@ -114,7 +114,7 @@
 ()Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/model/Person;&gt;;</t>
   </si>
   <si>
-    <t>{"id":null,"name":"p1#En#En#En#En#En","age":6}</t>
+    <t>{"id":null,"name":"p1#En","age":1}</t>
   </si>
   <si>
     <t>reactor.core.publisher.Mono&lt;org.unlogged.springwebfluxdemo.model.Person&gt;</t>
@@ -124,7 +124,7 @@
 ()Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/model/Person;&gt;;</t>
   </si>
   <si>
-    <t>{"id":null,"name":"p2#En#En#En#En#En#En#En","age":6}</t>
+    <t>{"id":null,"name":"p2#En","age":1}</t>
   </si>
   <si>
     <t>org.unlogged.springwebfluxdemo.CoffeeConfiguration</t>
@@ -2877,7 +2877,6 @@
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -2906,7 +2905,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2915,12 +2914,7 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -3140,7 +3134,8 @@
     <col customWidth="1" min="1" max="1" width="66.86"/>
     <col customWidth="1" min="2" max="2" width="57.14"/>
     <col customWidth="1" min="3" max="3" width="10.29"/>
-    <col customWidth="1" min="4" max="5" width="8.71"/>
+    <col customWidth="1" min="4" max="4" width="8.71"/>
+    <col customWidth="1" min="5" max="5" width="17.71"/>
     <col customWidth="1" min="6" max="6" width="34.29"/>
     <col customWidth="1" min="7" max="7" width="31694.0"/>
     <col customWidth="1" min="8" max="21" width="8.71"/>
@@ -3162,7 +3157,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -3197,7 +3192,7 @@
       <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -3226,16 +3221,16 @@
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -3264,7 +3259,7 @@
       <c r="E4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -3299,10 +3294,10 @@
       <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="1" t="s">
+      <c r="F5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -3334,10 +3329,10 @@
       <c r="E6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="F6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>33</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -3369,7 +3364,7 @@
       <c r="E7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -3404,7 +3399,7 @@
       <c r="E8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G8" s="1" t="s">
@@ -3439,7 +3434,7 @@
       <c r="E9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -3474,7 +3469,7 @@
       <c r="E10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -3509,7 +3504,7 @@
       <c r="E11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G11" s="1" t="s">
@@ -3544,7 +3539,7 @@
       <c r="E12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -3579,10 +3574,10 @@
       <c r="E13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="2" t="s">
+      <c r="F13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>51</v>
       </c>
       <c r="H13" s="1" t="s">
@@ -3614,7 +3609,7 @@
       <c r="E14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="1" t="s">
         <v>56</v>
       </c>
       <c r="G14" s="1" t="s">
@@ -3649,10 +3644,10 @@
       <c r="E15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" s="2" t="s">
+      <c r="F15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>51</v>
       </c>
       <c r="H15" s="1" t="s">
@@ -3684,7 +3679,7 @@
       <c r="E16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -3719,7 +3714,7 @@
       <c r="E17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G17" s="1" t="s">
@@ -3754,7 +3749,7 @@
       <c r="E18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G18" s="1" t="s">
@@ -3789,7 +3784,7 @@
       <c r="E19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G19" s="1" t="s">
@@ -3821,13 +3816,13 @@
       <c r="D20" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="2" t="s">
+      <c r="F20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H20" s="1" t="s">
@@ -3856,13 +3851,13 @@
       <c r="D21" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G21" s="2" t="s">
+      <c r="F21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H21" s="1" t="s">
@@ -3894,7 +3889,7 @@
       <c r="E22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G22" s="1" t="s">
@@ -3929,7 +3924,7 @@
       <c r="E23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G23" s="1" t="s">
@@ -3964,7 +3959,7 @@
       <c r="E24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G24" s="1" t="s">
@@ -3999,7 +3994,7 @@
       <c r="E25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G25" s="1" t="s">
@@ -4034,7 +4029,7 @@
       <c r="E26" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G26" s="1" t="s">
@@ -4069,7 +4064,7 @@
       <c r="E27" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G27" s="1" t="s">
@@ -4101,13 +4096,13 @@
       <c r="D28" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G28" s="2" t="s">
+      <c r="F28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>79</v>
       </c>
       <c r="H28" s="1" t="s">
@@ -4136,13 +4131,13 @@
       <c r="D29" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E29" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G29" s="2" t="s">
+      <c r="F29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>79</v>
       </c>
       <c r="H29" s="1" t="s">
@@ -4171,13 +4166,13 @@
       <c r="D30" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E30" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G30" s="2" t="s">
+      <c r="F30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>83</v>
       </c>
       <c r="H30" s="1" t="s">
@@ -4206,13 +4201,13 @@
       <c r="D31" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E31" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G31" s="2" t="s">
+      <c r="F31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>83</v>
       </c>
       <c r="H31" s="1" t="s">
@@ -4241,13 +4236,13 @@
       <c r="D32" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E32" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G32" s="2" t="s">
+      <c r="F32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>87</v>
       </c>
       <c r="H32" s="1" t="s">
@@ -4276,13 +4271,13 @@
       <c r="D33" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E33" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G33" s="2" t="s">
+      <c r="F33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>87</v>
       </c>
       <c r="H33" s="1" t="s">
@@ -4314,7 +4309,7 @@
       <c r="E34" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F34" s="4" t="s">
+      <c r="F34" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G34" s="3" t="s">
@@ -4359,7 +4354,7 @@
       <c r="E35" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="F35" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G35" s="3" t="s">
@@ -4404,7 +4399,7 @@
       <c r="E36" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G36" s="1" t="s">
@@ -4439,7 +4434,7 @@
       <c r="E37" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F37" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G37" s="1" t="s">
@@ -4474,7 +4469,7 @@
       <c r="E38" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F38" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G38" s="1" t="s">
@@ -4509,7 +4504,7 @@
       <c r="E39" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F39" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G39" s="1" t="s">
@@ -4544,7 +4539,7 @@
       <c r="E40" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F40" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G40" s="1" t="s">
@@ -4579,7 +4574,7 @@
       <c r="E41" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F41" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G41" s="1" t="s">
@@ -4614,7 +4609,7 @@
       <c r="E42" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="F42" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G42" s="1" t="s">
@@ -4649,7 +4644,7 @@
       <c r="E43" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="F43" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G43" s="1" t="s">
@@ -4684,7 +4679,7 @@
       <c r="E44" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="F44" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G44" s="1" t="s">
@@ -4719,7 +4714,7 @@
       <c r="E45" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="F45" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G45" s="1" t="s">
@@ -4754,7 +4749,7 @@
       <c r="E46" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="F46" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G46" s="1" t="s">
@@ -4789,7 +4784,7 @@
       <c r="E47" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F47" s="1" t="s">
         <v>56</v>
       </c>
       <c r="G47" s="1" t="s">
@@ -4824,7 +4819,7 @@
       <c r="E48" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="F48" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G48" s="1" t="s">
@@ -4859,7 +4854,7 @@
       <c r="E49" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="F49" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G49" s="1" t="s">
@@ -4894,7 +4889,7 @@
       <c r="E50" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="F50" s="4" t="s">
+      <c r="F50" s="3" t="s">
         <v>37</v>
       </c>
       <c r="G50" s="3" t="s">
@@ -4939,7 +4934,7 @@
       <c r="E51" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="F51" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G51" s="1" t="s">
@@ -4974,7 +4969,7 @@
       <c r="E52" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="F52" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G52" s="1" t="s">
@@ -5009,7 +5004,7 @@
       <c r="E53" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F53" s="2" t="s">
+      <c r="F53" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G53" s="1" t="s">
@@ -5044,7 +5039,7 @@
       <c r="E54" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F54" s="2" t="s">
+      <c r="F54" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G54" s="1" t="s">
@@ -5079,7 +5074,7 @@
       <c r="E55" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F55" s="2" t="s">
+      <c r="F55" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G55" s="1" t="s">
@@ -5114,7 +5109,7 @@
       <c r="E56" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F56" s="2" t="s">
+      <c r="F56" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G56" s="1" t="s">
@@ -5149,7 +5144,7 @@
       <c r="E57" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F57" s="2" t="s">
+      <c r="F57" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G57" s="1" t="s">
@@ -5184,7 +5179,7 @@
       <c r="E58" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F58" s="2" t="s">
+      <c r="F58" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G58" s="1" t="s">
@@ -5219,7 +5214,7 @@
       <c r="E59" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="F59" s="2" t="s">
+      <c r="F59" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G59" s="1" t="s">
@@ -5254,7 +5249,7 @@
       <c r="E60" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F60" s="2" t="s">
+      <c r="F60" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G60" s="1" t="s">
@@ -5289,7 +5284,7 @@
       <c r="E61" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F61" s="2" t="s">
+      <c r="F61" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G61" s="1" t="s">
@@ -5324,7 +5319,7 @@
       <c r="E62" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F62" s="2" t="s">
+      <c r="F62" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G62" s="1" t="s">
@@ -5359,7 +5354,7 @@
       <c r="E63" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F63" s="2" t="s">
+      <c r="F63" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G63" s="1" t="s">
@@ -5394,7 +5389,7 @@
       <c r="E64" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F64" s="2" t="s">
+      <c r="F64" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G64" s="1" t="s">
@@ -5429,7 +5424,7 @@
       <c r="E65" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="F65" s="2" t="s">
+      <c r="F65" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G65" s="1" t="s">
@@ -5464,7 +5459,7 @@
       <c r="E66" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F66" s="2" t="s">
+      <c r="F66" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G66" s="1" t="s">
@@ -5499,7 +5494,7 @@
       <c r="E67" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F67" s="2" t="s">
+      <c r="F67" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G67" s="1" t="s">
@@ -5534,7 +5529,7 @@
       <c r="E68" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="F68" s="2" t="s">
+      <c r="F68" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G68" s="1" t="s">
@@ -5569,7 +5564,7 @@
       <c r="E69" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="F69" s="2" t="s">
+      <c r="F69" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G69" s="1" t="s">
@@ -5604,7 +5599,7 @@
       <c r="E70" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="F70" s="2" t="s">
+      <c r="F70" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G70" s="1" t="s">
@@ -5639,7 +5634,7 @@
       <c r="E71" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="F71" s="2" t="s">
+      <c r="F71" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G71" s="1" t="s">
@@ -5674,7 +5669,7 @@
       <c r="E72" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F72" s="2" t="s">
+      <c r="F72" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G72" s="1" t="s">
@@ -5709,7 +5704,7 @@
       <c r="E73" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="F73" s="2" t="s">
+      <c r="F73" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G73" s="1" t="s">
@@ -5744,7 +5739,7 @@
       <c r="E74" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="F74" s="2" t="s">
+      <c r="F74" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G74" s="1" t="s">
@@ -5779,7 +5774,7 @@
       <c r="E75" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F75" s="2" t="s">
+      <c r="F75" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G75" s="1" t="s">
@@ -5814,7 +5809,7 @@
       <c r="E76" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="F76" s="2" t="s">
+      <c r="F76" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G76" s="1" t="s">
@@ -5849,7 +5844,7 @@
       <c r="E77" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="F77" s="2" t="s">
+      <c r="F77" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G77" s="1" t="s">
@@ -5884,7 +5879,7 @@
       <c r="E78" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F78" s="2" t="s">
+      <c r="F78" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G78" s="1" t="s">
@@ -5919,7 +5914,7 @@
       <c r="E79" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F79" s="2" t="s">
+      <c r="F79" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G79" s="1" t="s">
@@ -5954,7 +5949,7 @@
       <c r="E80" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="F80" s="2" t="s">
+      <c r="F80" s="1" t="s">
         <v>207</v>
       </c>
       <c r="G80" s="1" t="s">
@@ -5989,7 +5984,7 @@
       <c r="E81" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="F81" s="2" t="s">
+      <c r="F81" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G81" s="1" t="s">
@@ -6024,7 +6019,7 @@
       <c r="E82" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F82" s="2" t="s">
+      <c r="F82" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G82" s="1" t="s">
@@ -6059,7 +6054,7 @@
       <c r="E83" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="F83" s="2" t="s">
+      <c r="F83" s="1" t="s">
         <v>207</v>
       </c>
       <c r="G83" s="1" t="s">
@@ -6094,7 +6089,7 @@
       <c r="E84" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="F84" s="2" t="s">
+      <c r="F84" s="1" t="s">
         <v>207</v>
       </c>
       <c r="G84" s="1" t="s">
@@ -6129,7 +6124,7 @@
       <c r="E85" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="F85" s="2" t="s">
+      <c r="F85" s="1" t="s">
         <v>207</v>
       </c>
       <c r="G85" s="1" t="s">
@@ -6164,7 +6159,7 @@
       <c r="E86" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F86" s="2" t="s">
+      <c r="F86" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G86" s="1" t="s">
@@ -6199,7 +6194,7 @@
       <c r="E87" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F87" s="2" t="s">
+      <c r="F87" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G87" s="1" t="s">
@@ -6234,7 +6229,7 @@
       <c r="E88" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F88" s="2" t="s">
+      <c r="F88" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G88" s="1" t="s">
@@ -6269,7 +6264,7 @@
       <c r="E89" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F89" s="2" t="s">
+      <c r="F89" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G89" s="1" t="s">
@@ -6304,7 +6299,7 @@
       <c r="E90" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F90" s="2" t="s">
+      <c r="F90" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G90" s="1" t="s">
@@ -6339,7 +6334,7 @@
       <c r="E91" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F91" s="2" t="s">
+      <c r="F91" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G91" s="1" t="s">
@@ -6374,7 +6369,7 @@
       <c r="E92" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F92" s="2" t="s">
+      <c r="F92" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G92" s="1" t="s">
@@ -6409,7 +6404,7 @@
       <c r="E93" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F93" s="2" t="s">
+      <c r="F93" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G93" s="1" t="s">
@@ -6444,7 +6439,7 @@
       <c r="E94" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F94" s="2" t="s">
+      <c r="F94" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G94" s="1" t="s">
@@ -6479,7 +6474,7 @@
       <c r="E95" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F95" s="2" t="s">
+      <c r="F95" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G95" s="1" t="s">
@@ -6514,7 +6509,7 @@
       <c r="E96" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F96" s="2" t="s">
+      <c r="F96" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G96" s="1" t="s">
@@ -6549,7 +6544,7 @@
       <c r="E97" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F97" s="2" t="s">
+      <c r="F97" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G97" s="1" t="s">
@@ -6584,7 +6579,7 @@
       <c r="E98" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F98" s="2" t="s">
+      <c r="F98" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G98" s="1" t="s">
@@ -6619,7 +6614,7 @@
       <c r="E99" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F99" s="2" t="s">
+      <c r="F99" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G99" s="1" t="s">
@@ -6654,7 +6649,7 @@
       <c r="E100" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F100" s="2" t="s">
+      <c r="F100" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G100" s="1" t="s">
@@ -6689,7 +6684,7 @@
       <c r="E101" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F101" s="2" t="s">
+      <c r="F101" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G101" s="1" t="s">
@@ -6724,7 +6719,7 @@
       <c r="E102" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F102" s="2" t="s">
+      <c r="F102" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G102" s="1" t="s">
@@ -6759,7 +6754,7 @@
       <c r="E103" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="F103" s="2" t="s">
+      <c r="F103" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G103" s="1" t="s">
@@ -6794,7 +6789,7 @@
       <c r="E104" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F104" s="2" t="s">
+      <c r="F104" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G104" s="1" t="s">
@@ -6829,7 +6824,7 @@
       <c r="E105" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F105" s="2" t="s">
+      <c r="F105" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G105" s="1" t="s">
@@ -6864,7 +6859,7 @@
       <c r="E106" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F106" s="2" t="s">
+      <c r="F106" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G106" s="1" t="s">
@@ -6899,7 +6894,7 @@
       <c r="E107" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F107" s="2" t="s">
+      <c r="F107" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G107" s="1" t="s">
@@ -6934,7 +6929,7 @@
       <c r="E108" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F108" s="2" t="s">
+      <c r="F108" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G108" s="1" t="s">
@@ -6969,7 +6964,7 @@
       <c r="E109" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F109" s="2" t="s">
+      <c r="F109" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G109" s="1" t="s">
@@ -7004,7 +6999,7 @@
       <c r="E110" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F110" s="2" t="s">
+      <c r="F110" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G110" s="1" t="s">
@@ -7039,10 +7034,10 @@
       <c r="E111" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F111" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G111" s="2" t="s">
+      <c r="F111" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G111" s="1" t="s">
         <v>257</v>
       </c>
       <c r="H111" s="1" t="s">
@@ -7074,10 +7069,10 @@
       <c r="E112" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F112" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G112" s="2" t="s">
+      <c r="F112" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G112" s="1" t="s">
         <v>257</v>
       </c>
       <c r="H112" s="1" t="s">
@@ -7109,10 +7104,10 @@
       <c r="E113" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F113" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G113" s="2" t="s">
+      <c r="F113" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G113" s="1" t="s">
         <v>261</v>
       </c>
       <c r="H113" s="1" t="s">
@@ -7144,10 +7139,10 @@
       <c r="E114" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F114" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G114" s="2" t="s">
+      <c r="F114" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G114" s="1" t="s">
         <v>264</v>
       </c>
       <c r="H114" s="1" t="s">
@@ -7179,10 +7174,10 @@
       <c r="E115" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F115" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G115" s="2" t="s">
+      <c r="F115" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G115" s="1" t="s">
         <v>266</v>
       </c>
       <c r="H115" s="1" t="s">
@@ -7214,10 +7209,10 @@
       <c r="E116" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F116" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G116" s="2" t="s">
+      <c r="F116" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G116" s="1" t="s">
         <v>248</v>
       </c>
       <c r="H116" s="1" t="s">
@@ -7249,10 +7244,10 @@
       <c r="E117" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F117" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G117" s="2" t="s">
+      <c r="F117" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G117" s="1" t="s">
         <v>241</v>
       </c>
       <c r="H117" s="1" t="s">
@@ -7284,7 +7279,7 @@
       <c r="E118" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F118" s="2" t="s">
+      <c r="F118" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G118" s="1" t="s">
@@ -7319,7 +7314,7 @@
       <c r="E119" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F119" s="2" t="s">
+      <c r="F119" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G119" s="1" t="s">
@@ -7354,7 +7349,7 @@
       <c r="E120" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F120" s="2" t="s">
+      <c r="F120" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G120" s="1" t="s">
@@ -7389,7 +7384,7 @@
       <c r="E121" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F121" s="2" t="s">
+      <c r="F121" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G121" s="1" t="s">
@@ -7424,7 +7419,7 @@
       <c r="E122" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F122" s="2" t="s">
+      <c r="F122" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G122" s="1" t="s">
@@ -7459,7 +7454,7 @@
       <c r="E123" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F123" s="2" t="s">
+      <c r="F123" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G123" s="1" t="s">
@@ -7494,7 +7489,7 @@
       <c r="E124" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="F124" s="2" t="s">
+      <c r="F124" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G124" s="1" t="s">
@@ -7529,7 +7524,7 @@
       <c r="E125" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F125" s="2" t="s">
+      <c r="F125" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G125" s="1" t="s">
@@ -7564,7 +7559,7 @@
       <c r="E126" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F126" s="2" t="s">
+      <c r="F126" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G126" s="1" t="s">
@@ -7599,7 +7594,7 @@
       <c r="E127" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F127" s="2" t="s">
+      <c r="F127" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G127" s="1" t="s">
@@ -7634,7 +7629,7 @@
       <c r="E128" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F128" s="2" t="s">
+      <c r="F128" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G128" s="1" t="s">
@@ -7669,7 +7664,7 @@
       <c r="E129" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="F129" s="2" t="s">
+      <c r="F129" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G129" s="1" t="s">
@@ -7704,7 +7699,7 @@
       <c r="E130" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F130" s="2" t="s">
+      <c r="F130" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G130" s="1" t="s">
@@ -7739,7 +7734,7 @@
       <c r="E131" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="F131" s="2" t="s">
+      <c r="F131" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G131" s="1" t="s">
@@ -7774,7 +7769,7 @@
       <c r="E132" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F132" s="2" t="s">
+      <c r="F132" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G132" s="1" t="s">
@@ -7809,7 +7804,7 @@
       <c r="E133" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="F133" s="2" t="s">
+      <c r="F133" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G133" s="1" t="s">
@@ -7844,7 +7839,7 @@
       <c r="E134" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F134" s="2" t="s">
+      <c r="F134" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G134" s="1" t="s">
@@ -7879,7 +7874,7 @@
       <c r="E135" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="F135" s="2" t="s">
+      <c r="F135" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G135" s="1" t="s">
@@ -7914,7 +7909,7 @@
       <c r="E136" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F136" s="2" t="s">
+      <c r="F136" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G136" s="1" t="s">
@@ -7949,7 +7944,7 @@
       <c r="E137" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F137" s="2" t="s">
+      <c r="F137" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G137" s="1" t="s">
@@ -7984,7 +7979,7 @@
       <c r="E138" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F138" s="2" t="s">
+      <c r="F138" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G138" s="1" t="s">
@@ -8019,7 +8014,7 @@
       <c r="E139" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="F139" s="2" t="s">
+      <c r="F139" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G139" s="1" t="s">
@@ -8054,7 +8049,7 @@
       <c r="E140" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F140" s="2" t="s">
+      <c r="F140" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G140" s="1" t="s">
@@ -8089,7 +8084,7 @@
       <c r="E141" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="F141" s="2" t="s">
+      <c r="F141" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G141" s="1" t="s">
@@ -8124,7 +8119,7 @@
       <c r="E142" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F142" s="2" t="s">
+      <c r="F142" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G142" s="1" t="s">
@@ -8159,7 +8154,7 @@
       <c r="E143" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="F143" s="2" t="s">
+      <c r="F143" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G143" s="1" t="s">
@@ -8194,7 +8189,7 @@
       <c r="E144" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F144" s="2" t="s">
+      <c r="F144" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G144" s="1" t="s">
@@ -8229,7 +8224,7 @@
       <c r="E145" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F145" s="2" t="s">
+      <c r="F145" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G145" s="1" t="s">
@@ -8264,7 +8259,7 @@
       <c r="E146" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F146" s="2" t="s">
+      <c r="F146" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G146" s="1" t="s">
@@ -8299,7 +8294,7 @@
       <c r="E147" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="F147" s="2" t="s">
+      <c r="F147" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G147" s="1" t="s">
@@ -8334,7 +8329,7 @@
       <c r="E148" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F148" s="2" t="s">
+      <c r="F148" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G148" s="1" t="s">
@@ -8369,7 +8364,7 @@
       <c r="E149" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="F149" s="2" t="s">
+      <c r="F149" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G149" s="1" t="s">
@@ -8404,7 +8399,7 @@
       <c r="E150" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F150" s="2" t="s">
+      <c r="F150" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G150" s="1" t="s">
@@ -8439,7 +8434,7 @@
       <c r="E151" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="F151" s="2" t="s">
+      <c r="F151" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G151" s="1" t="s">
@@ -8474,7 +8469,7 @@
       <c r="E152" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F152" s="2" t="s">
+      <c r="F152" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G152" s="1" t="s">
@@ -8509,7 +8504,7 @@
       <c r="E153" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="F153" s="2" t="s">
+      <c r="F153" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G153" s="1" t="s">
@@ -8544,7 +8539,7 @@
       <c r="E154" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F154" s="2" t="s">
+      <c r="F154" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G154" s="1" t="s">
@@ -8579,7 +8574,7 @@
       <c r="E155" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="F155" s="2" t="s">
+      <c r="F155" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G155" s="1" t="s">
@@ -8614,7 +8609,7 @@
       <c r="E156" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F156" s="2" t="s">
+      <c r="F156" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G156" s="1" t="s">
@@ -8649,7 +8644,7 @@
       <c r="E157" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="F157" s="2" t="s">
+      <c r="F157" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G157" s="1" t="s">
@@ -8684,7 +8679,7 @@
       <c r="E158" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F158" s="2" t="s">
+      <c r="F158" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G158" s="1" t="s">
@@ -8719,7 +8714,7 @@
       <c r="E159" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="F159" s="2" t="s">
+      <c r="F159" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G159" s="1" t="s">
@@ -8754,7 +8749,7 @@
       <c r="E160" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F160" s="2" t="s">
+      <c r="F160" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G160" s="1" t="s">
@@ -8789,7 +8784,7 @@
       <c r="E161" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="F161" s="2" t="s">
+      <c r="F161" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G161" s="1" t="s">
@@ -8824,7 +8819,7 @@
       <c r="E162" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F162" s="2" t="s">
+      <c r="F162" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G162" s="1" t="s">
@@ -8859,7 +8854,7 @@
       <c r="E163" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F163" s="2" t="s">
+      <c r="F163" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G163" s="1" t="s">
@@ -8894,7 +8889,7 @@
       <c r="E164" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="F164" s="2" t="s">
+      <c r="F164" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G164" s="1" t="s">
@@ -8929,7 +8924,7 @@
       <c r="E165" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F165" s="2" t="s">
+      <c r="F165" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G165" s="1" t="s">
@@ -8964,7 +8959,7 @@
       <c r="E166" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F166" s="2" t="s">
+      <c r="F166" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G166" s="1" t="s">
@@ -8999,7 +8994,7 @@
       <c r="E167" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F167" s="2" t="s">
+      <c r="F167" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G167" s="1" t="s">
@@ -9034,7 +9029,7 @@
       <c r="E168" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="F168" s="2" t="s">
+      <c r="F168" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G168" s="1" t="s">
@@ -9069,7 +9064,7 @@
       <c r="E169" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F169" s="2" t="s">
+      <c r="F169" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G169" s="1" t="s">
@@ -9104,7 +9099,7 @@
       <c r="E170" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="F170" s="2" t="s">
+      <c r="F170" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G170" s="1" t="s">
@@ -9139,7 +9134,7 @@
       <c r="E171" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F171" s="2" t="s">
+      <c r="F171" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G171" s="1" t="s">
@@ -9174,7 +9169,7 @@
       <c r="E172" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="F172" s="2" t="s">
+      <c r="F172" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G172" s="1" t="s">
@@ -9209,7 +9204,7 @@
       <c r="E173" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F173" s="2" t="s">
+      <c r="F173" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G173" s="1" t="s">
@@ -9244,7 +9239,7 @@
       <c r="E174" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="F174" s="2" t="s">
+      <c r="F174" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G174" s="1" t="s">
@@ -9279,7 +9274,7 @@
       <c r="E175" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F175" s="2" t="s">
+      <c r="F175" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G175" s="1" t="s">
@@ -9314,7 +9309,7 @@
       <c r="E176" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="F176" s="2" t="s">
+      <c r="F176" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G176" s="1" t="s">
@@ -9349,7 +9344,7 @@
       <c r="E177" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F177" s="2" t="s">
+      <c r="F177" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G177" s="1" t="s">
@@ -9384,7 +9379,7 @@
       <c r="E178" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="F178" s="2" t="s">
+      <c r="F178" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G178" s="1" t="s">
@@ -9419,7 +9414,7 @@
       <c r="E179" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F179" s="2" t="s">
+      <c r="F179" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G179" s="1" t="s">
@@ -9454,7 +9449,7 @@
       <c r="E180" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="F180" s="2" t="s">
+      <c r="F180" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G180" s="1" t="s">
@@ -9489,7 +9484,7 @@
       <c r="E181" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F181" s="2" t="s">
+      <c r="F181" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G181" s="1" t="s">
@@ -9524,7 +9519,7 @@
       <c r="E182" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="F182" s="2" t="s">
+      <c r="F182" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G182" s="1" t="s">
@@ -9559,7 +9554,7 @@
       <c r="E183" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F183" s="2" t="s">
+      <c r="F183" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G183" s="1" t="s">
@@ -9594,7 +9589,7 @@
       <c r="E184" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="F184" s="2" t="s">
+      <c r="F184" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G184" s="1" t="s">
@@ -9629,7 +9624,7 @@
       <c r="E185" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F185" s="2" t="s">
+      <c r="F185" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G185" s="1" t="s">
@@ -9664,7 +9659,7 @@
       <c r="E186" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="F186" s="2" t="s">
+      <c r="F186" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G186" s="1" t="s">
@@ -9699,7 +9694,7 @@
       <c r="E187" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F187" s="2" t="s">
+      <c r="F187" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G187" s="1" t="s">
@@ -9734,7 +9729,7 @@
       <c r="E188" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F188" s="2" t="s">
+      <c r="F188" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G188" s="1" t="s">
@@ -9769,7 +9764,7 @@
       <c r="E189" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F189" s="2" t="s">
+      <c r="F189" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G189" s="1" t="s">
@@ -9804,7 +9799,7 @@
       <c r="E190" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F190" s="2" t="s">
+      <c r="F190" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G190" s="1" t="s">
@@ -9839,7 +9834,7 @@
       <c r="E191" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F191" s="2" t="s">
+      <c r="F191" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G191" s="1" t="s">
@@ -9874,7 +9869,7 @@
       <c r="E192" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F192" s="2" t="s">
+      <c r="F192" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G192" s="1" t="s">
@@ -9909,7 +9904,7 @@
       <c r="E193" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="F193" s="2" t="s">
+      <c r="F193" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G193" s="1" t="s">
@@ -9944,7 +9939,7 @@
       <c r="E194" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F194" s="2" t="s">
+      <c r="F194" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G194" s="1" t="s">
@@ -9979,7 +9974,7 @@
       <c r="E195" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F195" s="2" t="s">
+      <c r="F195" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G195" s="1" t="s">
@@ -10014,7 +10009,7 @@
       <c r="E196" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F196" s="2" t="s">
+      <c r="F196" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G196" s="1" t="s">
@@ -10049,7 +10044,7 @@
       <c r="E197" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F197" s="2" t="s">
+      <c r="F197" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G197" s="1" t="s">
@@ -10084,7 +10079,7 @@
       <c r="E198" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F198" s="2" t="s">
+      <c r="F198" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G198" s="1" t="s">
@@ -10119,7 +10114,7 @@
       <c r="E199" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F199" s="2" t="s">
+      <c r="F199" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G199" s="1" t="s">
@@ -10154,7 +10149,7 @@
       <c r="E200" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F200" s="2" t="s">
+      <c r="F200" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G200" s="1" t="s">
@@ -10189,7 +10184,7 @@
       <c r="E201" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F201" s="2" t="s">
+      <c r="F201" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G201" s="1" t="s">
@@ -10224,7 +10219,7 @@
       <c r="E202" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F202" s="2" t="s">
+      <c r="F202" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G202" s="1" t="s">
@@ -10259,7 +10254,7 @@
       <c r="E203" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F203" s="2" t="s">
+      <c r="F203" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G203" s="1" t="s">
@@ -10294,7 +10289,7 @@
       <c r="E204" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F204" s="2" t="s">
+      <c r="F204" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G204" s="1" t="s">
@@ -10329,7 +10324,7 @@
       <c r="E205" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F205" s="2" t="s">
+      <c r="F205" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G205" s="1" t="s">
@@ -10364,7 +10359,7 @@
       <c r="E206" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="F206" s="2" t="s">
+      <c r="F206" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G206" s="1" t="s">
@@ -10399,7 +10394,7 @@
       <c r="E207" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F207" s="2" t="s">
+      <c r="F207" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G207" s="1" t="s">
@@ -10434,7 +10429,7 @@
       <c r="E208" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F208" s="2" t="s">
+      <c r="F208" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G208" s="1" t="s">
@@ -10469,7 +10464,7 @@
       <c r="E209" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F209" s="2" t="s">
+      <c r="F209" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G209" s="1" t="s">
@@ -10504,7 +10499,7 @@
       <c r="E210" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F210" s="2" t="s">
+      <c r="F210" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G210" s="1" t="s">
@@ -10539,7 +10534,7 @@
       <c r="E211" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F211" s="2" t="s">
+      <c r="F211" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G211" s="1" t="s">
@@ -10571,13 +10566,13 @@
       <c r="D212" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E212" s="2" t="s">
+      <c r="E212" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F212" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G212" s="2" t="s">
+      <c r="F212" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G212" s="1" t="s">
         <v>414</v>
       </c>
       <c r="H212" s="1" t="s">
@@ -10606,13 +10601,13 @@
       <c r="D213" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E213" s="2" t="s">
+      <c r="E213" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F213" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G213" s="2" t="s">
+      <c r="F213" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G213" s="1" t="s">
         <v>414</v>
       </c>
       <c r="H213" s="1" t="s">
@@ -10644,7 +10639,7 @@
       <c r="E214" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F214" s="2" t="s">
+      <c r="F214" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G214" s="1" t="s">
@@ -10679,7 +10674,7 @@
       <c r="E215" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F215" s="2" t="s">
+      <c r="F215" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G215" s="1" t="s">
@@ -10714,7 +10709,7 @@
       <c r="E216" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F216" s="2" t="s">
+      <c r="F216" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G216" s="1" t="s">
@@ -10749,7 +10744,7 @@
       <c r="E217" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F217" s="2" t="s">
+      <c r="F217" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G217" s="1" t="s">
@@ -10784,7 +10779,7 @@
       <c r="E218" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F218" s="2" t="s">
+      <c r="F218" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G218" s="1" t="s">
@@ -10819,7 +10814,7 @@
       <c r="E219" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F219" s="2" t="s">
+      <c r="F219" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G219" s="1" t="s">
@@ -10851,13 +10846,13 @@
       <c r="D220" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E220" s="2" t="s">
+      <c r="E220" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F220" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G220" s="2" t="s">
+      <c r="F220" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G220" s="1" t="s">
         <v>79</v>
       </c>
       <c r="H220" s="1" t="s">
@@ -10886,13 +10881,13 @@
       <c r="D221" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E221" s="2" t="s">
+      <c r="E221" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F221" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G221" s="2" t="s">
+      <c r="F221" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G221" s="1" t="s">
         <v>79</v>
       </c>
       <c r="H221" s="1" t="s">
@@ -10921,13 +10916,13 @@
       <c r="D222" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E222" s="2" t="s">
+      <c r="E222" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F222" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G222" s="2" t="s">
+      <c r="F222" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G222" s="1" t="s">
         <v>415</v>
       </c>
       <c r="H222" s="1" t="s">
@@ -10956,13 +10951,13 @@
       <c r="D223" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E223" s="2" t="s">
+      <c r="E223" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F223" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G223" s="2" t="s">
+      <c r="F223" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G223" s="1" t="s">
         <v>415</v>
       </c>
       <c r="H223" s="1" t="s">
@@ -10991,13 +10986,13 @@
       <c r="D224" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E224" s="2" t="s">
+      <c r="E224" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F224" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G224" s="2" t="s">
+      <c r="F224" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G224" s="1" t="s">
         <v>87</v>
       </c>
       <c r="H224" s="1" t="s">
@@ -11026,13 +11021,13 @@
       <c r="D225" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E225" s="2" t="s">
+      <c r="E225" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F225" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G225" s="2" t="s">
+      <c r="F225" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G225" s="1" t="s">
         <v>87</v>
       </c>
       <c r="H225" s="1" t="s">
@@ -11064,7 +11059,7 @@
       <c r="E226" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F226" s="2" t="s">
+      <c r="F226" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G226" s="1" t="s">
@@ -11099,7 +11094,7 @@
       <c r="E227" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F227" s="2" t="s">
+      <c r="F227" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G227" s="1" t="s">
@@ -11134,7 +11129,7 @@
       <c r="E228" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F228" s="2" t="s">
+      <c r="F228" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G228" s="1" t="s">
@@ -11169,7 +11164,7 @@
       <c r="E229" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F229" s="2" t="s">
+      <c r="F229" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G229" s="1" t="s">
@@ -11204,7 +11199,7 @@
       <c r="E230" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="F230" s="2" t="s">
+      <c r="F230" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G230" s="1" t="s">
@@ -11239,7 +11234,7 @@
       <c r="E231" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F231" s="2" t="s">
+      <c r="F231" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G231" s="1" t="s">
@@ -11274,7 +11269,7 @@
       <c r="E232" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F232" s="2" t="s">
+      <c r="F232" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G232" s="1" t="s">
@@ -11306,13 +11301,13 @@
       <c r="D233" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E233" s="2" t="s">
+      <c r="E233" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="F233" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G233" s="2" t="s">
+      <c r="F233" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G233" s="1" t="s">
         <v>422</v>
       </c>
       <c r="H233" s="1" t="s">
@@ -11344,7 +11339,7 @@
       <c r="E234" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F234" s="2" t="s">
+      <c r="F234" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G234" s="1" t="s">
@@ -11379,7 +11374,7 @@
       <c r="E235" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F235" s="2" t="s">
+      <c r="F235" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G235" s="1" t="s">
@@ -11414,7 +11409,7 @@
       <c r="E236" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="F236" s="2" t="s">
+      <c r="F236" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G236" s="1" t="s">
@@ -11449,7 +11444,7 @@
       <c r="E237" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F237" s="2" t="s">
+      <c r="F237" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G237" s="1" t="s">
@@ -11484,7 +11479,7 @@
       <c r="E238" s="3" t="s">
         <v>432</v>
       </c>
-      <c r="F238" s="4" t="s">
+      <c r="F238" s="3" t="s">
         <v>207</v>
       </c>
       <c r="G238" s="3" t="s">
@@ -11529,7 +11524,7 @@
       <c r="E239" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="F239" s="5" t="s">
+      <c r="F239" s="4" t="s">
         <v>207</v>
       </c>
       <c r="G239" s="1" t="s">
@@ -11564,7 +11559,7 @@
       <c r="E240" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="F240" s="5" t="s">
+      <c r="F240" s="4" t="s">
         <v>207</v>
       </c>
       <c r="G240" s="1" t="s">
@@ -11599,7 +11594,7 @@
       <c r="E241" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="F241" s="5" t="s">
+      <c r="F241" s="4" t="s">
         <v>207</v>
       </c>
       <c r="G241" s="1" t="s">
@@ -11634,7 +11629,7 @@
       <c r="E242" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="F242" s="5" t="s">
+      <c r="F242" s="4" t="s">
         <v>207</v>
       </c>
       <c r="G242" s="1" t="s">
@@ -11669,7 +11664,7 @@
       <c r="E243" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="F243" s="5" t="s">
+      <c r="F243" s="4" t="s">
         <v>207</v>
       </c>
       <c r="G243" s="1" t="s">
@@ -11704,7 +11699,7 @@
       <c r="E244" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="F244" s="5" t="s">
+      <c r="F244" s="4" t="s">
         <v>207</v>
       </c>
       <c r="G244" s="1" t="s">
@@ -11739,7 +11734,7 @@
       <c r="E245" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="F245" s="5" t="s">
+      <c r="F245" s="4" t="s">
         <v>207</v>
       </c>
       <c r="G245" s="1" t="s">
@@ -11774,7 +11769,7 @@
       <c r="E246" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F246" s="2" t="s">
+      <c r="F246" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G246" s="1" t="s">
@@ -11809,7 +11804,7 @@
       <c r="E247" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F247" s="2" t="s">
+      <c r="F247" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G247" s="1" t="s">
@@ -11844,7 +11839,7 @@
       <c r="E248" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F248" s="2" t="s">
+      <c r="F248" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G248" s="1" t="s">
@@ -11879,7 +11874,7 @@
       <c r="E249" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F249" s="2" t="s">
+      <c r="F249" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G249" s="1" t="s">
@@ -11914,7 +11909,7 @@
       <c r="E250" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F250" s="2" t="s">
+      <c r="F250" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G250" s="1" t="s">
@@ -11949,7 +11944,7 @@
       <c r="E251" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="F251" s="2" t="s">
+      <c r="F251" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G251" s="1" t="s">
@@ -11984,7 +11979,7 @@
       <c r="E252" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F252" s="2" t="s">
+      <c r="F252" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G252" s="1" t="s">
@@ -12019,7 +12014,7 @@
       <c r="E253" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F253" s="2" t="s">
+      <c r="F253" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G253" s="1" t="s">
@@ -12054,7 +12049,7 @@
       <c r="E254" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F254" s="2" t="s">
+      <c r="F254" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G254" s="1" t="s">
@@ -12089,7 +12084,7 @@
       <c r="E255" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F255" s="2" t="s">
+      <c r="F255" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G255" s="1" t="s">
@@ -12124,7 +12119,7 @@
       <c r="E256" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F256" s="2" t="s">
+      <c r="F256" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G256" s="1" t="s">
@@ -12159,7 +12154,7 @@
       <c r="E257" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F257" s="2" t="s">
+      <c r="F257" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G257" s="1" t="s">
@@ -12194,7 +12189,7 @@
       <c r="E258" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F258" s="2" t="s">
+      <c r="F258" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G258" s="1" t="s">
@@ -12229,7 +12224,7 @@
       <c r="E259" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F259" s="2" t="s">
+      <c r="F259" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G259" s="1" t="s">
@@ -12264,7 +12259,7 @@
       <c r="E260" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F260" s="2" t="s">
+      <c r="F260" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G260" s="1" t="s">
@@ -12299,7 +12294,7 @@
       <c r="E261" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F261" s="2" t="s">
+      <c r="F261" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G261" s="1" t="s">
@@ -12334,7 +12329,7 @@
       <c r="E262" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F262" s="2" t="s">
+      <c r="F262" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G262" s="1" t="s">
@@ -12369,7 +12364,7 @@
       <c r="E263" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="F263" s="2" t="s">
+      <c r="F263" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G263" s="1" t="s">
@@ -12404,7 +12399,7 @@
       <c r="E264" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F264" s="2" t="s">
+      <c r="F264" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G264" s="1" t="s">
@@ -12439,7 +12434,7 @@
       <c r="E265" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F265" s="2" t="s">
+      <c r="F265" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G265" s="1" t="s">
@@ -12474,7 +12469,7 @@
       <c r="E266" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F266" s="2" t="s">
+      <c r="F266" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G266" s="1" t="s">
@@ -12509,7 +12504,7 @@
       <c r="E267" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="F267" s="2" t="s">
+      <c r="F267" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G267" s="1" t="s">
@@ -12544,7 +12539,7 @@
       <c r="E268" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F268" s="2" t="s">
+      <c r="F268" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G268" s="1" t="s">
@@ -12579,7 +12574,7 @@
       <c r="E269" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F269" s="2" t="s">
+      <c r="F269" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G269" s="1" t="s">
@@ -12611,13 +12606,13 @@
       <c r="D270" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E270" s="2" t="s">
+      <c r="E270" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="F270" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G270" s="2" t="s">
+      <c r="F270" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G270" s="1" t="s">
         <v>485</v>
       </c>
       <c r="H270" s="1" t="s">
@@ -12649,7 +12644,7 @@
       <c r="E271" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F271" s="2" t="s">
+      <c r="F271" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G271" s="1" t="s">
@@ -12684,7 +12679,7 @@
       <c r="E272" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="F272" s="2" t="s">
+      <c r="F272" s="1" t="s">
         <v>207</v>
       </c>
       <c r="G272" s="1" t="s">
@@ -12719,7 +12714,7 @@
       <c r="E273" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F273" s="2" t="s">
+      <c r="F273" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G273" s="1" t="s">
@@ -12751,13 +12746,13 @@
       <c r="D274" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E274" s="2" t="s">
+      <c r="E274" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F274" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G274" s="2" t="s">
+      <c r="F274" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G274" s="1" t="s">
         <v>500</v>
       </c>
       <c r="H274" s="1" t="s">
@@ -12789,7 +12784,7 @@
       <c r="E275" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F275" s="2" t="s">
+      <c r="F275" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G275" s="1" t="s">
@@ -12824,7 +12819,7 @@
       <c r="E276" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F276" s="2" t="s">
+      <c r="F276" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G276" s="1" t="s">
@@ -12859,7 +12854,7 @@
       <c r="E277" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F277" s="2" t="s">
+      <c r="F277" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G277" s="1" t="s">
@@ -12891,13 +12886,13 @@
       <c r="D278" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E278" s="2" t="s">
+      <c r="E278" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F278" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G278" s="2" t="s">
+      <c r="F278" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G278" s="1" t="s">
         <v>79</v>
       </c>
       <c r="H278" s="1" t="s">
@@ -12926,13 +12921,13 @@
       <c r="D279" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E279" s="2" t="s">
+      <c r="E279" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F279" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G279" s="2" t="s">
+      <c r="F279" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G279" s="1" t="s">
         <v>79</v>
       </c>
       <c r="H279" s="1" t="s">
@@ -12964,7 +12959,7 @@
       <c r="E280" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F280" s="2" t="s">
+      <c r="F280" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G280" s="1" t="s">
@@ -12996,13 +12991,13 @@
       <c r="D281" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E281" s="2" t="s">
+      <c r="E281" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F281" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G281" s="2" t="s">
+      <c r="F281" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G281" s="1" t="s">
         <v>500</v>
       </c>
       <c r="H281" s="1" t="s">
@@ -13031,13 +13026,13 @@
       <c r="D282" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E282" s="2" t="s">
+      <c r="E282" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F282" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G282" s="2" t="s">
+      <c r="F282" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G282" s="1" t="s">
         <v>510</v>
       </c>
       <c r="H282" s="1" t="s">
@@ -13069,7 +13064,7 @@
       <c r="E283" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F283" s="2" t="s">
+      <c r="F283" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G283" s="1" t="s">
@@ -13104,7 +13099,7 @@
       <c r="E284" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F284" s="2" t="s">
+      <c r="F284" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G284" s="1" t="s">
@@ -13139,7 +13134,7 @@
       <c r="E285" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F285" s="2" t="s">
+      <c r="F285" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G285" s="1" t="s">
@@ -13174,7 +13169,7 @@
       <c r="E286" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F286" s="2" t="s">
+      <c r="F286" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G286" s="1" t="s">
@@ -13209,7 +13204,7 @@
       <c r="E287" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F287" s="2" t="s">
+      <c r="F287" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G287" s="1" t="s">
@@ -13244,7 +13239,7 @@
       <c r="E288" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F288" s="2" t="s">
+      <c r="F288" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G288" s="1" t="s">
@@ -13279,7 +13274,7 @@
       <c r="E289" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F289" s="2" t="s">
+      <c r="F289" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G289" s="1" t="s">
@@ -13314,7 +13309,7 @@
       <c r="E290" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F290" s="2" t="s">
+      <c r="F290" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G290" s="1" t="s">
@@ -13349,7 +13344,7 @@
       <c r="E291" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F291" s="2" t="s">
+      <c r="F291" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G291" s="1" t="s">
@@ -13384,7 +13379,7 @@
       <c r="E292" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F292" s="2" t="s">
+      <c r="F292" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G292" s="1" t="s">
@@ -13419,7 +13414,7 @@
       <c r="E293" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F293" s="2" t="s">
+      <c r="F293" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G293" s="1" t="s">
@@ -13454,7 +13449,7 @@
       <c r="E294" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F294" s="2" t="s">
+      <c r="F294" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G294" s="1" t="s">
@@ -13489,7 +13484,7 @@
       <c r="E295" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F295" s="2" t="s">
+      <c r="F295" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G295" s="1" t="s">
@@ -13524,7 +13519,7 @@
       <c r="E296" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F296" s="2" t="s">
+      <c r="F296" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G296" s="1" t="s">
@@ -13559,7 +13554,7 @@
       <c r="E297" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F297" s="2" t="s">
+      <c r="F297" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G297" s="1" t="s">
@@ -13594,7 +13589,7 @@
       <c r="E298" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F298" s="2" t="s">
+      <c r="F298" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G298" s="1" t="s">
@@ -13629,7 +13624,7 @@
       <c r="E299" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F299" s="2" t="s">
+      <c r="F299" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G299" s="1" t="s">
@@ -13664,7 +13659,7 @@
       <c r="E300" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F300" s="2" t="s">
+      <c r="F300" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G300" s="1" t="s">
@@ -13699,7 +13694,7 @@
       <c r="E301" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="F301" s="2" t="s">
+      <c r="F301" s="1" t="s">
         <v>207</v>
       </c>
       <c r="G301" s="1" t="s">
@@ -13734,10 +13729,10 @@
       <c r="E302" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="F302" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G302" s="2" t="s">
+      <c r="F302" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G302" s="1" t="s">
         <v>484</v>
       </c>
       <c r="H302" s="1" t="s">
@@ -13769,7 +13764,7 @@
       <c r="E303" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="F303" s="2" t="s">
+      <c r="F303" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G303" s="1" t="s">
@@ -13804,7 +13799,7 @@
       <c r="E304" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="F304" s="2" t="s">
+      <c r="F304" s="1" t="s">
         <v>207</v>
       </c>
       <c r="G304" s="1" t="s">
@@ -13839,7 +13834,7 @@
       <c r="E305" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F305" s="2" t="s">
+      <c r="F305" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G305" s="1" t="s">
@@ -13874,7 +13869,7 @@
       <c r="E306" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F306" s="2" t="s">
+      <c r="F306" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G306" s="1" t="s">
@@ -13909,7 +13904,7 @@
       <c r="E307" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="F307" s="2" t="s">
+      <c r="F307" s="1" t="s">
         <v>207</v>
       </c>
       <c r="G307" s="1" t="s">
@@ -13944,7 +13939,7 @@
       <c r="E308" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F308" s="2" t="s">
+      <c r="F308" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G308" s="1" t="s">
@@ -13979,7 +13974,7 @@
       <c r="E309" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F309" s="2" t="s">
+      <c r="F309" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G309" s="1" t="s">
@@ -14014,7 +14009,7 @@
       <c r="E310" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F310" s="2" t="s">
+      <c r="F310" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G310" s="1" t="s">
@@ -14049,10 +14044,10 @@
       <c r="E311" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F311" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G311" s="2" t="s">
+      <c r="F311" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G311" s="1" t="s">
         <v>572</v>
       </c>
       <c r="H311" s="1" t="s">
@@ -14084,7 +14079,7 @@
       <c r="E312" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F312" s="2" t="s">
+      <c r="F312" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G312" s="1" t="s">
@@ -14119,7 +14114,7 @@
       <c r="E313" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F313" s="2" t="s">
+      <c r="F313" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G313" s="1" t="s">
@@ -14154,7 +14149,7 @@
       <c r="E314" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F314" s="2" t="s">
+      <c r="F314" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G314" s="1" t="s">
@@ -14189,7 +14184,7 @@
       <c r="E315" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F315" s="2" t="s">
+      <c r="F315" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G315" s="1" t="s">
@@ -14224,7 +14219,7 @@
       <c r="E316" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F316" s="2" t="s">
+      <c r="F316" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G316" s="1" t="s">
@@ -14259,7 +14254,7 @@
       <c r="E317" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F317" s="2" t="s">
+      <c r="F317" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G317" s="1" t="s">
@@ -14294,7 +14289,7 @@
       <c r="E318" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F318" s="2" t="s">
+      <c r="F318" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G318" s="1" t="s">
@@ -14329,7 +14324,7 @@
       <c r="E319" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F319" s="2" t="s">
+      <c r="F319" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G319" s="1" t="s">
@@ -14364,7 +14359,7 @@
       <c r="E320" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F320" s="2" t="s">
+      <c r="F320" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G320" s="1" t="s">
@@ -14399,7 +14394,7 @@
       <c r="E321" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F321" s="2" t="s">
+      <c r="F321" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G321" s="1" t="s">
@@ -14434,7 +14429,7 @@
       <c r="E322" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F322" s="2" t="s">
+      <c r="F322" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G322" s="1" t="s">
@@ -14469,7 +14464,7 @@
       <c r="E323" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F323" s="2" t="s">
+      <c r="F323" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G323" s="1" t="s">
@@ -14504,7 +14499,7 @@
       <c r="E324" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F324" s="2" t="s">
+      <c r="F324" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G324" s="1" t="s">
@@ -14539,7 +14534,7 @@
       <c r="E325" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F325" s="2" t="s">
+      <c r="F325" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G325" s="1" t="s">
@@ -14574,7 +14569,7 @@
       <c r="E326" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F326" s="2" t="s">
+      <c r="F326" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G326" s="1" t="s">
@@ -14609,7 +14604,7 @@
       <c r="E327" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F327" s="2" t="s">
+      <c r="F327" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G327" s="1" t="s">
@@ -14644,7 +14639,7 @@
       <c r="E328" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F328" s="2" t="s">
+      <c r="F328" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G328" s="1" t="s">
@@ -14679,7 +14674,7 @@
       <c r="E329" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F329" s="2" t="s">
+      <c r="F329" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G329" s="1" t="s">
@@ -14714,7 +14709,7 @@
       <c r="E330" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F330" s="2" t="s">
+      <c r="F330" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G330" s="1" t="s">
@@ -14749,7 +14744,7 @@
       <c r="E331" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F331" s="2" t="s">
+      <c r="F331" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G331" s="1" t="s">
@@ -14784,7 +14779,7 @@
       <c r="E332" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F332" s="2" t="s">
+      <c r="F332" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G332" s="1" t="s">
@@ -14819,7 +14814,7 @@
       <c r="E333" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F333" s="2" t="s">
+      <c r="F333" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G333" s="1" t="s">
@@ -14854,7 +14849,7 @@
       <c r="E334" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F334" s="2" t="s">
+      <c r="F334" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G334" s="1" t="s">
@@ -14889,7 +14884,7 @@
       <c r="E335" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F335" s="2" t="s">
+      <c r="F335" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G335" s="1" t="s">
@@ -14924,7 +14919,7 @@
       <c r="E336" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F336" s="2" t="s">
+      <c r="F336" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G336" s="1" t="s">
@@ -14959,7 +14954,7 @@
       <c r="E337" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F337" s="2" t="s">
+      <c r="F337" s="1" t="s">
         <v>207</v>
       </c>
       <c r="G337" s="1" t="s">
@@ -14994,7 +14989,7 @@
       <c r="E338" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F338" s="2" t="s">
+      <c r="F338" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G338" s="1" t="s">
@@ -15029,7 +15024,7 @@
       <c r="E339" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F339" s="2" t="s">
+      <c r="F339" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G339" s="1" t="s">
@@ -15064,7 +15059,7 @@
       <c r="E340" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F340" s="2" t="s">
+      <c r="F340" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G340" s="1" t="s">
@@ -15099,7 +15094,7 @@
       <c r="E341" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F341" s="2" t="s">
+      <c r="F341" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G341" s="1" t="s">
@@ -15134,7 +15129,7 @@
       <c r="E342" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F342" s="2" t="s">
+      <c r="F342" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G342" s="1" t="s">
@@ -15169,7 +15164,7 @@
       <c r="E343" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F343" s="2" t="s">
+      <c r="F343" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G343" s="1" t="s">
@@ -15204,7 +15199,7 @@
       <c r="E344" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F344" s="2" t="s">
+      <c r="F344" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G344" s="1" t="s">
@@ -15239,7 +15234,7 @@
       <c r="E345" s="1" t="s">
         <v>647</v>
       </c>
-      <c r="F345" s="2" t="s">
+      <c r="F345" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G345" s="1" t="s">
@@ -15274,10 +15269,10 @@
       <c r="E346" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F346" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G346" s="2" t="s">
+      <c r="F346" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G346" s="1" t="s">
         <v>257</v>
       </c>
       <c r="H346" s="1" t="s">
@@ -15309,10 +15304,10 @@
       <c r="E347" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F347" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G347" s="2" t="s">
+      <c r="F347" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G347" s="1" t="s">
         <v>257</v>
       </c>
       <c r="H347" s="1" t="s">
@@ -15344,7 +15339,7 @@
       <c r="E348" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F348" s="2" t="s">
+      <c r="F348" s="1" t="s">
         <v>54</v>
       </c>
       <c r="G348" s="1" t="s">
@@ -15379,10 +15374,10 @@
       <c r="E349" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F349" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G349" s="2" t="s">
+      <c r="F349" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G349" s="1" t="s">
         <v>652</v>
       </c>
       <c r="H349" s="1" t="s">
@@ -15414,10 +15409,10 @@
       <c r="E350" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F350" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G350" s="2" t="s">
+      <c r="F350" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G350" s="1" t="s">
         <v>652</v>
       </c>
       <c r="H350" s="1" t="s">
@@ -15449,7 +15444,7 @@
       <c r="E351" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F351" s="2" t="s">
+      <c r="F351" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G351" s="1" t="s">
@@ -15484,10 +15479,10 @@
       <c r="E352" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F352" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G352" s="2" t="s">
+      <c r="F352" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G352" s="1" t="s">
         <v>652</v>
       </c>
       <c r="H352" s="1" t="s">
@@ -15519,7 +15514,7 @@
       <c r="E353" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F353" s="2" t="s">
+      <c r="F353" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G353" s="1" t="s">
@@ -15554,10 +15549,10 @@
       <c r="E354" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F354" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G354" s="2" t="s">
+      <c r="F354" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G354" s="1" t="s">
         <v>659</v>
       </c>
       <c r="H354" s="1" t="s">
@@ -15589,10 +15584,10 @@
       <c r="E355" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F355" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G355" s="2" t="s">
+      <c r="F355" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G355" s="1" t="s">
         <v>662</v>
       </c>
       <c r="H355" s="1" t="s">
@@ -15624,7 +15619,7 @@
       <c r="E356" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F356" s="2" t="s">
+      <c r="F356" s="1" t="s">
         <v>54</v>
       </c>
       <c r="G356" s="1" t="s">
@@ -15659,10 +15654,10 @@
       <c r="E357" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F357" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G357" s="2" t="s">
+      <c r="F357" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G357" s="1" t="s">
         <v>666</v>
       </c>
       <c r="H357" s="1" t="s">
@@ -15694,7 +15689,7 @@
       <c r="E358" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F358" s="2" t="s">
+      <c r="F358" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G358" s="1" t="s">
@@ -15729,7 +15724,7 @@
       <c r="E359" s="1" t="s">
         <v>672</v>
       </c>
-      <c r="F359" s="2" t="s">
+      <c r="F359" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G359" s="1" t="s">
@@ -15764,7 +15759,7 @@
       <c r="E360" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F360" s="2" t="s">
+      <c r="F360" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G360" s="1" t="s">
@@ -15799,7 +15794,7 @@
       <c r="E361" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F361" s="2" t="s">
+      <c r="F361" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G361" s="1" t="s">
@@ -15834,7 +15829,7 @@
       <c r="E362" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F362" s="2" t="s">
+      <c r="F362" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G362" s="1" t="s">
@@ -15869,7 +15864,7 @@
       <c r="E363" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F363" s="2" t="s">
+      <c r="F363" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G363" s="1" t="s">
@@ -15904,7 +15899,7 @@
       <c r="E364" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F364" s="2" t="s">
+      <c r="F364" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G364" s="1" t="s">
@@ -15939,7 +15934,7 @@
       <c r="E365" s="1" t="s">
         <v>689</v>
       </c>
-      <c r="F365" s="2" t="s">
+      <c r="F365" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G365" s="1" t="s">
@@ -15974,7 +15969,7 @@
       <c r="E366" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="F366" s="2" t="s">
+      <c r="F366" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G366" s="1" t="s">
@@ -16009,7 +16004,7 @@
       <c r="E367" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F367" s="2" t="s">
+      <c r="F367" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G367" s="1" t="s">
@@ -16044,7 +16039,7 @@
       <c r="E368" s="1" t="s">
         <v>699</v>
       </c>
-      <c r="F368" s="2" t="s">
+      <c r="F368" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G368" s="1" t="s">
@@ -16079,10 +16074,10 @@
       <c r="E369" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F369" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G369" s="2" t="s">
+      <c r="F369" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G369" s="1" t="s">
         <v>704</v>
       </c>
       <c r="H369" s="1" t="s">
@@ -16114,10 +16109,10 @@
       <c r="E370" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F370" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G370" s="2" t="s">
+      <c r="F370" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G370" s="1" t="s">
         <v>704</v>
       </c>
       <c r="H370" s="1" t="s">
@@ -16149,10 +16144,10 @@
       <c r="E371" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F371" s="2" t="s">
+      <c r="F371" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G371" s="2" t="s">
+      <c r="G371" s="1" t="s">
         <v>708</v>
       </c>
       <c r="H371" s="1" t="s">
@@ -16184,10 +16179,10 @@
       <c r="E372" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F372" s="2" t="s">
+      <c r="F372" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G372" s="2" t="s">
+      <c r="G372" s="1" t="s">
         <v>708</v>
       </c>
       <c r="H372" s="1" t="s">
@@ -16216,13 +16211,13 @@
       <c r="D373" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E373" s="2" t="s">
+      <c r="E373" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F373" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G373" s="2" t="s">
+      <c r="F373" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G373" s="1" t="s">
         <v>711</v>
       </c>
       <c r="H373" s="1" t="s">
@@ -16251,13 +16246,13 @@
       <c r="D374" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E374" s="2" t="s">
+      <c r="E374" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F374" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G374" s="2" t="s">
+      <c r="F374" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G374" s="1" t="s">
         <v>711</v>
       </c>
       <c r="H374" s="1" t="s">
@@ -16289,10 +16284,10 @@
       <c r="E375" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F375" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G375" s="2" t="s">
+      <c r="F375" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G375" s="1" t="s">
         <v>715</v>
       </c>
       <c r="H375" s="1" t="s">
@@ -16324,10 +16319,10 @@
       <c r="E376" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F376" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G376" s="2" t="s">
+      <c r="F376" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G376" s="1" t="s">
         <v>715</v>
       </c>
       <c r="H376" s="1" t="s">
@@ -16359,10 +16354,10 @@
       <c r="E377" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F377" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G377" s="2" t="s">
+      <c r="F377" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G377" s="1" t="s">
         <v>715</v>
       </c>
       <c r="H377" s="1" t="s">
@@ -16394,10 +16389,10 @@
       <c r="E378" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F378" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G378" s="2" t="s">
+      <c r="F378" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G378" s="1" t="s">
         <v>715</v>
       </c>
       <c r="H378" s="1" t="s">
@@ -16429,10 +16424,10 @@
       <c r="E379" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F379" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G379" s="2" t="s">
+      <c r="F379" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G379" s="1" t="s">
         <v>715</v>
       </c>
       <c r="H379" s="1" t="s">
@@ -16464,7 +16459,7 @@
       <c r="E380" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F380" s="2" t="s">
+      <c r="F380" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G380" s="1" t="s">
@@ -16496,13 +16491,13 @@
       <c r="D381" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E381" s="2" t="s">
+      <c r="E381" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F381" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G381" s="2" t="s">
+      <c r="F381" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G381" s="1" t="s">
         <v>720</v>
       </c>
       <c r="H381" s="1" t="s">
@@ -16531,13 +16526,13 @@
       <c r="D382" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E382" s="2" t="s">
+      <c r="E382" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F382" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G382" s="2" t="s">
+      <c r="F382" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G382" s="1" t="s">
         <v>720</v>
       </c>
       <c r="H382" s="1" t="s">
@@ -16566,13 +16561,13 @@
       <c r="D383" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E383" s="2" t="s">
+      <c r="E383" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F383" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G383" s="2" t="s">
+      <c r="F383" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G383" s="1" t="s">
         <v>724</v>
       </c>
       <c r="H383" s="1" t="s">
@@ -16601,13 +16596,13 @@
       <c r="D384" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E384" s="2" t="s">
+      <c r="E384" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F384" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G384" s="2" t="s">
+      <c r="F384" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G384" s="1" t="s">
         <v>724</v>
       </c>
       <c r="H384" s="1" t="s">
@@ -16636,13 +16631,13 @@
       <c r="D385" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E385" s="2" t="s">
+      <c r="E385" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F385" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G385" s="2" t="s">
+      <c r="F385" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G385" s="1" t="s">
         <v>415</v>
       </c>
       <c r="H385" s="1" t="s">
@@ -16671,13 +16666,13 @@
       <c r="D386" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E386" s="2" t="s">
+      <c r="E386" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F386" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G386" s="2" t="s">
+      <c r="F386" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G386" s="1" t="s">
         <v>415</v>
       </c>
       <c r="H386" s="1" t="s">
@@ -16706,13 +16701,13 @@
       <c r="D387" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E387" s="2" t="s">
+      <c r="E387" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F387" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G387" s="2" t="s">
+      <c r="F387" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G387" s="1" t="s">
         <v>87</v>
       </c>
       <c r="H387" s="1" t="s">
@@ -16741,13 +16736,13 @@
       <c r="D388" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E388" s="2" t="s">
+      <c r="E388" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F388" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G388" s="2" t="s">
+      <c r="F388" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G388" s="1" t="s">
         <v>87</v>
       </c>
       <c r="H388" s="1" t="s">
@@ -16779,10 +16774,10 @@
       <c r="E389" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F389" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G389" s="2" t="s">
+      <c r="F389" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G389" s="1" t="s">
         <v>732</v>
       </c>
       <c r="H389" s="1" t="s">
@@ -16814,7 +16809,7 @@
       <c r="E390" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F390" s="2" t="s">
+      <c r="F390" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G390" s="1" t="s">
@@ -16849,10 +16844,10 @@
       <c r="E391" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F391" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G391" s="2" t="s">
+      <c r="F391" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G391" s="1" t="s">
         <v>735</v>
       </c>
       <c r="H391" s="1" t="s">
@@ -16884,10 +16879,10 @@
       <c r="E392" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F392" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G392" s="2" t="s">
+      <c r="F392" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G392" s="1" t="s">
         <v>735</v>
       </c>
       <c r="H392" s="1" t="s">
@@ -16919,7 +16914,7 @@
       <c r="E393" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F393" s="2" t="s">
+      <c r="F393" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G393" s="1" t="s">
@@ -16954,7 +16949,7 @@
       <c r="E394" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F394" s="2" t="s">
+      <c r="F394" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G394" s="1" t="s">
@@ -16989,7 +16984,7 @@
       <c r="E395" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F395" s="2" t="s">
+      <c r="F395" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G395" s="1" t="s">
@@ -17024,7 +17019,7 @@
       <c r="E396" s="1" t="s">
         <v>745</v>
       </c>
-      <c r="F396" s="2" t="s">
+      <c r="F396" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G396" s="1" t="s">
@@ -17059,7 +17054,7 @@
       <c r="E397" s="1" t="s">
         <v>745</v>
       </c>
-      <c r="F397" s="2" t="s">
+      <c r="F397" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G397" s="1" t="s">
@@ -17094,7 +17089,7 @@
       <c r="E398" s="1" t="s">
         <v>745</v>
       </c>
-      <c r="F398" s="2" t="s">
+      <c r="F398" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G398" s="1" t="s">
@@ -17129,7 +17124,7 @@
       <c r="E399" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F399" s="2" t="s">
+      <c r="F399" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G399" s="1" t="s">
@@ -17164,7 +17159,7 @@
       <c r="E400" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F400" s="2" t="s">
+      <c r="F400" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G400" s="1" t="s">
@@ -17199,7 +17194,7 @@
       <c r="E401" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F401" s="2" t="s">
+      <c r="F401" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G401" s="1" t="s">
@@ -17234,7 +17229,7 @@
       <c r="E402" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F402" s="2" t="s">
+      <c r="F402" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G402" s="1" t="s">
@@ -17269,7 +17264,7 @@
       <c r="E403" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F403" s="2" t="s">
+      <c r="F403" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G403" s="1" t="s">
@@ -17304,7 +17299,7 @@
       <c r="E404" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="F404" s="2" t="s">
+      <c r="F404" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G404" s="1" t="s">
@@ -17339,7 +17334,7 @@
       <c r="E405" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F405" s="2" t="s">
+      <c r="F405" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G405" s="1" t="s">
@@ -17374,7 +17369,7 @@
       <c r="E406" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F406" s="2" t="s">
+      <c r="F406" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G406" s="1" t="s">
@@ -17409,7 +17404,7 @@
       <c r="E407" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F407" s="2" t="s">
+      <c r="F407" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G407" s="1" t="s">
@@ -17444,7 +17439,7 @@
       <c r="E408" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F408" s="2" t="s">
+      <c r="F408" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G408" s="1" t="s">
@@ -17479,7 +17474,7 @@
       <c r="E409" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F409" s="2" t="s">
+      <c r="F409" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G409" s="1" t="s">
@@ -17514,7 +17509,7 @@
       <c r="E410" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F410" s="2" t="s">
+      <c r="F410" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G410" s="1" t="s">
@@ -17549,7 +17544,7 @@
       <c r="E411" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F411" s="2" t="s">
+      <c r="F411" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G411" s="1" t="s">
@@ -17584,7 +17579,7 @@
       <c r="E412" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F412" s="2" t="s">
+      <c r="F412" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G412" s="1" t="s">
@@ -17619,7 +17614,7 @@
       <c r="E413" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F413" s="2" t="s">
+      <c r="F413" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G413" s="1" t="s">
@@ -17654,7 +17649,7 @@
       <c r="E414" s="1" t="s">
         <v>766</v>
       </c>
-      <c r="F414" s="2" t="s">
+      <c r="F414" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G414" s="1" t="s">
@@ -17689,7 +17684,7 @@
       <c r="E415" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F415" s="2" t="s">
+      <c r="F415" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G415" s="1" t="s">
@@ -17724,7 +17719,7 @@
       <c r="E416" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="F416" s="2" t="s">
+      <c r="F416" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G416" s="1" t="s">
@@ -17759,7 +17754,7 @@
       <c r="E417" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F417" s="2" t="s">
+      <c r="F417" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G417" s="1" t="s">
@@ -17794,7 +17789,7 @@
       <c r="E418" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F418" s="2" t="s">
+      <c r="F418" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G418" s="1" t="s">
@@ -17829,7 +17824,7 @@
       <c r="E419" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F419" s="2" t="s">
+      <c r="F419" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G419" s="1" t="s">
@@ -17864,7 +17859,7 @@
       <c r="E420" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F420" s="2" t="s">
+      <c r="F420" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G420" s="1" t="s">
@@ -17899,7 +17894,7 @@
       <c r="E421" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F421" s="2" t="s">
+      <c r="F421" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G421" s="1" t="s">
@@ -17934,7 +17929,7 @@
       <c r="E422" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F422" s="2" t="s">
+      <c r="F422" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G422" s="1" t="s">
@@ -17969,7 +17964,7 @@
       <c r="E423" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F423" s="2" t="s">
+      <c r="F423" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G423" s="1" t="s">
@@ -18004,7 +17999,7 @@
       <c r="E424" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F424" s="2" t="s">
+      <c r="F424" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G424" s="1" t="s">
@@ -18039,7 +18034,7 @@
       <c r="E425" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F425" s="2" t="s">
+      <c r="F425" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G425" s="1" t="s">
@@ -18074,7 +18069,7 @@
       <c r="E426" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F426" s="2" t="s">
+      <c r="F426" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G426" s="1" t="s">
@@ -18109,7 +18104,7 @@
       <c r="E427" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F427" s="2" t="s">
+      <c r="F427" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G427" s="1" t="s">
@@ -18144,7 +18139,7 @@
       <c r="E428" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F428" s="2" t="s">
+      <c r="F428" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G428" s="1" t="s">
@@ -18179,7 +18174,7 @@
       <c r="E429" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F429" s="2" t="s">
+      <c r="F429" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G429" s="1" t="s">
@@ -18214,7 +18209,7 @@
       <c r="E430" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F430" s="2" t="s">
+      <c r="F430" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G430" s="1" t="s">
@@ -18249,7 +18244,7 @@
       <c r="E431" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F431" s="2" t="s">
+      <c r="F431" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G431" s="1" t="s">
@@ -18284,7 +18279,7 @@
       <c r="E432" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F432" s="2" t="s">
+      <c r="F432" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G432" s="1" t="s">
@@ -18319,7 +18314,7 @@
       <c r="E433" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F433" s="2" t="s">
+      <c r="F433" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G433" s="1" t="s">
@@ -18354,7 +18349,7 @@
       <c r="E434" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F434" s="2" t="s">
+      <c r="F434" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G434" s="1" t="s">
@@ -18389,7 +18384,7 @@
       <c r="E435" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F435" s="2" t="s">
+      <c r="F435" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G435" s="1" t="s">
@@ -18424,7 +18419,7 @@
       <c r="E436" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F436" s="2" t="s">
+      <c r="F436" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G436" s="1" t="s">
@@ -18459,7 +18454,7 @@
       <c r="E437" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F437" s="2" t="s">
+      <c r="F437" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G437" s="1" t="s">
@@ -18494,7 +18489,7 @@
       <c r="E438" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F438" s="2" t="s">
+      <c r="F438" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G438" s="1" t="s">
@@ -18529,7 +18524,7 @@
       <c r="E439" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F439" s="2" t="s">
+      <c r="F439" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G439" s="1" t="s">
@@ -18564,7 +18559,7 @@
       <c r="E440" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F440" s="2" t="s">
+      <c r="F440" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G440" s="1" t="s">
@@ -18599,7 +18594,7 @@
       <c r="E441" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F441" s="2" t="s">
+      <c r="F441" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G441" s="1" t="s">
@@ -18634,7 +18629,7 @@
       <c r="E442" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F442" s="2" t="s">
+      <c r="F442" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G442" s="1" t="s">
@@ -18669,7 +18664,7 @@
       <c r="E443" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F443" s="2" t="s">
+      <c r="F443" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G443" s="1" t="s">
@@ -18704,7 +18699,7 @@
       <c r="E444" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F444" s="2" t="s">
+      <c r="F444" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G444" s="1" t="s">
@@ -18739,7 +18734,7 @@
       <c r="E445" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F445" s="2" t="s">
+      <c r="F445" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G445" s="1" t="s">
@@ -18774,7 +18769,7 @@
       <c r="E446" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F446" s="2" t="s">
+      <c r="F446" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G446" s="1" t="s">
@@ -18809,7 +18804,7 @@
       <c r="E447" s="1" t="s">
         <v>807</v>
       </c>
-      <c r="F447" s="2" t="s">
+      <c r="F447" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G447" s="1" t="s">
@@ -18844,7 +18839,7 @@
       <c r="E448" s="1" t="s">
         <v>810</v>
       </c>
-      <c r="F448" s="2" t="s">
+      <c r="F448" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G448" s="1" t="s">

</xml_diff>

<commit_message>
adding 98 (71 integration +27 unit) cases to webflux demo
</commit_message>
<xml_diff>
--- a/src/test/resources/auto-test-resources/webflux-demo-integration-resources.xlsx
+++ b/src/test/resources/auto-test-resources/webflux-demo-integration-resources.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5899" uniqueCount="1026">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6609" uniqueCount="1201">
   <si>
     <t>Class</t>
   </si>
@@ -3630,6 +3630,646 @@
   </si>
   <si>
     <t>Exception: JWT signature does not match locally computed signature. JWT validity cannot be asserted and should not be trusted.</t>
+  </si>
+  <si>
+    <t>org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.externalservices.ExternalProductController</t>
+  </si>
+  <si>
+    <t>getProduct
+(Ljava/lang/Integer;)Lreactor/core/publisher/Mono&lt;Lorg/springframework/http/ResponseEntity&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/Product;&gt;;&gt;;</t>
+  </si>
+  <si>
+    <t>[java.lang.Integer : "0"
+]</t>
+  </si>
+  <si>
+    <t>{"headers":{},"body":{"id":0,"category":"Electronics","description":"Sample Product Description","price":100},"status":"OK"}</t>
+  </si>
+  <si>
+    <t>org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.externalservices.ExternalUserController</t>
+  </si>
+  <si>
+    <t>deduct
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/PaymentRequest;)Lreactor/core/publisher/Mono&lt;Lorg/springframework/http/ResponseEntity&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/PaymentResponse;&gt;;&gt;;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.PaymentRequest : {"userId":"0","amount":"0","orderId":"4d965dcf-c070-4b47-9715-9c0305b5ef7c"}
+]</t>
+  </si>
+  <si>
+    <t>{"headers":{},"body":{"userId":0,"name":null,"balance":0,"status":"SUCCESS"},"status":"OK"}</t>
+  </si>
+  <si>
+    <t>refund
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/PaymentRequest;)Lreactor/core/publisher/Mono&lt;Lorg/springframework/http/ResponseEntity&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/PaymentResponse;&gt;;&gt;;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.PaymentRequest : {"userId":"0","amount":"0","orderId":"25ad8373-752c-4a0a-a370-a0c216b25334"}
+]</t>
+  </si>
+  <si>
+    <t>org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.externalservices.InventoryController</t>
+  </si>
+  <si>
+    <t>deduct
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/InventoryRequest;)Lreactor/core/publisher/Mono&lt;Lorg/springframework/http/ResponseEntity&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/InventoryResponse;&gt;;&gt;;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.InventoryRequest : {"orderId":"adbbf726-ce97-44dc-b0b2-42777710e511","productId":"0","quantity":"0"}
+]</t>
+  </si>
+  <si>
+    <t>{"headers":{},"body":{"productId":0,"quantity":0,"remainingQuantity":null,"status":"SUCCESS"},"status":"OK"}</t>
+  </si>
+  <si>
+    <t>restore
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/InventoryRequest;)Lreactor/core/publisher/Mono&lt;Lorg/springframework/http/ResponseEntity&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/InventoryResponse;&gt;;&gt;;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.InventoryRequest : {"orderId":"17cf1d01-b449-4920-820c-6fad1da447e1","productId":"0","quantity":"0"}
+]</t>
+  </si>
+  <si>
+    <t>org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.externalservices.ShippingController</t>
+  </si>
+  <si>
+    <t>schedule
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/ShippingRequest;)Lreactor/core/publisher/Mono&lt;Lorg/springframework/http/ResponseEntity&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/ShippingResponse;&gt;;&gt;;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.ShippingRequest : {"quantity":"0","userId":"0","orderId":"6ffa1179-91f0-4f4e-b80c-b4406baa1e5e"}
+]</t>
+  </si>
+  <si>
+    <t>{"headers":{},"body":{"orderId":"a3a60921-2c2d-4a90-bccb-e33f7f247b68","quantity":0,"status":"SUCCESS","expectedDelivery":"2024-06-27","address":{"street":"123 Main St","city":"Anytown","state":"AnyState","zipCode":"12345"}},"status":"OK"}</t>
+  </si>
+  <si>
+    <t>cancel
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/ShippingRequest;)Lreactor/core/publisher/Mono&lt;Lorg/springframework/http/ResponseEntity&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/ShippingResponse;&gt;;&gt;;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.ShippingRequest : {"quantity":"0","userId":"0","orderId":"7d24c934-a54c-47af-b227-04684beae2b8"}
+]</t>
+  </si>
+  <si>
+    <t>{"headers":{},"body":{"orderId":"7d24c934-a54c-47af-b227-04684beae2b8","quantity":0,"status":"SUCCESS","expectedDelivery":null,"address":{"street":"123 Main St","city":"Anytown","state":"AnyState","zipCode":"12345"}},"status":"OK"}</t>
+  </si>
+  <si>
+    <t>org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.client.InventoryClient</t>
+  </si>
+  <si>
+    <t>deduct
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/InventoryRequest;)Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/InventoryResponse;&gt;;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.InventoryRequest : {"orderId":"39f1f9a2-0134-4083-95fd-616e2ba5fffa","productId":"0","quantity":"0"}
+]</t>
+  </si>
+  <si>
+    <t>{"productId":0,"quantity":0,"remainingQuantity":null,"status":"SUCCESS"}</t>
+  </si>
+  <si>
+    <t>restore
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/InventoryRequest;)Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/InventoryResponse;&gt;;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.InventoryRequest : {"orderId":"443a5065-d024-401b-a6f8-03260db6d993","productId":"0","quantity":"0"}
+]</t>
+  </si>
+  <si>
+    <t>callInventoryService
+(Ljava/lang/String;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/InventoryRequest;)Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/InventoryResponse;&gt;;</t>
+  </si>
+  <si>
+    <t>[java.lang.String : "string"
+, org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.InventoryRequest : {"orderId":"db6a3cd4-bc55-455c-8c5d-1ccd6261270d","productId":"0","quantity":"0"}
+]</t>
+  </si>
+  <si>
+    <t>{"productId":0,"quantity":0,"remainingQuantity":null,"status":"FAILED"}</t>
+  </si>
+  <si>
+    <t>buildErrorResponse
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/InventoryRequest;)Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/InventoryResponse;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.InventoryRequest : {"orderId":"336eea77-ca55-4217-9440-5e5a0cae42ef","productId":"0","quantity":"0"}
+]</t>
+  </si>
+  <si>
+    <t>org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.client.ProductClient</t>
+  </si>
+  <si>
+    <t>getProduct
+(Ljava/lang/Integer;)Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/Product;&gt;;</t>
+  </si>
+  <si>
+    <t>{"id":0,"category":"Electronics","description":"Sample Product Description","price":100}</t>
+  </si>
+  <si>
+    <t>org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.client.ShippingClient</t>
+  </si>
+  <si>
+    <t>schedule
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/ShippingRequest;)Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/ShippingResponse;&gt;;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.ShippingRequest : {"quantity":"0","userId":"0","orderId":"4c09c5dc-53cc-460d-a10c-3a33f588afc2"}
+]</t>
+  </si>
+  <si>
+    <t>{"orderId":"ae0a9cae-fed1-4dba-9ffd-a6698fece357","quantity":0,"status":"SUCCESS","expectedDelivery":"2024-06-27","address":{"street":"123 Main St","city":"Anytown","state":"AnyState","zipCode":"12345"}}</t>
+  </si>
+  <si>
+    <t>cancel
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/ShippingRequest;)Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/ShippingResponse;&gt;;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.ShippingRequest : {"quantity":"0","userId":"0","orderId":"f5381662-a428-4315-a5e0-d3371d8772e0"}
+]</t>
+  </si>
+  <si>
+    <t>{"orderId":"f5381662-a428-4315-a5e0-d3371d8772e0","quantity":0,"status":"SUCCESS","expectedDelivery":null,"address":{"street":"123 Main St","city":"Anytown","state":"AnyState","zipCode":"12345"}}</t>
+  </si>
+  <si>
+    <t>buildErrorResponse
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/ShippingRequest;)Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/ShippingResponse;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.ShippingRequest : {"quantity":"0","userId":"0","orderId":"e24c2ad4-ee62-426f-b5dd-965edcc8a811"}
+]</t>
+  </si>
+  <si>
+    <t>{"orderId":"e24c2ad4-ee62-426f-b5dd-965edcc8a811","quantity":0,"status":"FAILED","expectedDelivery":null,"address":null}</t>
+  </si>
+  <si>
+    <t>org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.client.UserClient</t>
+  </si>
+  <si>
+    <t>deduct
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/PaymentRequest;)Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/PaymentResponse;&gt;;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.PaymentRequest : {"userId":"0","amount":"0","orderId":"da199a9b-d00b-43e2-8b1b-1b309fdd4288"}
+]</t>
+  </si>
+  <si>
+    <t>{"userId":0,"name":null,"balance":0,"status":"SUCCESS"}</t>
+  </si>
+  <si>
+    <t>refund
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/PaymentRequest;)Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/PaymentResponse;&gt;;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.PaymentRequest : {"userId":"0","amount":"0","orderId":"19f21046-527f-437c-83fb-ccb0ed848963"}
+]</t>
+  </si>
+  <si>
+    <t>callUserService
+(Ljava/lang/String;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/PaymentRequest;)Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/PaymentResponse;&gt;;</t>
+  </si>
+  <si>
+    <t>[java.lang.String : "string"
+, org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.PaymentRequest : {"userId":"0","amount":"0","orderId":"feab609f-8f87-4ac6-b18a-388f13e19dff"}
+]</t>
+  </si>
+  <si>
+    <t>{"userId":0,"name":null,"balance":0,"status":"FAILED"}</t>
+  </si>
+  <si>
+    <t>buildErrorResponse
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/PaymentRequest;)Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/PaymentResponse;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.PaymentRequest : {"userId":"0","amount":"0","orderId":"b44554b5-0797-4740-90b2-a4735d7c32fc"}
+]</t>
+  </si>
+  <si>
+    <t>org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.controller.OrderController</t>
+  </si>
+  <si>
+    <t>placeOrder
+(Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/OrderRequest;&gt;;)Lreactor/core/publisher/Mono&lt;Lorg/springframework/http/ResponseEntity&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/OrderResponse;&gt;;&gt;;</t>
+  </si>
+  <si>
+    <t>[reactor.core.publisher.Mono : {"userId":"0","productId":"0","quantity":"0"}
+]</t>
+  </si>
+  <si>
+    <t>{"cause":null,"stackTrace":[{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onNext","fileName":"FluxMapFuseable.java","lineNumber":283,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"Operators.java","lineNumber":2571,"className":"reactor.core.publisher.Operators$ScalarSubscription","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxMapFuseable.java","lineNumber":360,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":144,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoFlatMap.java","lineNumber":194,"className":"reactor.core.publisher.MonoFlatMap$FlatMapMain","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":144,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoFlatMap.java","lineNumber":194,"className":"reactor.core.publisher.MonoFlatMap$FlatMapMain","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxMapFuseable.java","lineNumber":360,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxMapFuseable.java","lineNumber":360,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":144,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxDefaultIfEmpty.java","lineNumber":98,"className":"reactor.core.publisher.FluxDefaultIfEmpty$DefaultIfEmptySubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxContextWrite.java","lineNumber":136,"className":"reactor.core.publisher.FluxContextWrite$ContextWriteSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxDoFinally.java","lineNumber":140,"className":"reactor.core.publisher.FluxDoFinally$DoFinallySubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"LambdaMonoSubscriber.java","lineNumber":121,"className":"reactor.core.publisher.LambdaMonoSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxDoFinally.java","lineNumber":107,"className":"reactor.core.publisher.FluxDoFinally$DoFinallySubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxContextWrite.java","lineNumber":101,"className":"reactor.core.publisher.FluxContextWrite$ContextWriteSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"Operators.java","lineNumber":2051,"className":"reactor.core.publisher.Operators$BaseFluxToMonoOperator","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":178,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxMapFuseable.java","lineNumber":265,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxMapFuseable.java","lineNumber":265,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoFlatMap.java","lineNumber":117,"className":"reactor.core.publisher.MonoFlatMap$FlatMapMain","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":178,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoFlatMap.java","lineNumber":117,"className":"reactor.core.publisher.MonoFlatMap$FlatMapMain","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":178,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxMapFuseable.java","lineNumber":265,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"MonoJust.java","lineNumber":55,"className":"reactor.core.publisher.MonoJust","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"InternalMonoOperator.java","lineNumber":76,"className":"reactor.core.publisher.InternalMonoOperator","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"MonoDefer.java","lineNumber":53,"className":"reactor.core.publisher.MonoDefer","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"Mono.java","lineNumber":4512,"className":"reactor.core.publisher.Mono","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribeWith","fileName":"Mono.java","lineNumber":4578,"className":"reactor.core.publisher.Mono","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"Mono.java","lineNumber":4339,"className":"reactor.core.publisher.Mono","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"executeCommandRaw","fileName":"AgentCommandExecutorImpl.java","lineNumber":379,"className":"io.unlogged.AgentCommandExecutorImpl","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"executeCommand","fileName":"AgentCommandExecutorImpl.java","lineNumber":477,"className":"io.unlogged.AgentCommandExecutorImpl","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"serve","fileName":"AgentCommandServer.java","lineNumber":74,"className":"io.unlogged.command.AgentCommandServer","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"execute","fileName":"NanoHTTPD.java","lineNumber":945,"className":"fi.iki.elonen.NanoHTTPD$HTTPSession","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"run","fileName":"NanoHTTPD.java","lineNumber":192,"className":"fi.iki.elonen.NanoHTTPD$ClientHandler","nativeMethod":false},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"21.0.1","methodName":"run","fileName":"Thread.java","lineNumber":1583,"className":"java.lang.Thread","nativeMethod":false}],"message":"class reactor.core.publisher.Mono$Unlogged$jmm7vgjr cannot be cast to class org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.OrderRequest (reactor.core.publisher.Mono$Unlogged$jmm7vgjr and org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.OrderRequest are in unnamed module of loader 'app')","suppressed":[],"localizedMessage":"class reactor.core.publisher.Mono$Unlogged$jmm7vgjr cannot be cast to class org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.OrderRequest (reactor.core.publisher.Mono$Unlogged$jmm7vgjr and org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.OrderRequest are in unnamed module of loader 'app')"}</t>
+  </si>
+  <si>
+    <t>{"cause":null,"stackTrace":[{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onNext","fileName":"FluxMapFuseable.java","lineNumber":283,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"Operators.java","lineNumber":2571,"className":"reactor.core.publisher.Operators$ScalarSubscription","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxMapFuseable.java","lineNumber":360,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":144,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoFlatMap.java","lineNumber":194,"className":"reactor.core.publisher.MonoFlatMap$FlatMapMain","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":144,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoFlatMap.java","lineNumber":194,"className":"reactor.core.publisher.MonoFlatMap$FlatMapMain","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxMapFuseable.java","lineNumber":360,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxMapFuseable.java","lineNumber":360,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":144,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxDefaultIfEmpty.java","lineNumber":98,"className":"reactor.core.publisher.FluxDefaultIfEmpty$DefaultIfEmptySubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxContextWrite.java","lineNumber":136,"className":"reactor.core.publisher.FluxContextWrite$ContextWriteSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxDoFinally.java","lineNumber":140,"className":"reactor.core.publisher.FluxDoFinally$DoFinallySubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"LambdaMonoSubscriber.java","lineNumber":121,"className":"reactor.core.publisher.LambdaMonoSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxDoFinally.java","lineNumber":107,"className":"reactor.core.publisher.FluxDoFinally$DoFinallySubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxContextWrite.java","lineNumber":101,"className":"reactor.core.publisher.FluxContextWrite$ContextWriteSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"Operators.java","lineNumber":2051,"className":"reactor.core.publisher.Operators$BaseFluxToMonoOperator","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":178,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxMapFuseable.java","lineNumber":265,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxMapFuseable.java","lineNumber":265,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoFlatMap.java","lineNumber":117,"className":"reactor.core.publisher.MonoFlatMap$FlatMapMain","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":178,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoFlatMap.java","lineNumber":117,"className":"reactor.core.publisher.MonoFlatMap$FlatMapMain","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":178,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxMapFuseable.java","lineNumber":265,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"MonoJust.java","lineNumber":55,"className":"reactor.core.publisher.MonoJust","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"InternalMonoOperator.java","lineNumber":76,"className":"reactor.core.publisher.InternalMonoOperator","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"MonoDefer.java","lineNumber":53,"className":"reactor.core.publisher.MonoDefer","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"Mono.java","lineNumber":4512,"className":"reactor.core.publisher.Mono","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribeWith","fileName":"Mono.java","lineNumber":4578,"className":"reactor.core.publisher.Mono","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"Mono.java","lineNumber":4339,"className":"reactor.core.publisher.Mono","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"executeCommandRaw","fileName":"AgentCommandExecutorImpl.java","lineNumber":379,"className":"io.unlogged.AgentCommandExecutorImpl","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"executeCommand","fileName":"AgentCommandExecutorImpl.java","lineNumber":477,"className":"io.unlogged.AgentCommandExecutorImpl","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"serve","fileName":"AgentCommandServer.java","lineNumber":74,"className":"io.unlogged.command.AgentCommandServer","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"execute","fileName":"NanoHTTPD.java","lineNumber":945,"className":"fi.iki.elonen.NanoHTTPD$HTTPSession","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"run","fileName":"NanoHTTPD.java","lineNumber":192,"className":"fi.iki.elonen.NanoHTTPD$ClientHandler","nativeMethod":false},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"21.0.1","methodName":"run","fileName":"Thread.java","lineNumber":1583,"className":"java.lang.Thread","nativeMethod":false}],"message":"class reactor.core.publisher.Mono$Unlogged$9CUP1JUO cannot be cast to class org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.OrderRequest (reactor.core.publisher.Mono$Unlogged$9CUP1JUO and org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.OrderRequest are in unnamed module of loader 'app')","suppressed":[],"localizedMessage":"class reactor.core.publisher.Mono$Unlogged$9CUP1JUO cannot be cast to class org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.OrderRequest (reactor.core.publisher.Mono$Unlogged$9CUP1JUO and org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.OrderRequest are in unnamed module of loader 'app')"}</t>
+  </si>
+  <si>
+    <t>org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.service.InventoryOrchestrator</t>
+  </si>
+  <si>
+    <t>create
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/OrchestrationRequestContext;)Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/OrchestrationRequestContext;&gt;;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.OrchestrationRequestContext : {"orderId":"0e9bcb81-863a-499b-91fb-257ea1a152ea","orderRequest":{"userId":"0","productId":"0","quantity":"0"},"productPrice":"0","paymentRequest":{"userId":"0","amount":"0","orderId":"67570acf-d54f-41d0-baf8-da85fb816776"},"paymentResponse":{"userId":"0","name":"string","balance":"0","status":"SUCCESS"},"inventoryRequest":{"orderId":"da5e7dd0-8868-4273-9524-2c314b5b0764","productId":"0","quantity":"0"},"inventoryResponse":{"productId":"0","quantity":"0","remainingQuantity":"0","status":"SUCCESS"},"shippingRequest":{"quantity":"0","userId":"0","orderId":"a2e3a571-6e1f-4b72-b624-7f6690afe6d3"},"shippingResponse":{"orderId":"8fbcbb94-b206-490b-a5c7-8dec36c7394a","quantity":"0","status":"SUCCESS","expectedDelivery":"string","address":{"street":"string","city":"string","state":"string","zipCode":"string"}},"status":"SUCCESS"}
+]</t>
+  </si>
+  <si>
+    <t>{"orderId":"0e9bcb81-863a-499b-91fb-257ea1a152ea","orderRequest":{"userId":0,"productId":0,"quantity":0},"productPrice":0,"paymentRequest":{"userId":0,"amount":0,"orderId":"67570acf-d54f-41d0-baf8-da85fb816776"},"paymentResponse":{"userId":0,"name":"string","balance":0,"status":"SUCCESS"},"inventoryRequest":{"orderId":"da5e7dd0-8868-4273-9524-2c314b5b0764","productId":0,"quantity":0},"inventoryResponse":{"productId":0,"quantity":0,"remainingQuantity":null,"status":"SUCCESS"},"shippingRequest":{"quantity":0,"userId":0,"orderId":"a2e3a571-6e1f-4b72-b624-7f6690afe6d3"},"shippingResponse":{"orderId":"8fbcbb94-b206-490b-a5c7-8dec36c7394a","quantity":0,"status":"SUCCESS","expectedDelivery":"string","address":{"street":"string","city":"string","state":"string","zipCode":"string"}},"status":"SUCCESS"}</t>
+  </si>
+  <si>
+    <t>isSuccess
+()Ljava/util/function/Predicate&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/OrchestrationRequestContext;&gt;;</t>
+  </si>
+  <si>
+    <t>{"className": "null"}</t>
+  </si>
+  <si>
+    <t>cancel
+()Ljava/util/function/Consumer&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/OrchestrationRequestContext;&gt;;</t>
+  </si>
+  <si>
+    <t>org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.service.OrchestratorService</t>
+  </si>
+  <si>
+    <t>placeOrder
+(Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/OrderRequest;&gt;;)Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/OrderResponse;&gt;;</t>
+  </si>
+  <si>
+    <t>{"cause":null,"stackTrace":[{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onNext","fileName":"FluxMapFuseable.java","lineNumber":283,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"Operators.java","lineNumber":2571,"className":"reactor.core.publisher.Operators$ScalarSubscription","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxMapFuseable.java","lineNumber":360,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":144,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoFlatMap.java","lineNumber":194,"className":"reactor.core.publisher.MonoFlatMap$FlatMapMain","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":144,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoFlatMap.java","lineNumber":194,"className":"reactor.core.publisher.MonoFlatMap$FlatMapMain","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxMapFuseable.java","lineNumber":360,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxContextWrite.java","lineNumber":136,"className":"reactor.core.publisher.FluxContextWrite$ContextWriteSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxDoFinally.java","lineNumber":140,"className":"reactor.core.publisher.FluxDoFinally$DoFinallySubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"LambdaMonoSubscriber.java","lineNumber":121,"className":"reactor.core.publisher.LambdaMonoSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxDoFinally.java","lineNumber":107,"className":"reactor.core.publisher.FluxDoFinally$DoFinallySubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxContextWrite.java","lineNumber":101,"className":"reactor.core.publisher.FluxContextWrite$ContextWriteSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxMapFuseable.java","lineNumber":265,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoFlatMap.java","lineNumber":117,"className":"reactor.core.publisher.MonoFlatMap$FlatMapMain","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":178,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoFlatMap.java","lineNumber":117,"className":"reactor.core.publisher.MonoFlatMap$FlatMapMain","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":178,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxMapFuseable.java","lineNumber":265,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"MonoJust.java","lineNumber":55,"className":"reactor.core.publisher.MonoJust","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"InternalMonoOperator.java","lineNumber":76,"className":"reactor.core.publisher.InternalMonoOperator","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"MonoDefer.java","lineNumber":53,"className":"reactor.core.publisher.MonoDefer","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"Mono.java","lineNumber":4512,"className":"reactor.core.publisher.Mono","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribeWith","fileName":"Mono.java","lineNumber":4578,"className":"reactor.core.publisher.Mono","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"Mono.java","lineNumber":4339,"className":"reactor.core.publisher.Mono","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"executeCommandRaw","fileName":"AgentCommandExecutorImpl.java","lineNumber":379,"className":"io.unlogged.AgentCommandExecutorImpl","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"executeCommand","fileName":"AgentCommandExecutorImpl.java","lineNumber":477,"className":"io.unlogged.AgentCommandExecutorImpl","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"serve","fileName":"AgentCommandServer.java","lineNumber":74,"className":"io.unlogged.command.AgentCommandServer","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"execute","fileName":"NanoHTTPD.java","lineNumber":945,"className":"fi.iki.elonen.NanoHTTPD$HTTPSession","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"run","fileName":"NanoHTTPD.java","lineNumber":192,"className":"fi.iki.elonen.NanoHTTPD$ClientHandler","nativeMethod":false},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"21.0.1","methodName":"run","fileName":"Thread.java","lineNumber":1583,"className":"java.lang.Thread","nativeMethod":false}],"message":"class reactor.core.publisher.Mono$Unlogged$FYNA5b9E cannot be cast to class org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.OrderRequest (reactor.core.publisher.Mono$Unlogged$FYNA5b9E and org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.OrderRequest are in unnamed module of loader 'app')","suppressed":[],"localizedMessage":"class reactor.core.publisher.Mono$Unlogged$FYNA5b9E cannot be cast to class org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.OrderRequest (reactor.core.publisher.Mono$Unlogged$FYNA5b9E and org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.OrderRequest are in unnamed module of loader 'app')"}</t>
+  </si>
+  <si>
+    <t>getProduct
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/OrchestrationRequestContext;)Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/OrchestrationRequestContext;&gt;;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.OrchestrationRequestContext : {"orderId":"9aca22d2-00af-4fd4-948c-331b6be4e433","orderRequest":{"userId":"0","productId":"0","quantity":"0"},"productPrice":"0","paymentRequest":{"userId":"0","amount":"0","orderId":"f06db9b8-e828-4989-9d93-a38a84b992f5"},"paymentResponse":{"userId":"0","name":"string","balance":"0","status":"SUCCESS"},"inventoryRequest":{"orderId":"0f88b3ef-79b3-4fb3-9a97-b57bf63830a4","productId":"0","quantity":"0"},"inventoryResponse":{"productId":"0","quantity":"0","remainingQuantity":"0","status":"SUCCESS"},"shippingRequest":{"quantity":"0","userId":"0","orderId":"a79c8238-46ef-4719-bcaf-f81c9042943c"},"shippingResponse":{"orderId":"d7aa19d9-8519-45cf-9742-efcbec90e416","quantity":"0","status":"SUCCESS","expectedDelivery":"string","address":{"street":"string","city":"string","state":"string","zipCode":"string"}},"status":"SUCCESS"}
+]</t>
+  </si>
+  <si>
+    <t>{"orderId":"9aca22d2-00af-4fd4-948c-331b6be4e433","orderRequest":{"userId":0,"productId":0,"quantity":0},"productPrice":100,"paymentRequest":{"userId":0,"amount":0,"orderId":"f06db9b8-e828-4989-9d93-a38a84b992f5"},"paymentResponse":{"userId":0,"name":"string","balance":0,"status":"SUCCESS"},"inventoryRequest":{"orderId":"0f88b3ef-79b3-4fb3-9a97-b57bf63830a4","productId":0,"quantity":0},"inventoryResponse":{"productId":0,"quantity":0,"remainingQuantity":0,"status":"SUCCESS"},"shippingRequest":{"quantity":0,"userId":0,"orderId":"a79c8238-46ef-4719-bcaf-f81c9042943c"},"shippingResponse":{"orderId":"d7aa19d9-8519-45cf-9742-efcbec90e416","quantity":0,"status":"SUCCESS","expectedDelivery":"string","address":{"street":"string","city":"string","state":"string","zipCode":"string"}},"status":"SUCCESS"}</t>
+  </si>
+  <si>
+    <t>doOrderPostProcessing
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/OrchestrationRequestContext;)V</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.OrchestrationRequestContext : {"orderId":"adb89627-0556-48d4-af9e-ca184e31d308","orderRequest":{"userId":"0","productId":"0","quantity":"0"},"productPrice":"0","paymentRequest":{"userId":"0","amount":"0","orderId":"d35365dd-e399-4d1a-9096-9213b1599e7a"},"paymentResponse":{"userId":"0","name":"string","balance":"0","status":"SUCCESS"},"inventoryRequest":{"orderId":"f68ae484-bfdf-42d9-9548-969a4ca49c30","productId":"0","quantity":"0"},"inventoryResponse":{"productId":"0","quantity":"0","remainingQuantity":"0","status":"SUCCESS"},"shippingRequest":{"quantity":"0","userId":"0","orderId":"09c2a4ac-8ea2-4e87-bafd-7f6d38ca14ca"},"shippingResponse":{"orderId":"56aa245d-3a8d-4422-b18c-835e664f8213","quantity":"0","status":"SUCCESS","expectedDelivery":"string","address":{"street":"string","city":"string","state":"string","zipCode":"string"}},"status":"SUCCESS"}
+]</t>
+  </si>
+  <si>
+    <t>toOrderResponse
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/OrchestrationRequestContext;)Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/OrderResponse;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.OrchestrationRequestContext : {"orderId":"5266af89-4fcb-4dde-b714-65e31d3e9284","orderRequest":{"userId":"0","productId":"0","quantity":"0"},"productPrice":"0","paymentRequest":{"userId":"0","amount":"0","orderId":"76a73a66-f4ec-4d04-a559-454c64a7ce30"},"paymentResponse":{"userId":"0","name":"string","balance":"0","status":"SUCCESS"},"inventoryRequest":{"orderId":"e67071d3-51c6-4d9b-84a1-2e16dd7d2d8e","productId":"0","quantity":"0"},"inventoryResponse":{"productId":"0","quantity":"0","remainingQuantity":"0","status":"SUCCESS"},"shippingRequest":{"quantity":"0","userId":"0","orderId":"185d755e-f913-46bc-83e3-453e85cd168b"},"shippingResponse":{"orderId":"a2309e1f-f6db-45a9-82f7-1509c6fe693a","quantity":"0","status":"SUCCESS","expectedDelivery":"string","address":{"street":"string","city":"string","state":"string","zipCode":"string"}},"status":"SUCCESS"}
+]</t>
+  </si>
+  <si>
+    <t>{"userId":0,"productId":0,"orderId":"5266af89-4fcb-4dde-b714-65e31d3e9284","status":"SUCCESS","shippingAddress":{"street":"string","city":"string","state":"string","zipCode":"string"},"expectedDelivery":"string"}</t>
+  </si>
+  <si>
+    <t>org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.service.OrderCancellationService</t>
+  </si>
+  <si>
+    <t>cancelOrder
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/OrchestrationRequestContext;)V</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.OrchestrationRequestContext : {"orderId":"3379437e-d927-4104-8da6-a1e8aab10950","orderRequest":{"userId":"0","productId":"0","quantity":"0"},"productPrice":"0","paymentRequest":{"userId":"0","amount":"0","orderId":"9b53bfc2-1152-4342-afc8-89c7c162ebb9"},"paymentResponse":{"userId":"0","name":"string","balance":"0","status":"SUCCESS"},"inventoryRequest":{"orderId":"74e296dc-99d2-4112-ac00-9b9d29803daf","productId":"0","quantity":"0"},"inventoryResponse":{"productId":"0","quantity":"0","remainingQuantity":"0","status":"SUCCESS"},"shippingRequest":{"quantity":"0","userId":"0","orderId":"a5f177a4-9d9a-4e85-9b00-5e679e1ba58a"},"shippingResponse":{"orderId":"d41bf603-632b-4f2c-8f03-d5da18a3669b","quantity":"0","status":"SUCCESS","expectedDelivery":"string","address":{"street":"string","city":"string","state":"string","zipCode":"string"}},"status":"SUCCESS"}
+]</t>
+  </si>
+  <si>
+    <t>org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.service.OrderFulfillmentService</t>
+  </si>
+  <si>
+    <t>placeOrder
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/OrchestrationRequestContext;)Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/OrchestrationRequestContext;&gt;;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.OrchestrationRequestContext : {"orderId":"3816612c-dc4c-4cd3-bf1e-424a22b21ec8","orderRequest":{"userId":"0","productId":"0","quantity":"0"},"productPrice":"0","paymentRequest":{"userId":"0","amount":"0","orderId":"cf8f1ed8-0def-4037-845d-9ecc38652976"},"paymentResponse":{"userId":"0","name":"string","balance":"0","status":"SUCCESS"},"inventoryRequest":{"orderId":"8f296eb8-5e01-4226-be62-851098ebbe7b","productId":"0","quantity":"0"},"inventoryResponse":{"productId":"0","quantity":"0","remainingQuantity":"0","status":"SUCCESS"},"shippingRequest":{"quantity":"0","userId":"0","orderId":"da6aaa4c-dac5-4fd4-b7fd-17b064e2a441"},"shippingResponse":{"orderId":"14260a3a-1390-40e9-aadb-6691b0df25cf","quantity":"0","status":"SUCCESS","expectedDelivery":"string","address":{"street":"string","city":"string","state":"string","zipCode":"string"}},"status":"SUCCESS"}
+]</t>
+  </si>
+  <si>
+    <t>{"orderId":"3816612c-dc4c-4cd3-bf1e-424a22b21ec8","orderRequest":{"userId":0,"productId":0,"quantity":0},"productPrice":0,"paymentRequest":{"userId":0,"amount":0,"orderId":"cf8f1ed8-0def-4037-845d-9ecc38652976"},"paymentResponse":{"userId":0,"name":null,"balance":0,"status":"SUCCESS"},"inventoryRequest":{"orderId":"8f296eb8-5e01-4226-be62-851098ebbe7b","productId":0,"quantity":0},"inventoryResponse":{"productId":0,"quantity":0,"remainingQuantity":null,"status":"SUCCESS"},"shippingRequest":{"quantity":0,"userId":0,"orderId":"da6aaa4c-dac5-4fd4-b7fd-17b064e2a441"},"shippingResponse":{"orderId":"17a37a02-061d-4b49-9e25-283a454d2fc6","quantity":0,"status":"SUCCESS","expectedDelivery":"2024-06-27","address":{"street":"123 Main St","city":"Anytown","state":"AnyState","zipCode":"12345"}},"status":"SUCCESS"}</t>
+  </si>
+  <si>
+    <t>updateStatus
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorparallel/sec03/dto/OrchestrationRequestContext;)V</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.OrchestrationRequestContext : {"orderId":"26e4c3ea-f3ef-4bc8-9f58-6e81168bcc32","orderRequest":{"userId":"0","productId":"0","quantity":"0"},"productPrice":"0","paymentRequest":{"userId":"0","amount":"0","orderId":"5db1b205-69ff-42b2-bc21-f0fe8d2c855e"},"paymentResponse":{"userId":"0","name":"string","balance":"0","status":"SUCCESS"},"inventoryRequest":{"orderId":"3ef11df8-010d-4819-8930-fa52f32268c7","productId":"0","quantity":"0"},"inventoryResponse":{"productId":"0","quantity":"0","remainingQuantity":"0","status":"SUCCESS"},"shippingRequest":{"quantity":"0","userId":"0","orderId":"f3a579c3-5079-44b4-a620-680350dda177"},"shippingResponse":{"orderId":"31cf4e20-3d71-4f5d-a2ad-8da824bb6a36","quantity":"0","status":"SUCCESS","expectedDelivery":"string","address":{"street":"string","city":"string","state":"string","zipCode":"string"}},"status":"SUCCESS"}
+]</t>
+  </si>
+  <si>
+    <t>org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.service.PaymentOrchestrator</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.OrchestrationRequestContext : {"orderId":"96e17006-562f-451e-b2e4-de9542fa87d0","orderRequest":{"userId":"0","productId":"0","quantity":"0"},"productPrice":"0","paymentRequest":{"userId":"0","amount":"0","orderId":"bb9a373b-340e-430d-aaa9-1d1d6c6ee567"},"paymentResponse":{"userId":"0","name":"string","balance":"0","status":"SUCCESS"},"inventoryRequest":{"orderId":"e1e3348f-8bf3-42ec-8d19-401c91e5ade8","productId":"0","quantity":"0"},"inventoryResponse":{"productId":"0","quantity":"0","remainingQuantity":"0","status":"SUCCESS"},"shippingRequest":{"quantity":"0","userId":"0","orderId":"691be5c8-61cf-4eec-af51-3b42840d1e3d"},"shippingResponse":{"orderId":"5b3dea2f-f8bf-49ca-864c-c9d6c7be9820","quantity":"0","status":"SUCCESS","expectedDelivery":"string","address":{"street":"string","city":"string","state":"string","zipCode":"string"}},"status":"SUCCESS"}
+]</t>
+  </si>
+  <si>
+    <t>{"orderId":"96e17006-562f-451e-b2e4-de9542fa87d0","orderRequest":{"userId":0,"productId":0,"quantity":0},"productPrice":0,"paymentRequest":{"userId":0,"amount":0,"orderId":"bb9a373b-340e-430d-aaa9-1d1d6c6ee567"},"paymentResponse":{"userId":0,"name":null,"balance":0,"status":"SUCCESS"},"inventoryRequest":{"orderId":"e1e3348f-8bf3-42ec-8d19-401c91e5ade8","productId":0,"quantity":0},"inventoryResponse":{"productId":0,"quantity":0,"remainingQuantity":0,"status":"SUCCESS"},"shippingRequest":{"quantity":0,"userId":0,"orderId":"691be5c8-61cf-4eec-af51-3b42840d1e3d"},"shippingResponse":{"orderId":"5b3dea2f-f8bf-49ca-864c-c9d6c7be9820","quantity":0,"status":"SUCCESS","expectedDelivery":"string","address":{"street":"string","city":"string","state":"string","zipCode":"string"}},"status":"SUCCESS"}</t>
+  </si>
+  <si>
+    <t>org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.service.ShippingOrchestrator</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorparallel.sec03.dto.OrchestrationRequestContext : {"orderId":"c3c6fb53-38f3-416e-ac92-e0b85ed51895","orderRequest":{"userId":"0","productId":"0","quantity":"0"},"productPrice":"0","paymentRequest":{"userId":"0","amount":"0","orderId":"1fe763a3-9df4-4035-90da-6b9afd7a2373"},"paymentResponse":{"userId":"0","name":"string","balance":"0","status":"SUCCESS"},"inventoryRequest":{"orderId":"607abe51-e2b1-4171-8b1b-05261f1fe36b","productId":"0","quantity":"0"},"inventoryResponse":{"productId":"0","quantity":"0","remainingQuantity":"0","status":"SUCCESS"},"shippingRequest":{"quantity":"0","userId":"0","orderId":"d12cea1b-eea7-400f-88bb-5b213cbeb9bc"},"shippingResponse":{"orderId":"54a788a9-b789-4e25-af1f-62aee0c9101d","quantity":"0","status":"SUCCESS","expectedDelivery":"string","address":{"street":"string","city":"string","state":"string","zipCode":"string"}},"status":"SUCCESS"}
+]</t>
+  </si>
+  <si>
+    <t>{"orderId":"c3c6fb53-38f3-416e-ac92-e0b85ed51895","orderRequest":{"userId":0,"productId":0,"quantity":0},"productPrice":0,"paymentRequest":{"userId":0,"amount":0,"orderId":"1fe763a3-9df4-4035-90da-6b9afd7a2373"},"paymentResponse":{"userId":0,"name":"string","balance":0,"status":"SUCCESS"},"inventoryRequest":{"orderId":"607abe51-e2b1-4171-8b1b-05261f1fe36b","productId":0,"quantity":0},"inventoryResponse":{"productId":0,"quantity":0,"remainingQuantity":0,"status":"SUCCESS"},"shippingRequest":{"quantity":0,"userId":0,"orderId":"d12cea1b-eea7-400f-88bb-5b213cbeb9bc"},"shippingResponse":{"orderId":"8f421737-1b3c-40bc-a425-c76c1f9aeb3c","quantity":0,"status":"SUCCESS","expectedDelivery":"2024-06-27","address":{"street":"123 Main St","city":"Anytown","state":"AnyState","zipCode":"12345"}},"status":"SUCCESS"}</t>
+  </si>
+  <si>
+    <t>org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.client.InventoryClient</t>
+  </si>
+  <si>
+    <t>deduct
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/InventoryRequest;)Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/InventoryResponse;&gt;;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.dto.InventoryRequest : {"paymentId":"2c4fa23b-c4f5-4f6e-aa60-67030fe65469","productId":"0","quantity":"0"}
+]</t>
+  </si>
+  <si>
+    <t>{"inventoryId":null,"productId":0,"quantity":0,"remainingQuantity":null,"status":"SUCCESS"}</t>
+  </si>
+  <si>
+    <t>restore
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/InventoryRequest;)Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/InventoryResponse;&gt;;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.dto.InventoryRequest : {"paymentId":"0499db9e-5f5e-4191-b9e0-70dbe86c4541","productId":"0","quantity":"0"}
+]</t>
+  </si>
+  <si>
+    <t>callInventoryService
+(Ljava/lang/String;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/InventoryRequest;)Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/InventoryResponse;&gt;;</t>
+  </si>
+  <si>
+    <t>[java.lang.String : "string"
+, org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.dto.InventoryRequest : {"paymentId":"b8d61275-38f3-4a5a-87bc-2cece3efed89","productId":"0","quantity":"0"}
+]</t>
+  </si>
+  <si>
+    <t>{"inventoryId":null,"productId":0,"quantity":0,"remainingQuantity":null,"status":"FAILED"}</t>
+  </si>
+  <si>
+    <t>buildErrorResponse
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/InventoryRequest;)Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/InventoryResponse;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.dto.InventoryRequest : {"paymentId":"abdf546a-a805-426c-8a9d-4577076558ea","productId":"0","quantity":"0"}
+]</t>
+  </si>
+  <si>
+    <t>org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.client.ProductClient</t>
+  </si>
+  <si>
+    <t>getProduct
+(Ljava/lang/Integer;)Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/Product;&gt;;</t>
+  </si>
+  <si>
+    <t>org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.client.ShippingClient</t>
+  </si>
+  <si>
+    <t>schedule
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/ShippingRequest;)Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/ShippingResponse;&gt;;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.dto.ShippingRequest : {"quantity":"0","userId":"0","inventoryId":"e6d05c34-3371-47c6-a23e-a2c63acc3b84"}
+]</t>
+  </si>
+  <si>
+    <t>{"shippingId":null,"quantity":0,"status":"SUCCESS","expectedDelivery":"2024-06-27","address":{"street":"123 Main St","city":"Anytown","state":"AnyState","zipCode":"12345"}}</t>
+  </si>
+  <si>
+    <t>cancel
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/ShippingRequest;)Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/ShippingResponse;&gt;;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.dto.ShippingRequest : {"quantity":"0","userId":"0","inventoryId":"4d881cdb-fcad-4dbe-820d-c83207decfb9"}
+]</t>
+  </si>
+  <si>
+    <t>{"shippingId":null,"quantity":0,"status":"SUCCESS","expectedDelivery":null,"address":{"street":"123 Main St","city":"Anytown","state":"AnyState","zipCode":"12345"}}</t>
+  </si>
+  <si>
+    <t>callShippingService
+(Ljava/lang/String;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/ShippingRequest;)Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/ShippingResponse;&gt;;</t>
+  </si>
+  <si>
+    <t>[java.lang.String : "string"
+, org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.dto.ShippingRequest : {"quantity":"0","userId":"0","inventoryId":"45bf4e3f-75c8-406b-92ce-dae587b5dec4"}
+]</t>
+  </si>
+  <si>
+    <t>{"shippingId":null,"quantity":0,"status":"FAILED","expectedDelivery":null,"address":null}</t>
+  </si>
+  <si>
+    <t>buildErrorResponse
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/ShippingRequest;)Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/ShippingResponse;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.dto.ShippingRequest : {"quantity":"0","userId":"0","inventoryId":"90527fc0-a09c-48d2-82a7-32915122eca0"}
+]</t>
+  </si>
+  <si>
+    <t>org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.client.UserClient</t>
+  </si>
+  <si>
+    <t>deduct
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/PaymentRequest;)Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/PaymentResponse;&gt;;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.dto.PaymentRequest : {"userId":"0","amount":"0","orderId":"3b590670-f4ca-4bb2-a667-46e98364303e"}
+]</t>
+  </si>
+  <si>
+    <t>{"paymentId":null,"userId":0,"name":null,"balance":0,"status":"SUCCESS"}</t>
+  </si>
+  <si>
+    <t>refund
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/PaymentRequest;)Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/PaymentResponse;&gt;;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.dto.PaymentRequest : {"userId":"0","amount":"0","orderId":"1cd9dd66-7ca4-4306-b759-0cb536172e56"}
+]</t>
+  </si>
+  <si>
+    <t>callUserService
+(Ljava/lang/String;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/PaymentRequest;)Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/PaymentResponse;&gt;;</t>
+  </si>
+  <si>
+    <t>[java.lang.String : "string"
+, org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.dto.PaymentRequest : {"userId":"0","amount":"0","orderId":"afe6cba1-c305-4c46-aca2-45f0926e0eee"}
+]</t>
+  </si>
+  <si>
+    <t>{"paymentId":null,"userId":0,"name":null,"balance":0,"status":"FAILED"}</t>
+  </si>
+  <si>
+    <t>buildErrorResponse
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/PaymentRequest;)Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/PaymentResponse;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.dto.PaymentRequest : {"userId":"0","amount":"0","orderId":"02ae3a97-bbbb-44cb-8876-ed8717fd9b7b"}
+]</t>
+  </si>
+  <si>
+    <t>org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.controller.OrderController</t>
+  </si>
+  <si>
+    <t>placeOrder
+(Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/OrderRequest;&gt;;)Lreactor/core/publisher/Mono&lt;Lorg/springframework/http/ResponseEntity&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/OrderResponse;&gt;;&gt;;</t>
+  </si>
+  <si>
+    <t>{"cause":null,"stackTrace":[{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onNext","fileName":"FluxMapFuseable.java","lineNumber":283,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"Operators.java","lineNumber":2571,"className":"reactor.core.publisher.Operators$ScalarSubscription","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxMapFuseable.java","lineNumber":360,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":144,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoFlatMap.java","lineNumber":194,"className":"reactor.core.publisher.MonoFlatMap$FlatMapMain","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxMapFuseable.java","lineNumber":360,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxMapFuseable.java","lineNumber":360,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":144,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxDefaultIfEmpty.java","lineNumber":98,"className":"reactor.core.publisher.FluxDefaultIfEmpty$DefaultIfEmptySubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxContextWrite.java","lineNumber":136,"className":"reactor.core.publisher.FluxContextWrite$ContextWriteSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxDoFinally.java","lineNumber":140,"className":"reactor.core.publisher.FluxDoFinally$DoFinallySubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"LambdaMonoSubscriber.java","lineNumber":121,"className":"reactor.core.publisher.LambdaMonoSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxDoFinally.java","lineNumber":107,"className":"reactor.core.publisher.FluxDoFinally$DoFinallySubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxContextWrite.java","lineNumber":101,"className":"reactor.core.publisher.FluxContextWrite$ContextWriteSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"Operators.java","lineNumber":2051,"className":"reactor.core.publisher.Operators$BaseFluxToMonoOperator","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":178,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxMapFuseable.java","lineNumber":265,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxMapFuseable.java","lineNumber":265,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoFlatMap.java","lineNumber":117,"className":"reactor.core.publisher.MonoFlatMap$FlatMapMain","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":178,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxMapFuseable.java","lineNumber":265,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"MonoJust.java","lineNumber":55,"className":"reactor.core.publisher.MonoJust","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"InternalMonoOperator.java","lineNumber":76,"className":"reactor.core.publisher.InternalMonoOperator","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"MonoDefer.java","lineNumber":53,"className":"reactor.core.publisher.MonoDefer","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"Mono.java","lineNumber":4512,"className":"reactor.core.publisher.Mono","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribeWith","fileName":"Mono.java","lineNumber":4578,"className":"reactor.core.publisher.Mono","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"Mono.java","lineNumber":4339,"className":"reactor.core.publisher.Mono","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"executeCommandRaw","fileName":"AgentCommandExecutorImpl.java","lineNumber":379,"className":"io.unlogged.AgentCommandExecutorImpl","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"executeCommand","fileName":"AgentCommandExecutorImpl.java","lineNumber":477,"className":"io.unlogged.AgentCommandExecutorImpl","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"serve","fileName":"AgentCommandServer.java","lineNumber":74,"className":"io.unlogged.command.AgentCommandServer","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"execute","fileName":"NanoHTTPD.java","lineNumber":945,"className":"fi.iki.elonen.NanoHTTPD$HTTPSession","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"run","fileName":"NanoHTTPD.java","lineNumber":192,"className":"fi.iki.elonen.NanoHTTPD$ClientHandler","nativeMethod":false},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"21.0.1","methodName":"run","fileName":"Thread.java","lineNumber":1583,"className":"java.lang.Thread","nativeMethod":false}],"message":"class reactor.core.publisher.Mono$Unlogged$krH2ozp3 cannot be cast to class org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.dto.OrderRequest (reactor.core.publisher.Mono$Unlogged$krH2ozp3 and org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.dto.OrderRequest are in unnamed module of loader 'app')","suppressed":[],"localizedMessage":"class reactor.core.publisher.Mono$Unlogged$krH2ozp3 cannot be cast to class org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.dto.OrderRequest (reactor.core.publisher.Mono$Unlogged$krH2ozp3 and org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.dto.OrderRequest are in unnamed module of loader 'app')"}</t>
+  </si>
+  <si>
+    <t>org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.service.InventoryOrchestrator</t>
+  </si>
+  <si>
+    <t>create
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/OrchestrationRequestContext;)Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/OrchestrationRequestContext;&gt;;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.dto.OrchestrationRequestContext : {"orderId":"3d615566-d147-475c-9e1e-04bb7fbba82b","orderRequest":{"userId":"0","productId":"0","quantity":"0"},"productPrice":"0","paymentRequest":{"userId":"0","amount":"0","orderId":"e8a48f44-ea28-4124-a409-509873ae9dcb"},"paymentResponse":{"paymentId":"672c95d0-85a9-4f99-9c01-5a3cdbad8d8c","userId":"0","name":"string","balance":"0","status":"SUCCESS"},"inventoryRequest":{"paymentId":"56f7a621-f023-463b-bb33-48f030c5e722","productId":"0","quantity":"0"},"inventoryResponse":{"inventoryId":"d69b3a5c-bed6-43b8-bdff-ce05ffd46cd2","productId":"0","quantity":"0","remainingQuantity":"0","status":"SUCCESS"},"shippingRequest":{"quantity":"0","userId":"0","inventoryId":"4ee630ac-0e70-4bcc-b61a-8dc288183536"},"shippingResponse":{"shippingId":"3354db27-b392-49d8-8271-a6f979654220","quantity":"0","status":"SUCCESS","expectedDelivery":"string","address":{"street":"string","city":"string","state":"string","zipCode":"string"}},"status":"SUCCESS"}
+]</t>
+  </si>
+  <si>
+    <t>{"orderId":"3d615566-d147-475c-9e1e-04bb7fbba82b","orderRequest":{"userId":0,"productId":0,"quantity":0},"productPrice":0,"paymentRequest":{"userId":0,"amount":0,"orderId":"e8a48f44-ea28-4124-a409-509873ae9dcb"},"paymentResponse":{"paymentId":"672c95d0-85a9-4f99-9c01-5a3cdbad8d8c","userId":0,"name":"string","balance":0,"status":"SUCCESS"},"inventoryRequest":{"paymentId":"56f7a621-f023-463b-bb33-48f030c5e722","productId":0,"quantity":0},"inventoryResponse":{"inventoryId":null,"productId":0,"quantity":0,"remainingQuantity":null,"status":"SUCCESS"},"shippingRequest":{"quantity":0,"userId":0,"inventoryId":"4ee630ac-0e70-4bcc-b61a-8dc288183536"},"shippingResponse":{"shippingId":"3354db27-b392-49d8-8271-a6f979654220","quantity":0,"status":"SUCCESS","expectedDelivery":"string","address":{"street":"string","city":"string","state":"string","zipCode":"string"}},"status":"SUCCESS"}</t>
+  </si>
+  <si>
+    <t>isSuccess
+()Ljava/util/function/Predicate&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/OrchestrationRequestContext;&gt;;</t>
+  </si>
+  <si>
+    <t>cancel
+()Ljava/util/function/Consumer&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/OrchestrationRequestContext;&gt;;</t>
+  </si>
+  <si>
+    <t>org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.service.OrchestratorService</t>
+  </si>
+  <si>
+    <t>placeOrder
+(Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/OrderRequest;&gt;;)Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/OrderResponse;&gt;;</t>
+  </si>
+  <si>
+    <t>{"cause":null,"stackTrace":[{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onNext","fileName":"FluxMapFuseable.java","lineNumber":283,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"Operators.java","lineNumber":2571,"className":"reactor.core.publisher.Operators$ScalarSubscription","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxMapFuseable.java","lineNumber":360,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":144,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoFlatMap.java","lineNumber":194,"className":"reactor.core.publisher.MonoFlatMap$FlatMapMain","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxMapFuseable.java","lineNumber":360,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxPeekFuseable.java","lineNumber":437,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxContextWrite.java","lineNumber":136,"className":"reactor.core.publisher.FluxContextWrite$ContextWriteSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"MonoPeekTerminal.java","lineNumber":139,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"request","fileName":"FluxDoFinally.java","lineNumber":140,"className":"reactor.core.publisher.FluxDoFinally$DoFinallySubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"LambdaMonoSubscriber.java","lineNumber":121,"className":"reactor.core.publisher.LambdaMonoSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxDoFinally.java","lineNumber":107,"className":"reactor.core.publisher.FluxDoFinally$DoFinallySubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxContextWrite.java","lineNumber":101,"className":"reactor.core.publisher.FluxContextWrite$ContextWriteSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxMapFuseable.java","lineNumber":265,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":471,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoFlatMap.java","lineNumber":117,"className":"reactor.core.publisher.MonoFlatMap$FlatMapMain","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxPeekFuseable.java","lineNumber":178,"className":"reactor.core.publisher.FluxPeekFuseable$PeekFuseableSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"MonoPeekTerminal.java","lineNumber":152,"className":"reactor.core.publisher.MonoPeekTerminal$MonoTerminalPeekSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"onSubscribe","fileName":"FluxMapFuseable.java","lineNumber":265,"className":"reactor.core.publisher.FluxMapFuseable$MapFuseableConditionalSubscriber","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"MonoJust.java","lineNumber":55,"className":"reactor.core.publisher.MonoJust","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"InternalMonoOperator.java","lineNumber":76,"className":"reactor.core.publisher.InternalMonoOperator","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"MonoDefer.java","lineNumber":53,"className":"reactor.core.publisher.MonoDefer","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"Mono.java","lineNumber":4512,"className":"reactor.core.publisher.Mono","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribeWith","fileName":"Mono.java","lineNumber":4578,"className":"reactor.core.publisher.Mono","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"subscribe","fileName":"Mono.java","lineNumber":4339,"className":"reactor.core.publisher.Mono","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"executeCommandRaw","fileName":"AgentCommandExecutorImpl.java","lineNumber":379,"className":"io.unlogged.AgentCommandExecutorImpl","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"executeCommand","fileName":"AgentCommandExecutorImpl.java","lineNumber":477,"className":"io.unlogged.AgentCommandExecutorImpl","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"serve","fileName":"AgentCommandServer.java","lineNumber":74,"className":"io.unlogged.command.AgentCommandServer","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"execute","fileName":"NanoHTTPD.java","lineNumber":945,"className":"fi.iki.elonen.NanoHTTPD$HTTPSession","nativeMethod":false},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"run","fileName":"NanoHTTPD.java","lineNumber":192,"className":"fi.iki.elonen.NanoHTTPD$ClientHandler","nativeMethod":false},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"21.0.1","methodName":"run","fileName":"Thread.java","lineNumber":1583,"className":"java.lang.Thread","nativeMethod":false}],"message":"class reactor.core.publisher.Mono$Unlogged$SNxfAJNi cannot be cast to class org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.dto.OrderRequest (reactor.core.publisher.Mono$Unlogged$SNxfAJNi and org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.dto.OrderRequest are in unnamed module of loader 'app')","suppressed":[],"localizedMessage":"class reactor.core.publisher.Mono$Unlogged$SNxfAJNi cannot be cast to class org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.dto.OrderRequest (reactor.core.publisher.Mono$Unlogged$SNxfAJNi and org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.dto.OrderRequest are in unnamed module of loader 'app')"}</t>
+  </si>
+  <si>
+    <t>doOrderPostProcessing
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/OrchestrationRequestContext;)V</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.dto.OrchestrationRequestContext : {"orderId":"9a1b4849-50be-44de-8f0d-224680578e2e","orderRequest":{"userId":"0","productId":"0","quantity":"0"},"productPrice":"0","paymentRequest":{"userId":"0","amount":"0","orderId":"5b82c171-f3f2-4175-8a08-81f1e296a853"},"paymentResponse":{"paymentId":"3b4718fd-06d1-417b-9bce-15bacaabb232","userId":"0","name":"string","balance":"0","status":"SUCCESS"},"inventoryRequest":{"paymentId":"515cafc6-299f-4351-bce1-2d613b43aed0","productId":"0","quantity":"0"},"inventoryResponse":{"inventoryId":"f74b0140-d7b5-4077-94b4-5c6de3b35042","productId":"0","quantity":"0","remainingQuantity":"0","status":"SUCCESS"},"shippingRequest":{"quantity":"0","userId":"0","inventoryId":"69f1e079-1028-491c-b832-c92e8faad75d"},"shippingResponse":{"shippingId":"ba9bb515-6412-424a-ac79-a79460230111","quantity":"0","status":"SUCCESS","expectedDelivery":"string","address":{"street":"string","city":"string","state":"string","zipCode":"string"}},"status":"SUCCESS"}
+]</t>
+  </si>
+  <si>
+    <t>toOrderResponse
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/OrchestrationRequestContext;)Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/OrderResponse;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.dto.OrchestrationRequestContext : {"orderId":"b2256453-b827-4cc9-b5d8-7e6c382b70db","orderRequest":{"userId":"0","productId":"0","quantity":"0"},"productPrice":"0","paymentRequest":{"userId":"0","amount":"0","orderId":"c6d89726-c19d-4660-838f-4c7491bc7837"},"paymentResponse":{"paymentId":"b700f072-dca6-44c7-9a47-621e2144d85a","userId":"0","name":"string","balance":"0","status":"SUCCESS"},"inventoryRequest":{"paymentId":"543e6f88-5872-413a-87c9-0d668b1907a2","productId":"0","quantity":"0"},"inventoryResponse":{"inventoryId":"ecc1a694-b9f6-479a-9db4-cc500db2b344","productId":"0","quantity":"0","remainingQuantity":"0","status":"SUCCESS"},"shippingRequest":{"quantity":"0","userId":"0","inventoryId":"89d90e28-8992-423e-9803-f6419b8438c5"},"shippingResponse":{"shippingId":"216b0eee-3ae6-4dde-bce4-9b4aa78b8e21","quantity":"0","status":"SUCCESS","expectedDelivery":"string","address":{"street":"string","city":"string","state":"string","zipCode":"string"}},"status":"SUCCESS"}
+]</t>
+  </si>
+  <si>
+    <t>{"userId":0,"productId":0,"orderId":"b2256453-b827-4cc9-b5d8-7e6c382b70db","status":"SUCCESS","shippingAddress":{"street":"string","city":"string","state":"string","zipCode":"string"},"expectedDelivery":"string"}</t>
+  </si>
+  <si>
+    <t>org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.service.OrderCancellationService</t>
+  </si>
+  <si>
+    <t>init
+()V</t>
+  </si>
+  <si>
+    <t>cancelOrder
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/OrchestrationRequestContext;)V</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.dto.OrchestrationRequestContext : {"orderId":"0fdf2785-6560-4c70-91d1-9ceefb68e675","orderRequest":{"userId":"0","productId":"0","quantity":"0"},"productPrice":"0","paymentRequest":{"userId":"0","amount":"0","orderId":"1cd9125c-7f9c-4765-a89f-3ab6c6e111bb"},"paymentResponse":{"paymentId":"37b927d3-e9f1-4658-8e1c-9da24c9fd61d","userId":"0","name":"string","balance":"0","status":"SUCCESS"},"inventoryRequest":{"paymentId":"86cb8e7a-d823-470a-8113-7c745ea4cdfc","productId":"0","quantity":"0"},"inventoryResponse":{"inventoryId":"74cf4644-8c52-4d08-bf52-046eac10734a","productId":"0","quantity":"0","remainingQuantity":"0","status":"SUCCESS"},"shippingRequest":{"quantity":"0","userId":"0","inventoryId":"f28d8883-7f32-45dd-aa2d-b932b96aecb2"},"shippingResponse":{"shippingId":"46fdcda5-193d-4221-9100-931b41a5aec3","quantity":"0","status":"SUCCESS","expectedDelivery":"string","address":{"street":"string","city":"string","state":"string","zipCode":"string"}},"status":"SUCCESS"}
+]</t>
+  </si>
+  <si>
+    <t>org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.service.OrderFulfillmentService</t>
+  </si>
+  <si>
+    <t>placeOrder
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/OrchestrationRequestContext;)Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/OrchestrationRequestContext;&gt;;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.dto.OrchestrationRequestContext : {"orderId":"26a4b57c-2907-4be7-805d-db8778e11da6","orderRequest":{"userId":"0","productId":"0","quantity":"0"},"productPrice":"0","paymentRequest":{"userId":"0","amount":"0","orderId":"fd17dac4-92d2-4be3-9092-7326ce56b774"},"paymentResponse":{"paymentId":"94eca432-c847-4b2f-9fcd-515bd473d824","userId":"0","name":"string","balance":"0","status":"SUCCESS"},"inventoryRequest":{"paymentId":"c89860a7-3bf6-44c3-8170-5841296a3254","productId":"0","quantity":"0"},"inventoryResponse":{"inventoryId":"9480d9f2-92fe-46e8-915a-1d133dbcf813","productId":"0","quantity":"0","remainingQuantity":"0","status":"SUCCESS"},"shippingRequest":{"quantity":"0","userId":"0","inventoryId":"636129f4-bb8d-46e5-8cac-514572a5071a"},"shippingResponse":{"shippingId":"5479c8e0-cd64-45d2-b2f4-9180d78f153a","quantity":"0","status":"SUCCESS","expectedDelivery":"string","address":{"street":"string","city":"string","state":"string","zipCode":"string"}},"status":"SUCCESS"}
+]</t>
+  </si>
+  <si>
+    <t>{"orderId":"26a4b57c-2907-4be7-805d-db8778e11da6","orderRequest":{"userId":0,"productId":0,"quantity":0},"productPrice":100,"paymentRequest":{"userId":0,"amount":0,"orderId":"26a4b57c-2907-4be7-805d-db8778e11da6"},"paymentResponse":{"paymentId":null,"userId":0,"name":null,"balance":0,"status":"SUCCESS"},"inventoryRequest":{"paymentId":null,"productId":0,"quantity":0},"inventoryResponse":{"inventoryId":null,"productId":0,"quantity":0,"remainingQuantity":null,"status":"SUCCESS"},"shippingRequest":{"quantity":0,"userId":0,"inventoryId":null},"shippingResponse":{"shippingId":null,"quantity":0,"status":"SUCCESS","expectedDelivery":"2024-06-27","address":{"street":"123 Main St","city":"Anytown","state":"AnyState","zipCode":"12345"}},"status":"SUCCESS"}</t>
+  </si>
+  <si>
+    <t>getProduct
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/OrchestrationRequestContext;)Lreactor/core/publisher/Mono&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/orchestrator/orchestratorsequential/sec04/dto/OrchestrationRequestContext;&gt;;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.dto.OrchestrationRequestContext : {"orderId":"08b9f71b-86b0-4b15-b3ee-061a1617aab3","orderRequest":{"userId":"0","productId":"0","quantity":"0"},"productPrice":"0","paymentRequest":{"userId":"0","amount":"0","orderId":"43a403a5-ac3f-497c-8974-7566b8f60736"},"paymentResponse":{"paymentId":"640c5e1f-b808-4c3e-b6ac-5542c87c05c0","userId":"0","name":"string","balance":"0","status":"SUCCESS"},"inventoryRequest":{"paymentId":"ef804014-a9c2-41f7-b2b9-e59da5d0e76e","productId":"0","quantity":"0"},"inventoryResponse":{"inventoryId":"809c78b4-5f6a-4245-9701-9e133be12317","productId":"0","quantity":"0","remainingQuantity":"0","status":"SUCCESS"},"shippingRequest":{"quantity":"0","userId":"0","inventoryId":"dc0c7da4-374b-4056-b242-41ae69c2e813"},"shippingResponse":{"shippingId":"6e99be42-80f3-4fc9-984c-7293e2e30fd9","quantity":"0","status":"SUCCESS","expectedDelivery":"string","address":{"street":"string","city":"string","state":"string","zipCode":"string"}},"status":"SUCCESS"}
+]</t>
+  </si>
+  <si>
+    <t>{"orderId":"08b9f71b-86b0-4b15-b3ee-061a1617aab3","orderRequest":{"userId":0,"productId":0,"quantity":0},"productPrice":100,"paymentRequest":{"userId":0,"amount":0,"orderId":"43a403a5-ac3f-497c-8974-7566b8f60736"},"paymentResponse":{"paymentId":"640c5e1f-b808-4c3e-b6ac-5542c87c05c0","userId":0,"name":"string","balance":0,"status":"SUCCESS"},"inventoryRequest":{"paymentId":"ef804014-a9c2-41f7-b2b9-e59da5d0e76e","productId":0,"quantity":0},"inventoryResponse":{"inventoryId":"809c78b4-5f6a-4245-9701-9e133be12317","productId":0,"quantity":0,"remainingQuantity":0,"status":"SUCCESS"},"shippingRequest":{"quantity":0,"userId":0,"inventoryId":"dc0c7da4-374b-4056-b242-41ae69c2e813"},"shippingResponse":{"shippingId":"6e99be42-80f3-4fc9-984c-7293e2e30fd9","quantity":0,"status":"SUCCESS","expectedDelivery":"string","address":{"street":"string","city":"string","state":"string","zipCode":"string"}},"status":"SUCCESS"}</t>
+  </si>
+  <si>
+    <t>org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.service.PaymentOrchestrator</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.dto.OrchestrationRequestContext : {"orderId":"afc05092-22c0-4dc7-a034-4912a5752dec","orderRequest":{"userId":"0","productId":"0","quantity":"0"},"productPrice":"0","paymentRequest":{"userId":"0","amount":"0","orderId":"3f8550c3-20b0-4b9c-8106-1322a0793588"},"paymentResponse":{"paymentId":"07fbbab4-c2d1-4f39-91a1-f3a1409fe279","userId":"0","name":"string","balance":"0","status":"SUCCESS"},"inventoryRequest":{"paymentId":"61251e3b-d874-44ee-86e7-649343f7c8ad","productId":"0","quantity":"0"},"inventoryResponse":{"inventoryId":"e9bd765b-e0b5-4856-97d4-a0cac4e14425","productId":"0","quantity":"0","remainingQuantity":"0","status":"SUCCESS"},"shippingRequest":{"quantity":"0","userId":"0","inventoryId":"b02ededd-0c17-4d54-83fc-d0f2f4020df5"},"shippingResponse":{"shippingId":"ce80136e-eb35-411e-a40e-1019d7a94262","quantity":"0","status":"SUCCESS","expectedDelivery":"string","address":{"street":"string","city":"string","state":"string","zipCode":"string"}},"status":"SUCCESS"}
+]</t>
+  </si>
+  <si>
+    <t>{"orderId":"afc05092-22c0-4dc7-a034-4912a5752dec","orderRequest":{"userId":0,"productId":0,"quantity":0},"productPrice":0,"paymentRequest":{"userId":0,"amount":0,"orderId":"3f8550c3-20b0-4b9c-8106-1322a0793588"},"paymentResponse":{"paymentId":null,"userId":0,"name":null,"balance":0,"status":"SUCCESS"},"inventoryRequest":{"paymentId":"61251e3b-d874-44ee-86e7-649343f7c8ad","productId":0,"quantity":0},"inventoryResponse":{"inventoryId":"e9bd765b-e0b5-4856-97d4-a0cac4e14425","productId":0,"quantity":0,"remainingQuantity":0,"status":"SUCCESS"},"shippingRequest":{"quantity":0,"userId":0,"inventoryId":"b02ededd-0c17-4d54-83fc-d0f2f4020df5"},"shippingResponse":{"shippingId":"ce80136e-eb35-411e-a40e-1019d7a94262","quantity":0,"status":"SUCCESS","expectedDelivery":"string","address":{"street":"string","city":"string","state":"string","zipCode":"string"}},"status":"SUCCESS"}</t>
+  </si>
+  <si>
+    <t>org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.service.ShippingOrchestrator</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.orchestrator.orchestratorsequential.sec04.dto.OrchestrationRequestContext : {"orderId":"0a513a69-22c3-48d8-a093-72811c77c44e","orderRequest":{"userId":"0","productId":"0","quantity":"0"},"productPrice":"0","paymentRequest":{"userId":"0","amount":"0","orderId":"562e597d-2540-45d8-b90b-b1cda8f1ad80"},"paymentResponse":{"paymentId":"77f3601b-d864-4df7-806f-4bac083cbc6a","userId":"0","name":"string","balance":"0","status":"SUCCESS"},"inventoryRequest":{"paymentId":"c491eb08-ac9b-4501-b6c4-d4cfb60a5115","productId":"0","quantity":"0"},"inventoryResponse":{"inventoryId":"fbfc5fe1-49ad-404b-abbf-0b9ec2525393","productId":"0","quantity":"0","remainingQuantity":"0","status":"SUCCESS"},"shippingRequest":{"quantity":"0","userId":"0","inventoryId":"075fef31-3709-47df-a0a0-a0aebdfe18ec"},"shippingResponse":{"shippingId":"8938bf94-56f2-420c-b823-e96241c4beb8","quantity":"0","status":"SUCCESS","expectedDelivery":"string","address":{"street":"string","city":"string","state":"string","zipCode":"string"}},"status":"SUCCESS"}
+]</t>
+  </si>
+  <si>
+    <t>{"orderId":"0a513a69-22c3-48d8-a093-72811c77c44e","orderRequest":{"userId":0,"productId":0,"quantity":0},"productPrice":0,"paymentRequest":{"userId":0,"amount":0,"orderId":"562e597d-2540-45d8-b90b-b1cda8f1ad80"},"paymentResponse":{"paymentId":"77f3601b-d864-4df7-806f-4bac083cbc6a","userId":0,"name":"string","balance":0,"status":"SUCCESS"},"inventoryRequest":{"paymentId":"c491eb08-ac9b-4501-b6c4-d4cfb60a5115","productId":0,"quantity":0},"inventoryResponse":{"inventoryId":"fbfc5fe1-49ad-404b-abbf-0b9ec2525393","productId":0,"quantity":0,"remainingQuantity":0,"status":"SUCCESS"},"shippingRequest":{"quantity":0,"userId":0,"inventoryId":"075fef31-3709-47df-a0a0-a0aebdfe18ec"},"shippingResponse":{"shippingId":null,"quantity":0,"status":"SUCCESS","expectedDelivery":"2024-06-27","address":{"street":"123 Main St","city":"Anytown","state":"AnyState","zipCode":"12345"}},"status":"SUCCESS"}</t>
+  </si>
+  <si>
+    <t>org.unlogged.springwebfluxdemo.integrationpatterns.scattergather.client.BlueDartClient</t>
+  </si>
+  <si>
+    <t>getServiceOptions
+(Ljava/lang/String;Ljava/lang/String;)Lreactor/core/publisher/Flux&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/scattergather/dto/CarrierResponse;&gt;;</t>
+  </si>
+  <si>
+    <t>[java.lang.String : "string"
+, java.lang.String : "string"
+]</t>
+  </si>
+  <si>
+    <t>[{"serviceProvider":"BlueDart","from":"string","to":"string","price":12.0,"date":"2024-06-24"},{"serviceProvider":"BlueDart","from":"string","to":"string","price":18.0,"date":"2024-06-24"}]</t>
+  </si>
+  <si>
+    <t>org.unlogged.springwebfluxdemo.integrationpatterns.scattergather.client.DHLClient</t>
+  </si>
+  <si>
+    <t>normalizeResponse
+(Lorg/unlogged/springwebfluxdemo/integrationpatterns/scattergather/dto/CarrierResponse;Ljava/lang/String;Ljava/lang/String;)V</t>
+  </si>
+  <si>
+    <t>[org.unlogged.springwebfluxdemo.integrationpatterns.scattergather.dto.CarrierResponse : {"serviceProvider":"string","from":"string","to":"string","price":"0","date":{"year":"0","month":"0","day":"0"}}
+, java.lang.String : "string"
+, java.lang.String : "string"
+]</t>
+  </si>
+  <si>
+    <t>org.unlogged.springwebfluxdemo.integrationpatterns.scattergather.controller.CarrierController</t>
+  </si>
+  <si>
+    <t>getCarriers
+(Ljava/lang/String;Ljava/lang/String;)Lreactor/core/publisher/Flux&lt;Lorg/unlogged/springwebfluxdemo/integrationpatterns/scattergather/dto/CarrierResponse;&gt;;</t>
   </si>
 </sst>
 </file>
@@ -3679,7 +4319,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3688,6 +4328,12 @@
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -24620,77 +25266,3130 @@
       <c r="Y556" s="4"/>
       <c r="Z556" s="4"/>
     </row>
-    <row r="557" ht="15.75" customHeight="1"/>
-    <row r="558" ht="15.75" customHeight="1"/>
-    <row r="559" ht="15.75" customHeight="1"/>
-    <row r="560" ht="15.75" customHeight="1"/>
-    <row r="561" ht="15.75" customHeight="1"/>
-    <row r="562" ht="15.75" customHeight="1"/>
-    <row r="563" ht="15.75" customHeight="1"/>
-    <row r="564" ht="15.75" customHeight="1"/>
-    <row r="565" ht="15.75" customHeight="1"/>
-    <row r="566" ht="15.75" customHeight="1"/>
-    <row r="567" ht="15.75" customHeight="1"/>
-    <row r="568" ht="15.75" customHeight="1"/>
-    <row r="569" ht="15.75" customHeight="1"/>
-    <row r="570" ht="15.75" customHeight="1"/>
-    <row r="571" ht="15.75" customHeight="1"/>
-    <row r="572" ht="15.75" customHeight="1"/>
-    <row r="573" ht="15.75" customHeight="1"/>
-    <row r="574" ht="15.75" customHeight="1"/>
-    <row r="575" ht="15.75" customHeight="1"/>
-    <row r="576" ht="15.75" customHeight="1"/>
-    <row r="577" ht="15.75" customHeight="1"/>
-    <row r="578" ht="15.75" customHeight="1"/>
-    <row r="579" ht="15.75" customHeight="1"/>
-    <row r="580" ht="15.75" customHeight="1"/>
-    <row r="581" ht="15.75" customHeight="1"/>
-    <row r="582" ht="15.75" customHeight="1"/>
-    <row r="583" ht="15.75" customHeight="1"/>
-    <row r="584" ht="15.75" customHeight="1"/>
-    <row r="585" ht="15.75" customHeight="1"/>
-    <row r="586" ht="15.75" customHeight="1"/>
-    <row r="587" ht="15.75" customHeight="1"/>
-    <row r="588" ht="15.75" customHeight="1"/>
-    <row r="589" ht="15.75" customHeight="1"/>
-    <row r="590" ht="15.75" customHeight="1"/>
-    <row r="591" ht="15.75" customHeight="1"/>
-    <row r="592" ht="15.75" customHeight="1"/>
-    <row r="593" ht="15.75" customHeight="1"/>
-    <row r="594" ht="15.75" customHeight="1"/>
-    <row r="595" ht="15.75" customHeight="1"/>
-    <row r="596" ht="15.75" customHeight="1"/>
-    <row r="597" ht="15.75" customHeight="1"/>
-    <row r="598" ht="15.75" customHeight="1"/>
-    <row r="599" ht="15.75" customHeight="1"/>
-    <row r="600" ht="15.75" customHeight="1"/>
-    <row r="601" ht="15.75" customHeight="1"/>
-    <row r="602" ht="15.75" customHeight="1"/>
-    <row r="603" ht="15.75" customHeight="1"/>
-    <row r="604" ht="15.75" customHeight="1"/>
-    <row r="605" ht="15.75" customHeight="1"/>
-    <row r="606" ht="15.75" customHeight="1"/>
-    <row r="607" ht="15.75" customHeight="1"/>
-    <row r="608" ht="15.75" customHeight="1"/>
-    <row r="609" ht="15.75" customHeight="1"/>
-    <row r="610" ht="15.75" customHeight="1"/>
-    <row r="611" ht="15.75" customHeight="1"/>
-    <row r="612" ht="15.75" customHeight="1"/>
-    <row r="613" ht="15.75" customHeight="1"/>
-    <row r="614" ht="15.75" customHeight="1"/>
-    <row r="615" ht="15.75" customHeight="1"/>
-    <row r="616" ht="15.75" customHeight="1"/>
-    <row r="617" ht="15.75" customHeight="1"/>
-    <row r="618" ht="15.75" customHeight="1"/>
-    <row r="619" ht="15.75" customHeight="1"/>
-    <row r="620" ht="15.75" customHeight="1"/>
-    <row r="621" ht="15.75" customHeight="1"/>
-    <row r="622" ht="15.75" customHeight="1"/>
-    <row r="623" ht="15.75" customHeight="1"/>
-    <row r="624" ht="15.75" customHeight="1"/>
-    <row r="625" ht="15.75" customHeight="1"/>
-    <row r="626" ht="15.75" customHeight="1"/>
-    <row r="627" ht="15.75" customHeight="1"/>
+    <row r="557" ht="15.75" customHeight="1">
+      <c r="A557" s="5" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B557" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C557" s="5" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D557" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E557" s="5" t="s">
+        <v>1028</v>
+      </c>
+      <c r="F557" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G557" s="6" t="s">
+        <v>1029</v>
+      </c>
+      <c r="H557" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I557" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J557" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K557" s="5"/>
+      <c r="L557" s="5"/>
+      <c r="M557" s="5"/>
+      <c r="N557" s="5"/>
+      <c r="O557" s="5"/>
+      <c r="P557" s="5"/>
+      <c r="Q557" s="5"/>
+      <c r="R557" s="5"/>
+      <c r="S557" s="5"/>
+      <c r="T557" s="5"/>
+      <c r="U557" s="5"/>
+      <c r="V557" s="5"/>
+    </row>
+    <row r="558" ht="15.75" customHeight="1">
+      <c r="A558" s="5" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B558" s="5" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C558" s="5" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D558" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E558" s="5" t="s">
+        <v>1032</v>
+      </c>
+      <c r="F558" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G558" s="6" t="s">
+        <v>1033</v>
+      </c>
+      <c r="H558" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I558" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J558" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K558" s="5"/>
+      <c r="L558" s="5"/>
+      <c r="M558" s="5"/>
+      <c r="N558" s="5"/>
+      <c r="O558" s="5"/>
+      <c r="P558" s="5"/>
+      <c r="Q558" s="5"/>
+      <c r="R558" s="5"/>
+      <c r="S558" s="5"/>
+      <c r="T558" s="5"/>
+      <c r="U558" s="5"/>
+      <c r="V558" s="5"/>
+    </row>
+    <row r="559" ht="15.75" customHeight="1">
+      <c r="A559" s="5" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B559" s="5" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C559" s="5" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D559" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E559" s="5" t="s">
+        <v>1035</v>
+      </c>
+      <c r="F559" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G559" s="6" t="s">
+        <v>1033</v>
+      </c>
+      <c r="H559" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I559" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J559" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K559" s="5"/>
+      <c r="L559" s="5"/>
+      <c r="M559" s="5"/>
+      <c r="N559" s="5"/>
+      <c r="O559" s="5"/>
+      <c r="P559" s="5"/>
+      <c r="Q559" s="5"/>
+      <c r="R559" s="5"/>
+      <c r="S559" s="5"/>
+      <c r="T559" s="5"/>
+      <c r="U559" s="5"/>
+      <c r="V559" s="5"/>
+    </row>
+    <row r="560" ht="15.75" customHeight="1">
+      <c r="A560" s="5" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B560" s="5" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C560" s="5" t="s">
+        <v>1036</v>
+      </c>
+      <c r="D560" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E560" s="5" t="s">
+        <v>1038</v>
+      </c>
+      <c r="F560" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G560" s="6" t="s">
+        <v>1039</v>
+      </c>
+      <c r="H560" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I560" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J560" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K560" s="5"/>
+      <c r="L560" s="5"/>
+      <c r="M560" s="5"/>
+      <c r="N560" s="5"/>
+      <c r="O560" s="5"/>
+      <c r="P560" s="5"/>
+      <c r="Q560" s="5"/>
+      <c r="R560" s="5"/>
+      <c r="S560" s="5"/>
+      <c r="T560" s="5"/>
+      <c r="U560" s="5"/>
+      <c r="V560" s="5"/>
+    </row>
+    <row r="561" ht="15.75" customHeight="1">
+      <c r="A561" s="5" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B561" s="5" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C561" s="5" t="s">
+        <v>1036</v>
+      </c>
+      <c r="D561" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E561" s="5" t="s">
+        <v>1041</v>
+      </c>
+      <c r="F561" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G561" s="6" t="s">
+        <v>1039</v>
+      </c>
+      <c r="H561" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I561" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J561" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K561" s="5"/>
+      <c r="L561" s="5"/>
+      <c r="M561" s="5"/>
+      <c r="N561" s="5"/>
+      <c r="O561" s="5"/>
+      <c r="P561" s="5"/>
+      <c r="Q561" s="5"/>
+      <c r="R561" s="5"/>
+      <c r="S561" s="5"/>
+      <c r="T561" s="5"/>
+      <c r="U561" s="5"/>
+      <c r="V561" s="5"/>
+    </row>
+    <row r="562" ht="15.75" customHeight="1">
+      <c r="A562" s="5" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B562" s="5" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C562" s="5" t="s">
+        <v>1042</v>
+      </c>
+      <c r="D562" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E562" s="5" t="s">
+        <v>1044</v>
+      </c>
+      <c r="F562" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G562" s="6" t="s">
+        <v>1045</v>
+      </c>
+      <c r="H562" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I562" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J562" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K562" s="5"/>
+      <c r="L562" s="5"/>
+      <c r="M562" s="5"/>
+      <c r="N562" s="5"/>
+      <c r="O562" s="5"/>
+      <c r="P562" s="5"/>
+      <c r="Q562" s="5"/>
+      <c r="R562" s="5"/>
+      <c r="S562" s="5"/>
+      <c r="T562" s="5"/>
+      <c r="U562" s="5"/>
+      <c r="V562" s="5"/>
+    </row>
+    <row r="563" ht="15.75" customHeight="1">
+      <c r="A563" s="5" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B563" s="5" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C563" s="5" t="s">
+        <v>1042</v>
+      </c>
+      <c r="D563" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E563" s="5" t="s">
+        <v>1047</v>
+      </c>
+      <c r="F563" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G563" s="6" t="s">
+        <v>1048</v>
+      </c>
+      <c r="H563" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I563" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J563" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K563" s="5"/>
+      <c r="L563" s="5"/>
+      <c r="M563" s="5"/>
+      <c r="N563" s="5"/>
+      <c r="O563" s="5"/>
+      <c r="P563" s="5"/>
+      <c r="Q563" s="5"/>
+      <c r="R563" s="5"/>
+      <c r="S563" s="5"/>
+      <c r="T563" s="5"/>
+      <c r="U563" s="5"/>
+      <c r="V563" s="5"/>
+    </row>
+    <row r="564" ht="15.75" customHeight="1">
+      <c r="A564" s="5" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B564" s="5" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C564" s="5" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D564" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E564" s="5" t="s">
+        <v>1051</v>
+      </c>
+      <c r="F564" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G564" s="6" t="s">
+        <v>1052</v>
+      </c>
+      <c r="H564" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I564" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J564" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K564" s="5"/>
+      <c r="L564" s="5"/>
+      <c r="M564" s="5"/>
+      <c r="N564" s="5"/>
+      <c r="O564" s="5"/>
+      <c r="P564" s="5"/>
+      <c r="Q564" s="5"/>
+      <c r="R564" s="5"/>
+      <c r="S564" s="5"/>
+      <c r="T564" s="5"/>
+      <c r="U564" s="5"/>
+      <c r="V564" s="5"/>
+    </row>
+    <row r="565" ht="15.75" customHeight="1">
+      <c r="A565" s="5" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B565" s="5" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C565" s="5" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D565" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E565" s="5" t="s">
+        <v>1054</v>
+      </c>
+      <c r="F565" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G565" s="6" t="s">
+        <v>1052</v>
+      </c>
+      <c r="H565" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I565" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J565" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K565" s="5"/>
+      <c r="L565" s="5"/>
+      <c r="M565" s="5"/>
+      <c r="N565" s="5"/>
+      <c r="O565" s="5"/>
+      <c r="P565" s="5"/>
+      <c r="Q565" s="5"/>
+      <c r="R565" s="5"/>
+      <c r="S565" s="5"/>
+      <c r="T565" s="5"/>
+      <c r="U565" s="5"/>
+      <c r="V565" s="5"/>
+    </row>
+    <row r="566" ht="15.75" customHeight="1">
+      <c r="A566" s="5" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B566" s="5" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C566" s="5" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D566" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E566" s="5" t="s">
+        <v>1056</v>
+      </c>
+      <c r="F566" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G566" s="6" t="s">
+        <v>1057</v>
+      </c>
+      <c r="H566" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I566" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J566" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K566" s="5"/>
+      <c r="L566" s="5"/>
+      <c r="M566" s="5"/>
+      <c r="N566" s="5"/>
+      <c r="O566" s="5"/>
+      <c r="P566" s="5"/>
+      <c r="Q566" s="5"/>
+      <c r="R566" s="5"/>
+      <c r="S566" s="5"/>
+      <c r="T566" s="5"/>
+      <c r="U566" s="5"/>
+      <c r="V566" s="5"/>
+    </row>
+    <row r="567" ht="15.75" customHeight="1">
+      <c r="A567" s="5" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B567" s="5" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C567" s="5" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D567" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E567" s="5" t="s">
+        <v>1059</v>
+      </c>
+      <c r="F567" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G567" s="6" t="s">
+        <v>1057</v>
+      </c>
+      <c r="H567" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I567" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J567" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K567" s="5"/>
+      <c r="L567" s="5"/>
+      <c r="M567" s="5"/>
+      <c r="N567" s="5"/>
+      <c r="O567" s="5"/>
+      <c r="P567" s="5"/>
+      <c r="Q567" s="5"/>
+      <c r="R567" s="5"/>
+      <c r="S567" s="5"/>
+      <c r="T567" s="5"/>
+      <c r="U567" s="5"/>
+      <c r="V567" s="5"/>
+    </row>
+    <row r="568" ht="15.75" customHeight="1">
+      <c r="A568" s="5" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B568" s="5" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C568" s="5" t="s">
+        <v>1060</v>
+      </c>
+      <c r="D568" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E568" s="5" t="s">
+        <v>1028</v>
+      </c>
+      <c r="F568" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G568" s="6" t="s">
+        <v>1062</v>
+      </c>
+      <c r="H568" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I568" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J568" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K568" s="5"/>
+      <c r="L568" s="5"/>
+      <c r="M568" s="5"/>
+      <c r="N568" s="5"/>
+      <c r="O568" s="5"/>
+      <c r="P568" s="5"/>
+      <c r="Q568" s="5"/>
+      <c r="R568" s="5"/>
+      <c r="S568" s="5"/>
+      <c r="T568" s="5"/>
+      <c r="U568" s="5"/>
+      <c r="V568" s="5"/>
+    </row>
+    <row r="569" ht="15.75" customHeight="1">
+      <c r="A569" s="5" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B569" s="5" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C569" s="5" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D569" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E569" s="5" t="s">
+        <v>1065</v>
+      </c>
+      <c r="F569" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G569" s="6" t="s">
+        <v>1066</v>
+      </c>
+      <c r="H569" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I569" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J569" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K569" s="5"/>
+      <c r="L569" s="5"/>
+      <c r="M569" s="5"/>
+      <c r="N569" s="5"/>
+      <c r="O569" s="5"/>
+      <c r="P569" s="5"/>
+      <c r="Q569" s="5"/>
+      <c r="R569" s="5"/>
+      <c r="S569" s="5"/>
+      <c r="T569" s="5"/>
+      <c r="U569" s="5"/>
+      <c r="V569" s="5"/>
+    </row>
+    <row r="570" ht="15.75" customHeight="1">
+      <c r="A570" s="5" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B570" s="5" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C570" s="5" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D570" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E570" s="5" t="s">
+        <v>1068</v>
+      </c>
+      <c r="F570" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G570" s="6" t="s">
+        <v>1069</v>
+      </c>
+      <c r="H570" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I570" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J570" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K570" s="5"/>
+      <c r="L570" s="5"/>
+      <c r="M570" s="5"/>
+      <c r="N570" s="5"/>
+      <c r="O570" s="5"/>
+      <c r="P570" s="5"/>
+      <c r="Q570" s="5"/>
+      <c r="R570" s="5"/>
+      <c r="S570" s="5"/>
+      <c r="T570" s="5"/>
+      <c r="U570" s="5"/>
+      <c r="V570" s="5"/>
+    </row>
+    <row r="571" ht="15.75" customHeight="1">
+      <c r="A571" s="5" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B571" s="5" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C571" s="5" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D571" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E571" s="5" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F571" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G571" s="6" t="s">
+        <v>1072</v>
+      </c>
+      <c r="H571" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I571" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J571" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K571" s="5"/>
+      <c r="L571" s="5"/>
+      <c r="M571" s="5"/>
+      <c r="N571" s="5"/>
+      <c r="O571" s="5"/>
+      <c r="P571" s="5"/>
+      <c r="Q571" s="5"/>
+      <c r="R571" s="5"/>
+      <c r="S571" s="5"/>
+      <c r="T571" s="5"/>
+      <c r="U571" s="5"/>
+      <c r="V571" s="5"/>
+    </row>
+    <row r="572" ht="15.75" customHeight="1">
+      <c r="A572" s="5" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B572" s="5" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C572" s="5" t="s">
+        <v>1073</v>
+      </c>
+      <c r="D572" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E572" s="5" t="s">
+        <v>1075</v>
+      </c>
+      <c r="F572" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G572" s="6" t="s">
+        <v>1076</v>
+      </c>
+      <c r="H572" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I572" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J572" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K572" s="5"/>
+      <c r="L572" s="5"/>
+      <c r="M572" s="5"/>
+      <c r="N572" s="5"/>
+      <c r="O572" s="5"/>
+      <c r="P572" s="5"/>
+      <c r="Q572" s="5"/>
+      <c r="R572" s="5"/>
+      <c r="S572" s="5"/>
+      <c r="T572" s="5"/>
+      <c r="U572" s="5"/>
+      <c r="V572" s="5"/>
+    </row>
+    <row r="573" ht="15.75" customHeight="1">
+      <c r="A573" s="5" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B573" s="5" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C573" s="5" t="s">
+        <v>1073</v>
+      </c>
+      <c r="D573" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E573" s="5" t="s">
+        <v>1078</v>
+      </c>
+      <c r="F573" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G573" s="6" t="s">
+        <v>1076</v>
+      </c>
+      <c r="H573" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I573" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J573" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K573" s="5"/>
+      <c r="L573" s="5"/>
+      <c r="M573" s="5"/>
+      <c r="N573" s="5"/>
+      <c r="O573" s="5"/>
+      <c r="P573" s="5"/>
+      <c r="Q573" s="5"/>
+      <c r="R573" s="5"/>
+      <c r="S573" s="5"/>
+      <c r="T573" s="5"/>
+      <c r="U573" s="5"/>
+      <c r="V573" s="5"/>
+    </row>
+    <row r="574" ht="15.75" customHeight="1">
+      <c r="A574" s="5" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B574" s="5" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C574" s="5" t="s">
+        <v>1073</v>
+      </c>
+      <c r="D574" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E574" s="5" t="s">
+        <v>1080</v>
+      </c>
+      <c r="F574" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G574" s="6" t="s">
+        <v>1081</v>
+      </c>
+      <c r="H574" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I574" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J574" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K574" s="5"/>
+      <c r="L574" s="5"/>
+      <c r="M574" s="5"/>
+      <c r="N574" s="5"/>
+      <c r="O574" s="5"/>
+      <c r="P574" s="5"/>
+      <c r="Q574" s="5"/>
+      <c r="R574" s="5"/>
+      <c r="S574" s="5"/>
+      <c r="T574" s="5"/>
+      <c r="U574" s="5"/>
+      <c r="V574" s="5"/>
+    </row>
+    <row r="575" ht="15.75" customHeight="1">
+      <c r="A575" s="5" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B575" s="5" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C575" s="5" t="s">
+        <v>1073</v>
+      </c>
+      <c r="D575" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E575" s="5" t="s">
+        <v>1083</v>
+      </c>
+      <c r="F575" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G575" s="6" t="s">
+        <v>1081</v>
+      </c>
+      <c r="H575" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I575" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J575" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K575" s="5"/>
+      <c r="L575" s="5"/>
+      <c r="M575" s="5"/>
+      <c r="N575" s="5"/>
+      <c r="O575" s="5"/>
+      <c r="P575" s="5"/>
+      <c r="Q575" s="5"/>
+      <c r="R575" s="5"/>
+      <c r="S575" s="5"/>
+      <c r="T575" s="5"/>
+      <c r="U575" s="5"/>
+      <c r="V575" s="5"/>
+    </row>
+    <row r="576" ht="15.75" customHeight="1">
+      <c r="A576" s="5" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B576" s="5" t="s">
+        <v>1085</v>
+      </c>
+      <c r="C576" s="5" t="s">
+        <v>1084</v>
+      </c>
+      <c r="D576" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E576" s="5" t="s">
+        <v>1086</v>
+      </c>
+      <c r="F576" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G576" s="5" t="s">
+        <v>1087</v>
+      </c>
+      <c r="H576" s="5" t="s">
+        <v>1087</v>
+      </c>
+      <c r="I576" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="J576" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K576" s="5"/>
+      <c r="L576" s="5"/>
+      <c r="M576" s="5"/>
+      <c r="N576" s="5"/>
+      <c r="O576" s="5"/>
+      <c r="P576" s="5"/>
+      <c r="Q576" s="5"/>
+      <c r="R576" s="5"/>
+      <c r="S576" s="5"/>
+      <c r="T576" s="5"/>
+      <c r="U576" s="5"/>
+      <c r="V576" s="5"/>
+    </row>
+    <row r="577" ht="15.75" customHeight="1">
+      <c r="A577" s="5" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B577" s="5" t="s">
+        <v>1085</v>
+      </c>
+      <c r="C577" s="5" t="s">
+        <v>1084</v>
+      </c>
+      <c r="D577" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E577" s="5" t="s">
+        <v>1086</v>
+      </c>
+      <c r="F577" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G577" s="5" t="s">
+        <v>1088</v>
+      </c>
+      <c r="H577" s="5" t="s">
+        <v>1088</v>
+      </c>
+      <c r="I577" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="J577" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K577" s="5"/>
+      <c r="L577" s="5"/>
+      <c r="M577" s="5"/>
+      <c r="N577" s="5"/>
+      <c r="O577" s="5"/>
+      <c r="P577" s="5"/>
+      <c r="Q577" s="5"/>
+      <c r="R577" s="5"/>
+      <c r="S577" s="5"/>
+      <c r="T577" s="5"/>
+      <c r="U577" s="5"/>
+      <c r="V577" s="5"/>
+    </row>
+    <row r="578" ht="15.75" customHeight="1">
+      <c r="A578" s="5" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B578" s="5" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C578" s="5" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D578" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E578" s="5" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F578" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G578" s="6" t="s">
+        <v>1092</v>
+      </c>
+      <c r="H578" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I578" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J578" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K578" s="5"/>
+      <c r="L578" s="5"/>
+      <c r="M578" s="5"/>
+      <c r="N578" s="5"/>
+      <c r="O578" s="5"/>
+      <c r="P578" s="5"/>
+      <c r="Q578" s="5"/>
+      <c r="R578" s="5"/>
+      <c r="S578" s="5"/>
+      <c r="T578" s="5"/>
+      <c r="U578" s="5"/>
+      <c r="V578" s="5"/>
+    </row>
+    <row r="579" ht="15.75" customHeight="1">
+      <c r="A579" s="5" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B579" s="5" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C579" s="5" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D579" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E579" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F579" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G579" s="6" t="s">
+        <v>1094</v>
+      </c>
+      <c r="H579" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I579" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J579" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K579" s="5"/>
+      <c r="L579" s="5"/>
+      <c r="M579" s="5"/>
+      <c r="N579" s="5"/>
+      <c r="O579" s="5"/>
+      <c r="P579" s="5"/>
+      <c r="Q579" s="5"/>
+      <c r="R579" s="5"/>
+      <c r="S579" s="5"/>
+      <c r="T579" s="5"/>
+      <c r="U579" s="5"/>
+      <c r="V579" s="5"/>
+    </row>
+    <row r="580" ht="15.75" customHeight="1">
+      <c r="A580" s="5" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B580" s="5" t="s">
+        <v>1095</v>
+      </c>
+      <c r="C580" s="5" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D580" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E580" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F580" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G580" s="6" t="s">
+        <v>1094</v>
+      </c>
+      <c r="H580" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I580" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J580" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K580" s="5"/>
+      <c r="L580" s="5"/>
+      <c r="M580" s="5"/>
+      <c r="N580" s="5"/>
+      <c r="O580" s="5"/>
+      <c r="P580" s="5"/>
+      <c r="Q580" s="5"/>
+      <c r="R580" s="5"/>
+      <c r="S580" s="5"/>
+      <c r="T580" s="5"/>
+      <c r="U580" s="5"/>
+      <c r="V580" s="5"/>
+    </row>
+    <row r="581" ht="15.75" customHeight="1">
+      <c r="A581" s="5" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B581" s="5" t="s">
+        <v>1097</v>
+      </c>
+      <c r="C581" s="5" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D581" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E581" s="5" t="s">
+        <v>1086</v>
+      </c>
+      <c r="F581" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G581" s="5" t="s">
+        <v>1098</v>
+      </c>
+      <c r="H581" s="5" t="s">
+        <v>1098</v>
+      </c>
+      <c r="I581" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="J581" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K581" s="5"/>
+      <c r="L581" s="5"/>
+      <c r="M581" s="5"/>
+      <c r="N581" s="5"/>
+      <c r="O581" s="5"/>
+      <c r="P581" s="5"/>
+      <c r="Q581" s="5"/>
+      <c r="R581" s="5"/>
+      <c r="S581" s="5"/>
+      <c r="T581" s="5"/>
+      <c r="U581" s="5"/>
+      <c r="V581" s="5"/>
+    </row>
+    <row r="582" ht="15.75" customHeight="1">
+      <c r="A582" s="5" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B582" s="5" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C582" s="5" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D582" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E582" s="5" t="s">
+        <v>1100</v>
+      </c>
+      <c r="F582" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G582" s="6" t="s">
+        <v>1101</v>
+      </c>
+      <c r="H582" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I582" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J582" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K582" s="5"/>
+      <c r="L582" s="5"/>
+      <c r="M582" s="5"/>
+      <c r="N582" s="5"/>
+      <c r="O582" s="5"/>
+      <c r="P582" s="5"/>
+      <c r="Q582" s="5"/>
+      <c r="R582" s="5"/>
+      <c r="S582" s="5"/>
+      <c r="T582" s="5"/>
+      <c r="U582" s="5"/>
+      <c r="V582" s="5"/>
+    </row>
+    <row r="583" ht="15.75" customHeight="1">
+      <c r="A583" s="5" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B583" s="5" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C583" s="5" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D583" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E583" s="5" t="s">
+        <v>1103</v>
+      </c>
+      <c r="F583" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G583" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="H583" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I583" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J583" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K583" s="5"/>
+      <c r="L583" s="5"/>
+      <c r="M583" s="5"/>
+      <c r="N583" s="5"/>
+      <c r="O583" s="5"/>
+      <c r="P583" s="5"/>
+      <c r="Q583" s="5"/>
+      <c r="R583" s="5"/>
+      <c r="S583" s="5"/>
+      <c r="T583" s="5"/>
+      <c r="U583" s="5"/>
+      <c r="V583" s="5"/>
+    </row>
+    <row r="584" ht="15.75" customHeight="1">
+      <c r="A584" s="5" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B584" s="5" t="s">
+        <v>1104</v>
+      </c>
+      <c r="C584" s="5" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D584" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E584" s="5" t="s">
+        <v>1105</v>
+      </c>
+      <c r="F584" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G584" s="6" t="s">
+        <v>1106</v>
+      </c>
+      <c r="H584" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I584" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J584" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K584" s="5"/>
+      <c r="L584" s="5"/>
+      <c r="M584" s="5"/>
+      <c r="N584" s="5"/>
+      <c r="O584" s="5"/>
+      <c r="P584" s="5"/>
+      <c r="Q584" s="5"/>
+      <c r="R584" s="5"/>
+      <c r="S584" s="5"/>
+      <c r="T584" s="5"/>
+      <c r="U584" s="5"/>
+      <c r="V584" s="5"/>
+    </row>
+    <row r="585" ht="15.75" customHeight="1">
+      <c r="A585" s="5" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B585" s="5" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C585" s="5" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D585" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E585" s="5" t="s">
+        <v>1109</v>
+      </c>
+      <c r="F585" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G585" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="H585" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I585" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J585" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K585" s="5"/>
+      <c r="L585" s="5"/>
+      <c r="M585" s="5"/>
+      <c r="N585" s="5"/>
+      <c r="O585" s="5"/>
+      <c r="P585" s="5"/>
+      <c r="Q585" s="5"/>
+      <c r="R585" s="5"/>
+      <c r="S585" s="5"/>
+      <c r="T585" s="5"/>
+      <c r="U585" s="5"/>
+      <c r="V585" s="5"/>
+    </row>
+    <row r="586" ht="15.75" customHeight="1">
+      <c r="A586" s="5" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B586" s="5" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C586" s="5" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D586" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E586" s="5" t="s">
+        <v>1112</v>
+      </c>
+      <c r="F586" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G586" s="6" t="s">
+        <v>1113</v>
+      </c>
+      <c r="H586" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I586" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J586" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K586" s="5"/>
+      <c r="L586" s="5"/>
+      <c r="M586" s="5"/>
+      <c r="N586" s="5"/>
+      <c r="O586" s="5"/>
+      <c r="P586" s="5"/>
+      <c r="Q586" s="5"/>
+      <c r="R586" s="5"/>
+      <c r="S586" s="5"/>
+      <c r="T586" s="5"/>
+      <c r="U586" s="5"/>
+      <c r="V586" s="5"/>
+    </row>
+    <row r="587" ht="15.75" customHeight="1">
+      <c r="A587" s="5" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B587" s="5" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C587" s="5" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D587" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E587" s="5" t="s">
+        <v>1115</v>
+      </c>
+      <c r="F587" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G587" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="H587" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I587" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J587" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K587" s="5"/>
+      <c r="L587" s="5"/>
+      <c r="M587" s="5"/>
+      <c r="N587" s="5"/>
+      <c r="O587" s="5"/>
+      <c r="P587" s="5"/>
+      <c r="Q587" s="5"/>
+      <c r="R587" s="5"/>
+      <c r="S587" s="5"/>
+      <c r="T587" s="5"/>
+      <c r="U587" s="5"/>
+      <c r="V587" s="5"/>
+    </row>
+    <row r="588" ht="15.75" customHeight="1">
+      <c r="A588" s="5" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B588" s="5" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C588" s="5" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D588" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E588" s="5" t="s">
+        <v>1117</v>
+      </c>
+      <c r="F588" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G588" s="6" t="s">
+        <v>1118</v>
+      </c>
+      <c r="H588" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I588" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J588" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K588" s="5"/>
+      <c r="L588" s="5"/>
+      <c r="M588" s="5"/>
+      <c r="N588" s="5"/>
+      <c r="O588" s="5"/>
+      <c r="P588" s="5"/>
+      <c r="Q588" s="5"/>
+      <c r="R588" s="5"/>
+      <c r="S588" s="5"/>
+      <c r="T588" s="5"/>
+      <c r="U588" s="5"/>
+      <c r="V588" s="5"/>
+    </row>
+    <row r="589" ht="15.75" customHeight="1">
+      <c r="A589" s="5" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B589" s="5" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C589" s="5" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D589" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E589" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F589" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G589" s="6" t="s">
+        <v>1094</v>
+      </c>
+      <c r="H589" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I589" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J589" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K589" s="5"/>
+      <c r="L589" s="5"/>
+      <c r="M589" s="5"/>
+      <c r="N589" s="5"/>
+      <c r="O589" s="5"/>
+      <c r="P589" s="5"/>
+      <c r="Q589" s="5"/>
+      <c r="R589" s="5"/>
+      <c r="S589" s="5"/>
+      <c r="T589" s="5"/>
+      <c r="U589" s="5"/>
+      <c r="V589" s="5"/>
+    </row>
+    <row r="590" ht="15.75" customHeight="1">
+      <c r="A590" s="5" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B590" s="5" t="s">
+        <v>1095</v>
+      </c>
+      <c r="C590" s="5" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D590" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E590" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F590" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G590" s="6" t="s">
+        <v>1094</v>
+      </c>
+      <c r="H590" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I590" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J590" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K590" s="5"/>
+      <c r="L590" s="5"/>
+      <c r="M590" s="5"/>
+      <c r="N590" s="5"/>
+      <c r="O590" s="5"/>
+      <c r="P590" s="5"/>
+      <c r="Q590" s="5"/>
+      <c r="R590" s="5"/>
+      <c r="S590" s="5"/>
+      <c r="T590" s="5"/>
+      <c r="U590" s="5"/>
+      <c r="V590" s="5"/>
+    </row>
+    <row r="591" ht="15.75" customHeight="1">
+      <c r="A591" s="5" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B591" s="5" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C591" s="5" t="s">
+        <v>1119</v>
+      </c>
+      <c r="D591" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E591" s="5" t="s">
+        <v>1120</v>
+      </c>
+      <c r="F591" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G591" s="6" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H591" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I591" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J591" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K591" s="5"/>
+      <c r="L591" s="5"/>
+      <c r="M591" s="5"/>
+      <c r="N591" s="5"/>
+      <c r="O591" s="5"/>
+      <c r="P591" s="5"/>
+      <c r="Q591" s="5"/>
+      <c r="R591" s="5"/>
+      <c r="S591" s="5"/>
+      <c r="T591" s="5"/>
+      <c r="U591" s="5"/>
+      <c r="V591" s="5"/>
+    </row>
+    <row r="592" ht="15.75" customHeight="1">
+      <c r="A592" s="5" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B592" s="5" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C592" s="5" t="s">
+        <v>1119</v>
+      </c>
+      <c r="D592" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E592" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F592" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G592" s="6" t="s">
+        <v>1094</v>
+      </c>
+      <c r="H592" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I592" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J592" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K592" s="5"/>
+      <c r="L592" s="5"/>
+      <c r="M592" s="5"/>
+      <c r="N592" s="5"/>
+      <c r="O592" s="5"/>
+      <c r="P592" s="5"/>
+      <c r="Q592" s="5"/>
+      <c r="R592" s="5"/>
+      <c r="S592" s="5"/>
+      <c r="T592" s="5"/>
+      <c r="U592" s="5"/>
+      <c r="V592" s="5"/>
+    </row>
+    <row r="593" ht="15.75" customHeight="1">
+      <c r="A593" s="5" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B593" s="5" t="s">
+        <v>1095</v>
+      </c>
+      <c r="C593" s="5" t="s">
+        <v>1119</v>
+      </c>
+      <c r="D593" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E593" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F593" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G593" s="6" t="s">
+        <v>1094</v>
+      </c>
+      <c r="H593" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I593" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J593" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K593" s="5"/>
+      <c r="L593" s="5"/>
+      <c r="M593" s="5"/>
+      <c r="N593" s="5"/>
+      <c r="O593" s="5"/>
+      <c r="P593" s="5"/>
+      <c r="Q593" s="5"/>
+      <c r="R593" s="5"/>
+      <c r="S593" s="5"/>
+      <c r="T593" s="5"/>
+      <c r="U593" s="5"/>
+      <c r="V593" s="5"/>
+    </row>
+    <row r="594" ht="15.75" customHeight="1">
+      <c r="A594" s="5" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B594" s="5" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C594" s="5" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D594" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E594" s="5" t="s">
+        <v>1124</v>
+      </c>
+      <c r="F594" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G594" s="6" t="s">
+        <v>1125</v>
+      </c>
+      <c r="H594" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I594" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J594" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K594" s="5"/>
+      <c r="L594" s="5"/>
+      <c r="M594" s="5"/>
+      <c r="N594" s="5"/>
+      <c r="O594" s="5"/>
+      <c r="P594" s="5"/>
+      <c r="Q594" s="5"/>
+      <c r="R594" s="5"/>
+      <c r="S594" s="5"/>
+      <c r="T594" s="5"/>
+      <c r="U594" s="5"/>
+      <c r="V594" s="5"/>
+    </row>
+    <row r="595" ht="15.75" customHeight="1">
+      <c r="A595" s="5" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B595" s="5" t="s">
+        <v>1126</v>
+      </c>
+      <c r="C595" s="5" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D595" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E595" s="5" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F595" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G595" s="6" t="s">
+        <v>1125</v>
+      </c>
+      <c r="H595" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I595" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J595" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K595" s="5"/>
+      <c r="L595" s="5"/>
+      <c r="M595" s="5"/>
+      <c r="N595" s="5"/>
+      <c r="O595" s="5"/>
+      <c r="P595" s="5"/>
+      <c r="Q595" s="5"/>
+      <c r="R595" s="5"/>
+      <c r="S595" s="5"/>
+      <c r="T595" s="5"/>
+      <c r="U595" s="5"/>
+      <c r="V595" s="5"/>
+    </row>
+    <row r="596" ht="15.75" customHeight="1">
+      <c r="A596" s="5" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B596" s="5" t="s">
+        <v>1128</v>
+      </c>
+      <c r="C596" s="5" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D596" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E596" s="5" t="s">
+        <v>1129</v>
+      </c>
+      <c r="F596" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G596" s="6" t="s">
+        <v>1130</v>
+      </c>
+      <c r="H596" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I596" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J596" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K596" s="5"/>
+      <c r="L596" s="5"/>
+      <c r="M596" s="5"/>
+      <c r="N596" s="5"/>
+      <c r="O596" s="5"/>
+      <c r="P596" s="5"/>
+      <c r="Q596" s="5"/>
+      <c r="R596" s="5"/>
+      <c r="S596" s="5"/>
+      <c r="T596" s="5"/>
+      <c r="U596" s="5"/>
+      <c r="V596" s="5"/>
+    </row>
+    <row r="597" ht="15.75" customHeight="1">
+      <c r="A597" s="5" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B597" s="5" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C597" s="5" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D597" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E597" s="5" t="s">
+        <v>1132</v>
+      </c>
+      <c r="F597" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G597" s="6" t="s">
+        <v>1130</v>
+      </c>
+      <c r="H597" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I597" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J597" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K597" s="5"/>
+      <c r="L597" s="5"/>
+      <c r="M597" s="5"/>
+      <c r="N597" s="5"/>
+      <c r="O597" s="5"/>
+      <c r="P597" s="5"/>
+      <c r="Q597" s="5"/>
+      <c r="R597" s="5"/>
+      <c r="S597" s="5"/>
+      <c r="T597" s="5"/>
+      <c r="U597" s="5"/>
+      <c r="V597" s="5"/>
+    </row>
+    <row r="598" ht="15.75" customHeight="1">
+      <c r="A598" s="5" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B598" s="5" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C598" s="5" t="s">
+        <v>1133</v>
+      </c>
+      <c r="D598" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E598" s="5" t="s">
+        <v>1028</v>
+      </c>
+      <c r="F598" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G598" s="6" t="s">
+        <v>1062</v>
+      </c>
+      <c r="H598" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I598" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J598" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K598" s="5"/>
+      <c r="L598" s="5"/>
+      <c r="M598" s="5"/>
+      <c r="N598" s="5"/>
+      <c r="O598" s="5"/>
+      <c r="P598" s="5"/>
+      <c r="Q598" s="5"/>
+      <c r="R598" s="5"/>
+      <c r="S598" s="5"/>
+      <c r="T598" s="5"/>
+      <c r="U598" s="5"/>
+      <c r="V598" s="5"/>
+    </row>
+    <row r="599" ht="15.75" customHeight="1">
+      <c r="A599" s="5" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B599" s="5" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C599" s="5" t="s">
+        <v>1135</v>
+      </c>
+      <c r="D599" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E599" s="5" t="s">
+        <v>1137</v>
+      </c>
+      <c r="F599" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G599" s="6" t="s">
+        <v>1138</v>
+      </c>
+      <c r="H599" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I599" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J599" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K599" s="5"/>
+      <c r="L599" s="5"/>
+      <c r="M599" s="5"/>
+      <c r="N599" s="5"/>
+      <c r="O599" s="5"/>
+      <c r="P599" s="5"/>
+      <c r="Q599" s="5"/>
+      <c r="R599" s="5"/>
+      <c r="S599" s="5"/>
+      <c r="T599" s="5"/>
+      <c r="U599" s="5"/>
+      <c r="V599" s="5"/>
+    </row>
+    <row r="600" ht="15.75" customHeight="1">
+      <c r="A600" s="5" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B600" s="5" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C600" s="5" t="s">
+        <v>1135</v>
+      </c>
+      <c r="D600" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E600" s="5" t="s">
+        <v>1140</v>
+      </c>
+      <c r="F600" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G600" s="6" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H600" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I600" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J600" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K600" s="5"/>
+      <c r="L600" s="5"/>
+      <c r="M600" s="5"/>
+      <c r="N600" s="5"/>
+      <c r="O600" s="5"/>
+      <c r="P600" s="5"/>
+      <c r="Q600" s="5"/>
+      <c r="R600" s="5"/>
+      <c r="S600" s="5"/>
+      <c r="T600" s="5"/>
+      <c r="U600" s="5"/>
+      <c r="V600" s="5"/>
+    </row>
+    <row r="601" ht="15.75" customHeight="1">
+      <c r="A601" s="5" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B601" s="5" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C601" s="5" t="s">
+        <v>1135</v>
+      </c>
+      <c r="D601" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E601" s="5" t="s">
+        <v>1143</v>
+      </c>
+      <c r="F601" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G601" s="6" t="s">
+        <v>1144</v>
+      </c>
+      <c r="H601" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I601" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J601" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K601" s="5"/>
+      <c r="L601" s="5"/>
+      <c r="M601" s="5"/>
+      <c r="N601" s="5"/>
+      <c r="O601" s="5"/>
+      <c r="P601" s="5"/>
+      <c r="Q601" s="5"/>
+      <c r="R601" s="5"/>
+      <c r="S601" s="5"/>
+      <c r="T601" s="5"/>
+      <c r="U601" s="5"/>
+      <c r="V601" s="5"/>
+    </row>
+    <row r="602" ht="15.75" customHeight="1">
+      <c r="A602" s="5" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B602" s="5" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C602" s="5" t="s">
+        <v>1135</v>
+      </c>
+      <c r="D602" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E602" s="5" t="s">
+        <v>1146</v>
+      </c>
+      <c r="F602" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G602" s="6" t="s">
+        <v>1144</v>
+      </c>
+      <c r="H602" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I602" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J602" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K602" s="5"/>
+      <c r="L602" s="5"/>
+      <c r="M602" s="5"/>
+      <c r="N602" s="5"/>
+      <c r="O602" s="5"/>
+      <c r="P602" s="5"/>
+      <c r="Q602" s="5"/>
+      <c r="R602" s="5"/>
+      <c r="S602" s="5"/>
+      <c r="T602" s="5"/>
+      <c r="U602" s="5"/>
+      <c r="V602" s="5"/>
+    </row>
+    <row r="603" ht="15.75" customHeight="1">
+      <c r="A603" s="5" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B603" s="5" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C603" s="5" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D603" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E603" s="5" t="s">
+        <v>1149</v>
+      </c>
+      <c r="F603" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G603" s="6" t="s">
+        <v>1150</v>
+      </c>
+      <c r="H603" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I603" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J603" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K603" s="5"/>
+      <c r="L603" s="5"/>
+      <c r="M603" s="5"/>
+      <c r="N603" s="5"/>
+      <c r="O603" s="5"/>
+      <c r="P603" s="5"/>
+      <c r="Q603" s="5"/>
+      <c r="R603" s="5"/>
+      <c r="S603" s="5"/>
+      <c r="T603" s="5"/>
+      <c r="U603" s="5"/>
+      <c r="V603" s="5"/>
+    </row>
+    <row r="604" ht="15.75" customHeight="1">
+      <c r="A604" s="5" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B604" s="5" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C604" s="5" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D604" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E604" s="5" t="s">
+        <v>1152</v>
+      </c>
+      <c r="F604" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G604" s="6" t="s">
+        <v>1150</v>
+      </c>
+      <c r="H604" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I604" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J604" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K604" s="5"/>
+      <c r="L604" s="5"/>
+      <c r="M604" s="5"/>
+      <c r="N604" s="5"/>
+      <c r="O604" s="5"/>
+      <c r="P604" s="5"/>
+      <c r="Q604" s="5"/>
+      <c r="R604" s="5"/>
+      <c r="S604" s="5"/>
+      <c r="T604" s="5"/>
+      <c r="U604" s="5"/>
+      <c r="V604" s="5"/>
+    </row>
+    <row r="605" ht="15.75" customHeight="1">
+      <c r="A605" s="5" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B605" s="5" t="s">
+        <v>1153</v>
+      </c>
+      <c r="C605" s="5" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D605" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E605" s="5" t="s">
+        <v>1154</v>
+      </c>
+      <c r="F605" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G605" s="6" t="s">
+        <v>1155</v>
+      </c>
+      <c r="H605" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I605" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J605" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K605" s="5"/>
+      <c r="L605" s="5"/>
+      <c r="M605" s="5"/>
+      <c r="N605" s="5"/>
+      <c r="O605" s="5"/>
+      <c r="P605" s="5"/>
+      <c r="Q605" s="5"/>
+      <c r="R605" s="5"/>
+      <c r="S605" s="5"/>
+      <c r="T605" s="5"/>
+      <c r="U605" s="5"/>
+      <c r="V605" s="5"/>
+    </row>
+    <row r="606" ht="15.75" customHeight="1">
+      <c r="A606" s="5" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B606" s="5" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C606" s="5" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D606" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E606" s="5" t="s">
+        <v>1157</v>
+      </c>
+      <c r="F606" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G606" s="6" t="s">
+        <v>1155</v>
+      </c>
+      <c r="H606" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I606" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J606" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K606" s="5"/>
+      <c r="L606" s="5"/>
+      <c r="M606" s="5"/>
+      <c r="N606" s="5"/>
+      <c r="O606" s="5"/>
+      <c r="P606" s="5"/>
+      <c r="Q606" s="5"/>
+      <c r="R606" s="5"/>
+      <c r="S606" s="5"/>
+      <c r="T606" s="5"/>
+      <c r="U606" s="5"/>
+      <c r="V606" s="5"/>
+    </row>
+    <row r="607" ht="15.75" customHeight="1">
+      <c r="A607" s="5" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B607" s="5" t="s">
+        <v>1159</v>
+      </c>
+      <c r="C607" s="5" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D607" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E607" s="5" t="s">
+        <v>1086</v>
+      </c>
+      <c r="F607" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G607" s="5" t="s">
+        <v>1160</v>
+      </c>
+      <c r="H607" s="5" t="s">
+        <v>1160</v>
+      </c>
+      <c r="I607" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="J607" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K607" s="5"/>
+      <c r="L607" s="5"/>
+      <c r="M607" s="5"/>
+      <c r="N607" s="5"/>
+      <c r="O607" s="5"/>
+      <c r="P607" s="5"/>
+      <c r="Q607" s="5"/>
+      <c r="R607" s="5"/>
+      <c r="S607" s="5"/>
+      <c r="T607" s="5"/>
+      <c r="U607" s="5"/>
+      <c r="V607" s="5"/>
+    </row>
+    <row r="608" ht="15.75" customHeight="1">
+      <c r="A608" s="5" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B608" s="5" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C608" s="5" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D608" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E608" s="5" t="s">
+        <v>1163</v>
+      </c>
+      <c r="F608" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G608" s="6" t="s">
+        <v>1164</v>
+      </c>
+      <c r="H608" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I608" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J608" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K608" s="5"/>
+      <c r="L608" s="5"/>
+      <c r="M608" s="5"/>
+      <c r="N608" s="5"/>
+      <c r="O608" s="5"/>
+      <c r="P608" s="5"/>
+      <c r="Q608" s="5"/>
+      <c r="R608" s="5"/>
+      <c r="S608" s="5"/>
+      <c r="T608" s="5"/>
+      <c r="U608" s="5"/>
+      <c r="V608" s="5"/>
+    </row>
+    <row r="609" ht="15.75" customHeight="1">
+      <c r="A609" s="5" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B609" s="5" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C609" s="5" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D609" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E609" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F609" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G609" s="6" t="s">
+        <v>1094</v>
+      </c>
+      <c r="H609" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I609" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J609" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K609" s="5"/>
+      <c r="L609" s="5"/>
+      <c r="M609" s="5"/>
+      <c r="N609" s="5"/>
+      <c r="O609" s="5"/>
+      <c r="P609" s="5"/>
+      <c r="Q609" s="5"/>
+      <c r="R609" s="5"/>
+      <c r="S609" s="5"/>
+      <c r="T609" s="5"/>
+      <c r="U609" s="5"/>
+      <c r="V609" s="5"/>
+    </row>
+    <row r="610" ht="15.75" customHeight="1">
+      <c r="A610" s="5" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B610" s="5" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C610" s="5" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D610" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E610" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F610" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G610" s="6" t="s">
+        <v>1094</v>
+      </c>
+      <c r="H610" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I610" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J610" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K610" s="5"/>
+      <c r="L610" s="5"/>
+      <c r="M610" s="5"/>
+      <c r="N610" s="5"/>
+      <c r="O610" s="5"/>
+      <c r="P610" s="5"/>
+      <c r="Q610" s="5"/>
+      <c r="R610" s="5"/>
+      <c r="S610" s="5"/>
+      <c r="T610" s="5"/>
+      <c r="U610" s="5"/>
+      <c r="V610" s="5"/>
+    </row>
+    <row r="611" ht="15.75" customHeight="1">
+      <c r="A611" s="5" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B611" s="5" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C611" s="5" t="s">
+        <v>1167</v>
+      </c>
+      <c r="D611" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E611" s="5" t="s">
+        <v>1086</v>
+      </c>
+      <c r="F611" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G611" s="5" t="s">
+        <v>1169</v>
+      </c>
+      <c r="H611" s="5" t="s">
+        <v>1169</v>
+      </c>
+      <c r="I611" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="J611" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K611" s="5"/>
+      <c r="L611" s="5"/>
+      <c r="M611" s="5"/>
+      <c r="N611" s="5"/>
+      <c r="O611" s="5"/>
+      <c r="P611" s="5"/>
+      <c r="Q611" s="5"/>
+      <c r="R611" s="5"/>
+      <c r="S611" s="5"/>
+      <c r="T611" s="5"/>
+      <c r="U611" s="5"/>
+      <c r="V611" s="5"/>
+    </row>
+    <row r="612" ht="15.75" customHeight="1">
+      <c r="A612" s="5" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B612" s="5" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C612" s="5" t="s">
+        <v>1167</v>
+      </c>
+      <c r="D612" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E612" s="5" t="s">
+        <v>1171</v>
+      </c>
+      <c r="F612" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G612" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="H612" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I612" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J612" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K612" s="5"/>
+      <c r="L612" s="5"/>
+      <c r="M612" s="5"/>
+      <c r="N612" s="5"/>
+      <c r="O612" s="5"/>
+      <c r="P612" s="5"/>
+      <c r="Q612" s="5"/>
+      <c r="R612" s="5"/>
+      <c r="S612" s="5"/>
+      <c r="T612" s="5"/>
+      <c r="U612" s="5"/>
+      <c r="V612" s="5"/>
+    </row>
+    <row r="613" ht="15.75" customHeight="1">
+      <c r="A613" s="5" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B613" s="5" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C613" s="5" t="s">
+        <v>1167</v>
+      </c>
+      <c r="D613" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E613" s="5" t="s">
+        <v>1173</v>
+      </c>
+      <c r="F613" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G613" s="6" t="s">
+        <v>1174</v>
+      </c>
+      <c r="H613" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I613" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J613" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K613" s="5"/>
+      <c r="L613" s="5"/>
+      <c r="M613" s="5"/>
+      <c r="N613" s="5"/>
+      <c r="O613" s="5"/>
+      <c r="P613" s="5"/>
+      <c r="Q613" s="5"/>
+      <c r="R613" s="5"/>
+      <c r="S613" s="5"/>
+      <c r="T613" s="5"/>
+      <c r="U613" s="5"/>
+      <c r="V613" s="5"/>
+    </row>
+    <row r="614" ht="15.75" customHeight="1">
+      <c r="A614" s="5" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B614" s="5" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C614" s="5" t="s">
+        <v>1175</v>
+      </c>
+      <c r="D614" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E614" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F614" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G614" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="H614" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I614" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J614" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K614" s="5"/>
+      <c r="L614" s="5"/>
+      <c r="M614" s="5"/>
+      <c r="N614" s="5"/>
+      <c r="O614" s="5"/>
+      <c r="P614" s="5"/>
+      <c r="Q614" s="5"/>
+      <c r="R614" s="5"/>
+      <c r="S614" s="5"/>
+      <c r="T614" s="5"/>
+      <c r="U614" s="5"/>
+      <c r="V614" s="5"/>
+    </row>
+    <row r="615" ht="15.75" customHeight="1">
+      <c r="A615" s="5" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B615" s="5" t="s">
+        <v>1177</v>
+      </c>
+      <c r="C615" s="5" t="s">
+        <v>1175</v>
+      </c>
+      <c r="D615" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E615" s="5" t="s">
+        <v>1178</v>
+      </c>
+      <c r="F615" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G615" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="H615" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I615" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J615" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K615" s="5"/>
+      <c r="L615" s="5"/>
+      <c r="M615" s="5"/>
+      <c r="N615" s="5"/>
+      <c r="O615" s="5"/>
+      <c r="P615" s="5"/>
+      <c r="Q615" s="5"/>
+      <c r="R615" s="5"/>
+      <c r="S615" s="5"/>
+      <c r="T615" s="5"/>
+      <c r="U615" s="5"/>
+      <c r="V615" s="5"/>
+    </row>
+    <row r="616" ht="15.75" customHeight="1">
+      <c r="A616" s="5" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B616" s="5" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C616" s="5" t="s">
+        <v>1179</v>
+      </c>
+      <c r="D616" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E616" s="5" t="s">
+        <v>1181</v>
+      </c>
+      <c r="F616" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G616" s="6" t="s">
+        <v>1182</v>
+      </c>
+      <c r="H616" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I616" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J616" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K616" s="5"/>
+      <c r="L616" s="5"/>
+      <c r="M616" s="5"/>
+      <c r="N616" s="5"/>
+      <c r="O616" s="5"/>
+      <c r="P616" s="5"/>
+      <c r="Q616" s="5"/>
+      <c r="R616" s="5"/>
+      <c r="S616" s="5"/>
+      <c r="T616" s="5"/>
+      <c r="U616" s="5"/>
+      <c r="V616" s="5"/>
+    </row>
+    <row r="617" ht="15.75" customHeight="1">
+      <c r="A617" s="5" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B617" s="5" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C617" s="5" t="s">
+        <v>1179</v>
+      </c>
+      <c r="D617" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E617" s="5" t="s">
+        <v>1184</v>
+      </c>
+      <c r="F617" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G617" s="6" t="s">
+        <v>1185</v>
+      </c>
+      <c r="H617" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I617" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J617" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K617" s="5"/>
+      <c r="L617" s="5"/>
+      <c r="M617" s="5"/>
+      <c r="N617" s="5"/>
+      <c r="O617" s="5"/>
+      <c r="P617" s="5"/>
+      <c r="Q617" s="5"/>
+      <c r="R617" s="5"/>
+      <c r="S617" s="5"/>
+      <c r="T617" s="5"/>
+      <c r="U617" s="5"/>
+      <c r="V617" s="5"/>
+    </row>
+    <row r="618" ht="15.75" customHeight="1">
+      <c r="A618" s="5" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B618" s="5" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C618" s="5" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D618" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E618" s="5" t="s">
+        <v>1187</v>
+      </c>
+      <c r="F618" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G618" s="6" t="s">
+        <v>1188</v>
+      </c>
+      <c r="H618" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I618" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J618" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K618" s="5"/>
+      <c r="L618" s="5"/>
+      <c r="M618" s="5"/>
+      <c r="N618" s="5"/>
+      <c r="O618" s="5"/>
+      <c r="P618" s="5"/>
+      <c r="Q618" s="5"/>
+      <c r="R618" s="5"/>
+      <c r="S618" s="5"/>
+      <c r="T618" s="5"/>
+      <c r="U618" s="5"/>
+      <c r="V618" s="5"/>
+    </row>
+    <row r="619" ht="15.75" customHeight="1">
+      <c r="A619" s="5" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B619" s="5" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C619" s="5" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D619" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E619" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F619" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G619" s="6" t="s">
+        <v>1094</v>
+      </c>
+      <c r="H619" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I619" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J619" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K619" s="5"/>
+      <c r="L619" s="5"/>
+      <c r="M619" s="5"/>
+      <c r="N619" s="5"/>
+      <c r="O619" s="5"/>
+      <c r="P619" s="5"/>
+      <c r="Q619" s="5"/>
+      <c r="R619" s="5"/>
+      <c r="S619" s="5"/>
+      <c r="T619" s="5"/>
+      <c r="U619" s="5"/>
+      <c r="V619" s="5"/>
+    </row>
+    <row r="620" ht="15.75" customHeight="1">
+      <c r="A620" s="5" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B620" s="5" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C620" s="5" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D620" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E620" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F620" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G620" s="6" t="s">
+        <v>1094</v>
+      </c>
+      <c r="H620" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I620" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J620" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K620" s="5"/>
+      <c r="L620" s="5"/>
+      <c r="M620" s="5"/>
+      <c r="N620" s="5"/>
+      <c r="O620" s="5"/>
+      <c r="P620" s="5"/>
+      <c r="Q620" s="5"/>
+      <c r="R620" s="5"/>
+      <c r="S620" s="5"/>
+      <c r="T620" s="5"/>
+      <c r="U620" s="5"/>
+      <c r="V620" s="5"/>
+    </row>
+    <row r="621" ht="15.75" customHeight="1">
+      <c r="A621" s="5" t="s">
+        <v>1189</v>
+      </c>
+      <c r="B621" s="5" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C621" s="5" t="s">
+        <v>1189</v>
+      </c>
+      <c r="D621" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E621" s="5" t="s">
+        <v>1190</v>
+      </c>
+      <c r="F621" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G621" s="6" t="s">
+        <v>1191</v>
+      </c>
+      <c r="H621" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I621" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J621" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K621" s="5"/>
+      <c r="L621" s="5"/>
+      <c r="M621" s="5"/>
+      <c r="N621" s="5"/>
+      <c r="O621" s="5"/>
+      <c r="P621" s="5"/>
+      <c r="Q621" s="5"/>
+      <c r="R621" s="5"/>
+      <c r="S621" s="5"/>
+      <c r="T621" s="5"/>
+      <c r="U621" s="5"/>
+      <c r="V621" s="5"/>
+    </row>
+    <row r="622" ht="15.75" customHeight="1">
+      <c r="A622" s="5" t="s">
+        <v>1189</v>
+      </c>
+      <c r="B622" s="5" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C622" s="5" t="s">
+        <v>1189</v>
+      </c>
+      <c r="D622" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E622" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F622" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G622" s="6" t="s">
+        <v>1094</v>
+      </c>
+      <c r="H622" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I622" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J622" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K622" s="5"/>
+      <c r="L622" s="5"/>
+      <c r="M622" s="5"/>
+      <c r="N622" s="5"/>
+      <c r="O622" s="5"/>
+      <c r="P622" s="5"/>
+      <c r="Q622" s="5"/>
+      <c r="R622" s="5"/>
+      <c r="S622" s="5"/>
+      <c r="T622" s="5"/>
+      <c r="U622" s="5"/>
+      <c r="V622" s="5"/>
+    </row>
+    <row r="623" ht="15.75" customHeight="1">
+      <c r="A623" s="5" t="s">
+        <v>1189</v>
+      </c>
+      <c r="B623" s="5" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C623" s="5" t="s">
+        <v>1189</v>
+      </c>
+      <c r="D623" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E623" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F623" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G623" s="6" t="s">
+        <v>1094</v>
+      </c>
+      <c r="H623" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I623" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J623" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K623" s="5"/>
+      <c r="L623" s="5"/>
+      <c r="M623" s="5"/>
+      <c r="N623" s="5"/>
+      <c r="O623" s="5"/>
+      <c r="P623" s="5"/>
+      <c r="Q623" s="5"/>
+      <c r="R623" s="5"/>
+      <c r="S623" s="5"/>
+      <c r="T623" s="5"/>
+      <c r="U623" s="5"/>
+      <c r="V623" s="5"/>
+    </row>
+    <row r="624" ht="15.75" customHeight="1">
+      <c r="A624" s="5" t="s">
+        <v>1192</v>
+      </c>
+      <c r="B624" s="5" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C624" s="5" t="s">
+        <v>1192</v>
+      </c>
+      <c r="D624" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E624" s="5" t="s">
+        <v>1194</v>
+      </c>
+      <c r="F624" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G624" s="6" t="s">
+        <v>1195</v>
+      </c>
+      <c r="H624" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I624" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J624" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K624" s="5"/>
+      <c r="L624" s="5"/>
+      <c r="M624" s="5"/>
+      <c r="N624" s="5"/>
+      <c r="O624" s="5"/>
+      <c r="P624" s="5"/>
+      <c r="Q624" s="5"/>
+      <c r="R624" s="5"/>
+      <c r="S624" s="5"/>
+      <c r="T624" s="5"/>
+      <c r="U624" s="5"/>
+      <c r="V624" s="5"/>
+    </row>
+    <row r="625" ht="15.75" customHeight="1">
+      <c r="A625" s="5" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B625" s="5" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C625" s="5" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D625" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E625" s="5" t="s">
+        <v>1194</v>
+      </c>
+      <c r="F625" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G625" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H625" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I625" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J625" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K625" s="5"/>
+      <c r="L625" s="5"/>
+      <c r="M625" s="5"/>
+      <c r="N625" s="5"/>
+      <c r="O625" s="5"/>
+      <c r="P625" s="5"/>
+      <c r="Q625" s="5"/>
+      <c r="R625" s="5"/>
+      <c r="S625" s="5"/>
+      <c r="T625" s="5"/>
+      <c r="U625" s="5"/>
+      <c r="V625" s="5"/>
+    </row>
+    <row r="626" ht="15.75" customHeight="1">
+      <c r="A626" s="5" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B626" s="5" t="s">
+        <v>1197</v>
+      </c>
+      <c r="C626" s="5" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D626" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E626" s="5" t="s">
+        <v>1198</v>
+      </c>
+      <c r="F626" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G626" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="H626" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I626" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J626" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K626" s="5"/>
+      <c r="L626" s="5"/>
+      <c r="M626" s="5"/>
+      <c r="N626" s="5"/>
+      <c r="O626" s="5"/>
+      <c r="P626" s="5"/>
+      <c r="Q626" s="5"/>
+      <c r="R626" s="5"/>
+      <c r="S626" s="5"/>
+      <c r="T626" s="5"/>
+      <c r="U626" s="5"/>
+      <c r="V626" s="5"/>
+    </row>
+    <row r="627" ht="15.75" customHeight="1">
+      <c r="A627" s="5" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B627" s="5" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C627" s="5" t="s">
+        <v>1199</v>
+      </c>
+      <c r="D627" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E627" s="5" t="s">
+        <v>1194</v>
+      </c>
+      <c r="F627" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G627" s="6" t="s">
+        <v>1195</v>
+      </c>
+      <c r="H627" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I627" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J627" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K627" s="5"/>
+      <c r="L627" s="5"/>
+      <c r="M627" s="5"/>
+      <c r="N627" s="5"/>
+      <c r="O627" s="5"/>
+      <c r="P627" s="5"/>
+      <c r="Q627" s="5"/>
+      <c r="R627" s="5"/>
+      <c r="S627" s="5"/>
+      <c r="T627" s="5"/>
+      <c r="U627" s="5"/>
+      <c r="V627" s="5"/>
+    </row>
     <row r="628" ht="15.75" customHeight="1"/>
     <row r="629" ht="15.75" customHeight="1"/>
     <row r="630" ht="15.75" customHeight="1"/>

</xml_diff>